<commit_message>
Adding full unit test of P002
</commit_message>
<xml_diff>
--- a/Documentation/Memory Map/MemoryMap.xlsx
+++ b/Documentation/Memory Map/MemoryMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\version-control\EDD-LCP_PistonDriver\Documentation\Memory Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643F53B7-74D6-4B8A-A444-51A48BF069D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AC83B5-5F2A-40D3-B999-8029700BC14B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="3" xr2:uid="{9A36670B-9FAC-4E7D-BCC1-D5C646D37D72}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{9A36670B-9FAC-4E7D-BCC1-D5C646D37D72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -647,18 +647,52 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -675,6 +709,51 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -728,7 +807,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -773,7 +852,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -782,32 +861,20 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -877,56 +944,77 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1276,14 +1364,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A8E1FA9-3B7B-40E2-8D50-8D8CFAA9B0B9}">
   <dimension ref="A6:W23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.6640625" customWidth="1"/>
     <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:23" ht="15" thickBot="1"/>
@@ -1343,30 +1432,30 @@
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
     </row>
-    <row r="8" spans="1:23" ht="16.2" thickBot="1">
+    <row r="8" spans="1:23" ht="15.6">
       <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21" t="s">
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62"/>
-      <c r="O8" s="62"/>
-      <c r="P8" s="62"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="25"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="23"/>
       <c r="S8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1379,34 +1468,34 @@
       <c r="B9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="26" t="s">
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27" t="s">
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="28" t="s">
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="P9" s="29" t="s">
+      <c r="P9" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="Q9" s="28" t="s">
+      <c r="Q9" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="R9" s="30" t="s">
+      <c r="R9" s="61" t="s">
         <v>33</v>
       </c>
       <c r="S9" s="1"/>
@@ -1420,26 +1509,26 @@
       <c r="B10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53" t="s">
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="54"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="62"/>
       <c r="S10" s="3" t="s">
         <v>10</v>
       </c>
@@ -1453,26 +1542,26 @@
       <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="26" t="s">
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="57"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="52"/>
+      <c r="Q11" s="52"/>
+      <c r="R11" s="64"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
@@ -1484,26 +1573,26 @@
       <c r="B12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="26" t="s">
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="57"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="64"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
@@ -1515,22 +1604,22 @@
       <c r="B13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="42"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="38"/>
       <c r="S13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1544,22 +1633,22 @@
       <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="38"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="34"/>
       <c r="S14" s="9"/>
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>
@@ -1571,22 +1660,22 @@
       <c r="B15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="30"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="26"/>
       <c r="S15" s="9"/>
       <c r="T15" s="5"/>
       <c r="U15" s="5"/>
@@ -1598,32 +1687,32 @@
       <c r="B16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61" t="s">
+      <c r="D16" s="57"/>
+      <c r="E16" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61" t="s">
+      <c r="F16" s="57"/>
+      <c r="G16" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="61"/>
-      <c r="I16" s="61" t="s">
+      <c r="H16" s="57"/>
+      <c r="I16" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61" t="s">
+      <c r="J16" s="57"/>
+      <c r="K16" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="L16" s="61"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="30"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="26"/>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
@@ -1635,22 +1724,22 @@
       <c r="B17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="30"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="26"/>
       <c r="S17" s="9"/>
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
@@ -1662,22 +1751,22 @@
       <c r="B18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="30"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="26"/>
       <c r="S18" s="9"/>
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
@@ -1689,22 +1778,22 @@
       <c r="B19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="30"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="26"/>
       <c r="S19" s="9"/>
       <c r="T19" s="5"/>
       <c r="U19" s="5"/>
@@ -1716,22 +1805,22 @@
       <c r="B20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="30"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="26"/>
       <c r="S20" s="9"/>
       <c r="T20" s="5"/>
       <c r="U20" s="5"/>
@@ -1743,22 +1832,22 @@
       <c r="B21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="30"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="26"/>
       <c r="S21" s="9"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
@@ -1770,22 +1859,22 @@
       <c r="B22" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="30"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="26"/>
       <c r="S22" s="9"/>
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
@@ -1797,22 +1886,22 @@
       <c r="B23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="50"/>
-      <c r="R23" s="51"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="47"/>
       <c r="S23" s="9"/>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
@@ -1851,13 +1940,14 @@
   <dimension ref="A6:W23"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20:R20"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.6640625" customWidth="1"/>
     <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:23" ht="15" thickBot="1"/>
@@ -1921,30 +2011,30 @@
       <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21" t="s">
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21" t="s">
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="63" t="s">
+      <c r="L8" s="59"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="63"/>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="64"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="68"/>
       <c r="S8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1957,28 +2047,28 @@
       <c r="B9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="26" t="s">
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27" t="s">
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="30"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="26"/>
       <c r="S9" s="1"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
@@ -1990,28 +2080,28 @@
       <c r="B10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53" t="s">
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53" t="s">
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="33"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="29"/>
       <c r="S10" s="3" t="s">
         <v>10</v>
       </c>
@@ -2025,26 +2115,26 @@
       <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56" t="s">
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="58"/>
-      <c r="Q11" s="58"/>
-      <c r="R11" s="59"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="49"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
@@ -2056,22 +2146,22 @@
       <c r="B12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="59"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="49"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
@@ -2083,22 +2173,22 @@
       <c r="B13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="42"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="38"/>
       <c r="S13" s="3" t="s">
         <v>14</v>
       </c>
@@ -2112,22 +2202,22 @@
       <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="38"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="34"/>
       <c r="S14" s="9"/>
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>
@@ -2139,22 +2229,22 @@
       <c r="B15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="30"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="26"/>
       <c r="S15" s="9"/>
       <c r="T15" s="5"/>
       <c r="U15" s="5"/>
@@ -2166,32 +2256,32 @@
       <c r="B16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="28" t="s">
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="28" t="s">
+      <c r="H16" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="I16" s="28" t="s">
+      <c r="I16" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="28" t="s">
+      <c r="J16" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="30"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="26"/>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
@@ -2203,22 +2293,22 @@
       <c r="B17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="30"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="26"/>
       <c r="S17" s="9"/>
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
@@ -2230,22 +2320,22 @@
       <c r="B18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="30"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="26"/>
       <c r="S18" s="9"/>
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
@@ -2257,22 +2347,22 @@
       <c r="B19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="30"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="26"/>
       <c r="S19" s="9"/>
       <c r="T19" s="5"/>
       <c r="U19" s="5"/>
@@ -2284,7 +2374,7 @@
       <c r="B20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="65" t="s">
+      <c r="C20" s="69" t="s">
         <v>59</v>
       </c>
       <c r="D20" s="66"/>
@@ -2302,12 +2392,12 @@
       <c r="L20" s="66"/>
       <c r="M20" s="66"/>
       <c r="N20" s="66"/>
-      <c r="O20" s="61" t="s">
+      <c r="O20" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="P20" s="61"/>
-      <c r="Q20" s="61"/>
-      <c r="R20" s="67"/>
+      <c r="P20" s="57"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="70"/>
       <c r="S20" s="9"/>
       <c r="T20" s="5"/>
       <c r="U20" s="5"/>
@@ -2319,22 +2409,22 @@
       <c r="B21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="30"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="26"/>
       <c r="S21" s="9"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
@@ -2346,22 +2436,22 @@
       <c r="B22" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="30"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="26"/>
       <c r="S22" s="9"/>
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
@@ -2373,22 +2463,22 @@
       <c r="B23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="50"/>
-      <c r="R23" s="51"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="47"/>
       <c r="S23" s="9"/>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
@@ -2426,8 +2516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A89A20B-8671-496F-AF4B-48097BE9ED08}">
   <dimension ref="A6:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10:R10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2497,26 +2587,26 @@
       <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21" t="s">
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="68"/>
+      <c r="L8" s="59"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="59"/>
+      <c r="Q8" s="59"/>
+      <c r="R8" s="71"/>
       <c r="S8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2529,26 +2619,26 @@
       <c r="B9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="27" t="s">
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="69"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="72"/>
       <c r="S9" s="1"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
@@ -2560,26 +2650,26 @@
       <c r="B10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53" t="s">
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="54"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="62"/>
       <c r="S10" s="3" t="s">
         <v>10</v>
       </c>
@@ -2593,22 +2683,22 @@
       <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="58"/>
-      <c r="Q11" s="58"/>
-      <c r="R11" s="59"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="49"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
@@ -2620,22 +2710,22 @@
       <c r="B12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="59"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="49"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
@@ -2647,22 +2737,22 @@
       <c r="B13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="42"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="38"/>
       <c r="S13" s="3" t="s">
         <v>14</v>
       </c>
@@ -2676,22 +2766,22 @@
       <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="38"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="34"/>
       <c r="S14" s="9"/>
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>
@@ -2703,22 +2793,22 @@
       <c r="B15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="30"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="26"/>
       <c r="S15" s="9"/>
       <c r="T15" s="5"/>
       <c r="U15" s="5"/>
@@ -2730,22 +2820,22 @@
       <c r="B16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="30"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="26"/>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
@@ -2757,22 +2847,22 @@
       <c r="B17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="30"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="26"/>
       <c r="S17" s="9"/>
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
@@ -2784,22 +2874,22 @@
       <c r="B18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="30"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="26"/>
       <c r="S18" s="9"/>
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
@@ -2811,22 +2901,22 @@
       <c r="B19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="30"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="26"/>
       <c r="S19" s="9"/>
       <c r="T19" s="5"/>
       <c r="U19" s="5"/>
@@ -2838,22 +2928,22 @@
       <c r="B20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="30"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="26"/>
       <c r="S20" s="9"/>
       <c r="T20" s="5"/>
       <c r="U20" s="5"/>
@@ -2865,22 +2955,22 @@
       <c r="B21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="30"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="26"/>
       <c r="S21" s="9"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
@@ -2892,22 +2982,22 @@
       <c r="B22" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="30"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="26"/>
       <c r="S22" s="9"/>
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
@@ -2919,22 +3009,22 @@
       <c r="B23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="50"/>
-      <c r="R23" s="51"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="47"/>
       <c r="S23" s="9"/>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>

</xml_diff>

<commit_message>
Fixing struct with single bytes.
Was using lists, but that was bad bad bad.  Now using slice to deal with single, works much better
</commit_message>
<xml_diff>
--- a/Documentation/Memory Map/MemoryMap.xlsx
+++ b/Documentation/Memory Map/MemoryMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\version-control\EDD-LCP_PistonDriver\Documentation\Memory Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE208F5-8F80-4CB2-9EC2-F2D32471EA16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440C8F0D-9DAC-4884-9B19-DC18FE2C75E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{9A36670B-9FAC-4E7D-BCC1-D5C646D37D72}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{9A36670B-9FAC-4E7D-BCC1-D5C646D37D72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="104">
   <si>
     <t>A</t>
   </si>
@@ -303,9 +303,6 @@
     <t>0x4c43503030303130</t>
   </si>
   <si>
-    <t>0x4c43502d504953</t>
-  </si>
-  <si>
     <t>0x07e5</t>
   </si>
   <si>
@@ -343,6 +340,9 @@
   </si>
   <si>
     <t>VAR_WRITE needs to be set to 0xA5 in order to write to any settable system variables</t>
+  </si>
+  <si>
+    <t>0x4c43502d50495300</t>
   </si>
 </sst>
 </file>
@@ -596,7 +596,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1181,6 +1181,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1204,7 +1241,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1615,7 +1652,19 @@
     <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1972,8 +2021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D570E7CD-E1C0-4A6C-BD44-8A443DE8F490}">
   <dimension ref="B7:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2401,15 +2450,15 @@
       <c r="K23" s="133" t="s">
         <v>40</v>
       </c>
-      <c r="L23" s="142"/>
-      <c r="M23" s="142"/>
-      <c r="N23" s="142"/>
-      <c r="O23" s="142"/>
-      <c r="P23" s="142"/>
-      <c r="Q23" s="142"/>
+      <c r="L23" s="143"/>
+      <c r="M23" s="143"/>
+      <c r="N23" s="143"/>
+      <c r="O23" s="143"/>
+      <c r="P23" s="143"/>
+      <c r="Q23" s="143"/>
       <c r="R23" s="134"/>
     </row>
-    <row r="24" spans="2:18" ht="16.2" thickBot="1">
+    <row r="24" spans="2:18" ht="16.2" customHeight="1" thickBot="1">
       <c r="B24" s="10" t="s">
         <v>24</v>
       </c>
@@ -2427,18 +2476,18 @@
         <v>65</v>
       </c>
       <c r="L24" s="134"/>
-      <c r="M24" s="135" t="s">
+      <c r="M24" s="142" t="s">
         <v>42</v>
       </c>
-      <c r="N24" s="135"/>
-      <c r="O24" s="135" t="s">
+      <c r="N24" s="142" t="s">
         <v>43</v>
       </c>
-      <c r="P24" s="135"/>
-      <c r="Q24" s="135" t="s">
+      <c r="O24" s="144" t="s">
         <v>44</v>
       </c>
-      <c r="R24" s="136"/>
+      <c r="P24" s="145"/>
+      <c r="Q24" s="145"/>
+      <c r="R24" s="146"/>
     </row>
     <row r="26" spans="2:18">
       <c r="C26" s="139" t="s">
@@ -2464,23 +2513,21 @@
     </row>
     <row r="28" spans="2:18">
       <c r="C28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="30">
     <mergeCell ref="K26:R26"/>
     <mergeCell ref="C26:J26"/>
     <mergeCell ref="K23:R23"/>
+    <mergeCell ref="O24:R24"/>
     <mergeCell ref="K19:R19"/>
     <mergeCell ref="K20:R20"/>
     <mergeCell ref="K21:R21"/>
     <mergeCell ref="K22:R22"/>
     <mergeCell ref="C24:J24"/>
     <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:R24"/>
     <mergeCell ref="C14:F14"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="G17:J17"/>
@@ -2510,8 +2557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D8C36D-939B-444F-978B-726CF9EB90A8}">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16:Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2753,7 +2800,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="112"/>
       <c r="D7" s="112"/>
@@ -2918,7 +2965,7 @@
       <c r="H10" s="103"/>
       <c r="I10" s="104"/>
       <c r="J10" s="120" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K10" s="120"/>
       <c r="L10" s="120"/>
@@ -2941,11 +2988,17 @@
       <c r="F11" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="107"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="140"/>
+      <c r="G11" s="107" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="107" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="140" t="s">
+        <v>6</v>
+      </c>
       <c r="J11" s="120" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K11" s="120"/>
       <c r="L11" s="120"/>
@@ -2984,7 +3037,7 @@
         <v>6</v>
       </c>
       <c r="J12" s="130" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K12" s="130"/>
       <c r="L12" s="130"/>
@@ -3023,7 +3076,7 @@
         <v>6</v>
       </c>
       <c r="J13" s="124" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K13" s="124"/>
       <c r="L13" s="124"/>
@@ -3062,7 +3115,7 @@
         <v>6</v>
       </c>
       <c r="J14" s="120" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K14" s="120"/>
       <c r="L14" s="120"/>
@@ -3101,7 +3154,7 @@
         <v>6</v>
       </c>
       <c r="J15" s="124" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K15" s="124"/>
       <c r="L15" s="124"/>
@@ -3140,14 +3193,14 @@
         <v>6</v>
       </c>
       <c r="J16" s="133" t="s">
-        <v>90</v>
-      </c>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
-      <c r="M16" s="142"/>
-      <c r="N16" s="142"/>
-      <c r="O16" s="142"/>
-      <c r="P16" s="142"/>
+        <v>103</v>
+      </c>
+      <c r="K16" s="143"/>
+      <c r="L16" s="143"/>
+      <c r="M16" s="143"/>
+      <c r="N16" s="143"/>
+      <c r="O16" s="143"/>
+      <c r="P16" s="143"/>
       <c r="Q16" s="134"/>
     </row>
     <row r="17" spans="1:17" ht="16.2" thickBot="1">
@@ -3165,19 +3218,19 @@
       <c r="H17" s="100"/>
       <c r="I17" s="101"/>
       <c r="J17" s="133" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K17" s="134"/>
       <c r="L17" s="135" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M17" s="135"/>
       <c r="N17" s="135" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O17" s="135"/>
       <c r="P17" s="135" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q17" s="136"/>
     </row>
@@ -3601,14 +3654,14 @@
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
       <c r="J34" s="133" t="s">
-        <v>102</v>
-      </c>
-      <c r="K34" s="142"/>
-      <c r="L34" s="142"/>
-      <c r="M34" s="142"/>
-      <c r="N34" s="142"/>
-      <c r="O34" s="142"/>
-      <c r="P34" s="142"/>
+        <v>101</v>
+      </c>
+      <c r="K34" s="143"/>
+      <c r="L34" s="143"/>
+      <c r="M34" s="143"/>
+      <c r="N34" s="143"/>
+      <c r="O34" s="143"/>
+      <c r="P34" s="143"/>
       <c r="Q34" s="134"/>
     </row>
     <row r="35" spans="1:17" ht="16.2" thickBot="1">

</xml_diff>

<commit_message>
LCP Command I2C Interface major update.
Adding commands to read/write to all addresses.  memory map looks complete, too
</commit_message>
<xml_diff>
--- a/Documentation/Memory Map/MemoryMap.xlsx
+++ b/Documentation/Memory Map/MemoryMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\version-control\EDD-LCP_PistonDriver\Documentation\Memory Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440C8F0D-9DAC-4884-9B19-DC18FE2C75E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D13B096-480F-4AC3-A07E-15566474BB41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{9A36670B-9FAC-4E7D-BCC1-D5C646D37D72}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{9A36670B-9FAC-4E7D-BCC1-D5C646D37D72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="105">
   <si>
     <t>A</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>0x4c43502d50495300</t>
+  </si>
+  <si>
+    <t>LEN_TOTAL_IN</t>
   </si>
 </sst>
 </file>
@@ -596,7 +599,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -1218,6 +1221,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1241,7 +1257,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1382,75 +1398,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1523,6 +1470,72 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1532,6 +1545,12 @@
     <xf numFmtId="0" fontId="20" fillId="6" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1541,130 +1560,139 @@
     <xf numFmtId="0" fontId="20" fillId="6" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2021,61 +2049,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D570E7CD-E1C0-4A6C-BD44-8A443DE8F490}">
   <dimension ref="B7:R28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11:N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="7" spans="2:18" ht="15" thickBot="1"/>
     <row r="8" spans="2:18" ht="16.2" thickBot="1">
-      <c r="B8" s="137"/>
-      <c r="C8" s="95">
+      <c r="B8" s="80"/>
+      <c r="C8" s="72">
         <v>0</v>
       </c>
-      <c r="D8" s="96">
+      <c r="D8" s="73">
         <v>1</v>
       </c>
-      <c r="E8" s="97">
+      <c r="E8" s="74">
         <v>2</v>
       </c>
-      <c r="F8" s="97">
+      <c r="F8" s="74">
         <v>3</v>
       </c>
-      <c r="G8" s="97">
+      <c r="G8" s="74">
         <v>4</v>
       </c>
-      <c r="H8" s="97">
+      <c r="H8" s="74">
         <v>5</v>
       </c>
-      <c r="I8" s="97">
-        <v>6</v>
-      </c>
-      <c r="J8" s="97">
+      <c r="I8" s="74">
+        <v>6</v>
+      </c>
+      <c r="J8" s="74">
         <v>7</v>
       </c>
-      <c r="K8" s="97">
+      <c r="K8" s="74">
         <v>8</v>
       </c>
-      <c r="L8" s="97">
+      <c r="L8" s="74">
         <v>9</v>
       </c>
-      <c r="M8" s="97" t="s">
+      <c r="M8" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="N8" s="97" t="s">
+      <c r="N8" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="O8" s="97" t="s">
+      <c r="O8" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="P8" s="97" t="s">
+      <c r="P8" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="Q8" s="97" t="s">
+      <c r="Q8" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="R8" s="98" t="s">
+      <c r="R8" s="75" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2083,30 +2111,30 @@
       <c r="B9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="115" t="s">
+      <c r="C9" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="116"/>
-      <c r="E9" s="116"/>
-      <c r="F9" s="117"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="113"/>
       <c r="G9" s="24"/>
       <c r="H9" s="24"/>
       <c r="I9" s="24"/>
-      <c r="J9" s="141" t="s">
+      <c r="J9" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="118" t="s">
+      <c r="K9" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="118"/>
-      <c r="M9" s="118"/>
-      <c r="N9" s="118"/>
-      <c r="O9" s="118" t="s">
+      <c r="L9" s="114"/>
+      <c r="M9" s="114"/>
+      <c r="N9" s="114"/>
+      <c r="O9" s="114" t="s">
         <v>48</v>
       </c>
-      <c r="P9" s="118"/>
-      <c r="Q9" s="118"/>
-      <c r="R9" s="119"/>
+      <c r="P9" s="114"/>
+      <c r="Q9" s="114"/>
+      <c r="R9" s="115"/>
     </row>
     <row r="10" spans="2:18" ht="15.6">
       <c r="B10" s="14" t="s">
@@ -2120,145 +2148,147 @@
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
-      <c r="K10" s="120" t="s">
+      <c r="K10" s="96" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="120"/>
-      <c r="M10" s="120"/>
-      <c r="N10" s="120"/>
-      <c r="O10" s="121" t="s">
+      <c r="L10" s="96"/>
+      <c r="M10" s="96"/>
+      <c r="N10" s="96"/>
+      <c r="O10" s="116" t="s">
         <v>47</v>
       </c>
-      <c r="P10" s="121"/>
-      <c r="Q10" s="121"/>
-      <c r="R10" s="122"/>
+      <c r="P10" s="116"/>
+      <c r="Q10" s="116"/>
+      <c r="R10" s="117"/>
     </row>
     <row r="11" spans="2:18" ht="15.6">
       <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="118" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="114"/>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114"/>
+      <c r="D11" s="119"/>
+      <c r="E11" s="119"/>
+      <c r="F11" s="119"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
       <c r="J11" s="24"/>
-      <c r="K11" s="120" t="s">
-        <v>52</v>
-      </c>
-      <c r="L11" s="120"/>
-      <c r="M11" s="120"/>
-      <c r="N11" s="120"/>
-      <c r="O11" s="120" t="s">
-        <v>53</v>
-      </c>
-      <c r="P11" s="120"/>
-      <c r="Q11" s="120"/>
-      <c r="R11" s="123"/>
+      <c r="K11" s="96" t="s">
+        <v>104</v>
+      </c>
+      <c r="L11" s="96"/>
+      <c r="M11" s="96"/>
+      <c r="N11" s="96"/>
+      <c r="O11" s="96"/>
+      <c r="P11" s="96"/>
+      <c r="Q11" s="96"/>
+      <c r="R11" s="97"/>
     </row>
     <row r="12" spans="2:18" ht="15.6">
       <c r="B12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="94"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="93"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
-      <c r="K12" s="124" t="s">
-        <v>49</v>
-      </c>
-      <c r="L12" s="124"/>
-      <c r="M12" s="124"/>
-      <c r="N12" s="124"/>
-      <c r="O12" s="125" t="s">
-        <v>50</v>
-      </c>
-      <c r="P12" s="125"/>
-      <c r="Q12" s="125"/>
-      <c r="R12" s="126"/>
-    </row>
-    <row r="13" spans="2:18" ht="15.6">
+      <c r="K12" s="96" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12" s="96"/>
+      <c r="M12" s="96"/>
+      <c r="N12" s="96"/>
+      <c r="O12" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="P12" s="96"/>
+      <c r="Q12" s="96"/>
+      <c r="R12" s="97"/>
+    </row>
+    <row r="13" spans="2:18" ht="15.6" customHeight="1">
       <c r="B13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="109" t="s">
+      <c r="C13" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
-      <c r="G13" s="110" t="s">
+      <c r="D13" s="109"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="109"/>
+      <c r="G13" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="110"/>
-      <c r="K13" s="127" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" s="127"/>
-      <c r="M13" s="127"/>
-      <c r="N13" s="127"/>
-      <c r="O13" s="120" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" s="120"/>
-      <c r="Q13" s="120"/>
-      <c r="R13" s="123"/>
-    </row>
-    <row r="14" spans="2:18" ht="15.6">
+      <c r="H13" s="109"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="109"/>
+      <c r="K13" s="94" t="s">
+        <v>49</v>
+      </c>
+      <c r="L13" s="94"/>
+      <c r="M13" s="94"/>
+      <c r="N13" s="94"/>
+      <c r="O13" s="106" t="s">
+        <v>50</v>
+      </c>
+      <c r="P13" s="106"/>
+      <c r="Q13" s="106"/>
+      <c r="R13" s="107"/>
+    </row>
+    <row r="14" spans="2:18" ht="22.8" customHeight="1">
       <c r="B14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="111" t="s">
+      <c r="C14" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="112"/>
-      <c r="E14" s="112"/>
-      <c r="F14" s="112"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="93"/>
-      <c r="I14" s="93"/>
-      <c r="J14" s="93"/>
-      <c r="K14" s="93"/>
-      <c r="L14" s="93"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="34"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="86" t="s">
+        <v>29</v>
+      </c>
+      <c r="L14" s="87"/>
+      <c r="M14" s="87"/>
+      <c r="N14" s="147"/>
+      <c r="O14" s="148" t="s">
+        <v>27</v>
+      </c>
+      <c r="P14" s="149"/>
+      <c r="Q14" s="149"/>
+      <c r="R14" s="150"/>
     </row>
     <row r="15" spans="2:18" ht="22.8">
       <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="107" t="s">
+      <c r="D15" s="76" t="s">
         <v>57</v>
       </c>
       <c r="E15" s="20"/>
-      <c r="F15" s="107" t="s">
+      <c r="F15" s="76" t="s">
         <v>68</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
-      <c r="K15" s="128" t="s">
+      <c r="K15" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="L15" s="129" t="s">
+      <c r="L15" s="79" t="s">
         <v>58</v>
       </c>
       <c r="M15" s="29"/>
@@ -2293,55 +2323,55 @@
       <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="102" t="s">
+      <c r="C17" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="103"/>
-      <c r="E17" s="103"/>
-      <c r="F17" s="103"/>
-      <c r="G17" s="103" t="s">
+      <c r="D17" s="104"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="103"/>
-      <c r="I17" s="103"/>
-      <c r="J17" s="104"/>
-      <c r="K17" s="120" t="s">
+      <c r="H17" s="104"/>
+      <c r="I17" s="104"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="L17" s="120"/>
-      <c r="M17" s="120"/>
-      <c r="N17" s="120"/>
-      <c r="O17" s="120"/>
-      <c r="P17" s="120"/>
-      <c r="Q17" s="120"/>
-      <c r="R17" s="123"/>
+      <c r="L17" s="96"/>
+      <c r="M17" s="96"/>
+      <c r="N17" s="96"/>
+      <c r="O17" s="96"/>
+      <c r="P17" s="96"/>
+      <c r="Q17" s="96"/>
+      <c r="R17" s="97"/>
     </row>
     <row r="18" spans="2:18" ht="15.6">
       <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="102" t="s">
+      <c r="C18" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="103"/>
-      <c r="E18" s="103"/>
-      <c r="F18" s="103"/>
-      <c r="G18" s="107" t="s">
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="H18" s="107"/>
-      <c r="I18" s="107"/>
-      <c r="J18" s="140"/>
-      <c r="K18" s="120" t="s">
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="L18" s="120"/>
-      <c r="M18" s="120"/>
-      <c r="N18" s="120"/>
-      <c r="O18" s="120"/>
-      <c r="P18" s="120"/>
-      <c r="Q18" s="120"/>
-      <c r="R18" s="123"/>
+      <c r="L18" s="96"/>
+      <c r="M18" s="96"/>
+      <c r="N18" s="96"/>
+      <c r="O18" s="96"/>
+      <c r="P18" s="96"/>
+      <c r="Q18" s="96"/>
+      <c r="R18" s="97"/>
     </row>
     <row r="19" spans="2:18" ht="15.6">
       <c r="B19" s="6" t="s">
@@ -2355,16 +2385,16 @@
       <c r="H19" s="20"/>
       <c r="I19" s="20"/>
       <c r="J19" s="20"/>
-      <c r="K19" s="130" t="s">
+      <c r="K19" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="L19" s="130"/>
-      <c r="M19" s="130"/>
-      <c r="N19" s="130"/>
-      <c r="O19" s="130"/>
-      <c r="P19" s="130"/>
-      <c r="Q19" s="130"/>
-      <c r="R19" s="131"/>
+      <c r="L19" s="92"/>
+      <c r="M19" s="92"/>
+      <c r="N19" s="92"/>
+      <c r="O19" s="92"/>
+      <c r="P19" s="92"/>
+      <c r="Q19" s="92"/>
+      <c r="R19" s="93"/>
     </row>
     <row r="20" spans="2:18" ht="15.6">
       <c r="B20" s="6" t="s">
@@ -2378,16 +2408,16 @@
       <c r="H20" s="20"/>
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
-      <c r="K20" s="124" t="s">
+      <c r="K20" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="L20" s="124"/>
-      <c r="M20" s="124"/>
-      <c r="N20" s="124"/>
-      <c r="O20" s="124"/>
-      <c r="P20" s="124"/>
-      <c r="Q20" s="124"/>
-      <c r="R20" s="132"/>
+      <c r="L20" s="94"/>
+      <c r="M20" s="94"/>
+      <c r="N20" s="94"/>
+      <c r="O20" s="94"/>
+      <c r="P20" s="94"/>
+      <c r="Q20" s="94"/>
+      <c r="R20" s="95"/>
     </row>
     <row r="21" spans="2:18" ht="15.6">
       <c r="B21" s="6" t="s">
@@ -2401,16 +2431,16 @@
       <c r="H21" s="38"/>
       <c r="I21" s="38"/>
       <c r="J21" s="38"/>
-      <c r="K21" s="120" t="s">
+      <c r="K21" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="L21" s="120"/>
-      <c r="M21" s="120"/>
-      <c r="N21" s="120"/>
-      <c r="O21" s="120"/>
-      <c r="P21" s="120"/>
-      <c r="Q21" s="120"/>
-      <c r="R21" s="123"/>
+      <c r="L21" s="96"/>
+      <c r="M21" s="96"/>
+      <c r="N21" s="96"/>
+      <c r="O21" s="96"/>
+      <c r="P21" s="96"/>
+      <c r="Q21" s="96"/>
+      <c r="R21" s="97"/>
     </row>
     <row r="22" spans="2:18" ht="15.6">
       <c r="B22" s="6" t="s">
@@ -2424,16 +2454,16 @@
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
       <c r="J22" s="20"/>
-      <c r="K22" s="124" t="s">
+      <c r="K22" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="L22" s="124"/>
-      <c r="M22" s="124"/>
-      <c r="N22" s="124"/>
-      <c r="O22" s="124"/>
-      <c r="P22" s="124"/>
-      <c r="Q22" s="124"/>
-      <c r="R22" s="132"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="94"/>
+      <c r="N22" s="94"/>
+      <c r="O22" s="94"/>
+      <c r="P22" s="94"/>
+      <c r="Q22" s="94"/>
+      <c r="R22" s="95"/>
     </row>
     <row r="23" spans="2:18" ht="15.6" customHeight="1">
       <c r="B23" s="6" t="s">
@@ -2447,69 +2477,69 @@
       <c r="H23" s="20"/>
       <c r="I23" s="20"/>
       <c r="J23" s="20"/>
-      <c r="K23" s="133" t="s">
+      <c r="K23" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="L23" s="143"/>
-      <c r="M23" s="143"/>
-      <c r="N23" s="143"/>
-      <c r="O23" s="143"/>
-      <c r="P23" s="143"/>
-      <c r="Q23" s="143"/>
-      <c r="R23" s="134"/>
+      <c r="L23" s="87"/>
+      <c r="M23" s="87"/>
+      <c r="N23" s="87"/>
+      <c r="O23" s="87"/>
+      <c r="P23" s="87"/>
+      <c r="Q23" s="87"/>
+      <c r="R23" s="88"/>
     </row>
     <row r="24" spans="2:18" ht="16.2" customHeight="1" thickBot="1">
       <c r="B24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="99" t="s">
+      <c r="C24" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="100"/>
-      <c r="E24" s="100"/>
-      <c r="F24" s="100"/>
-      <c r="G24" s="100"/>
-      <c r="H24" s="100"/>
-      <c r="I24" s="100"/>
-      <c r="J24" s="101"/>
-      <c r="K24" s="133" t="s">
+      <c r="D24" s="99"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="99"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="99"/>
+      <c r="J24" s="100"/>
+      <c r="K24" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="L24" s="134"/>
-      <c r="M24" s="142" t="s">
+      <c r="L24" s="88"/>
+      <c r="M24" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="N24" s="142" t="s">
+      <c r="N24" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="O24" s="144" t="s">
+      <c r="O24" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="P24" s="145"/>
-      <c r="Q24" s="145"/>
-      <c r="R24" s="146"/>
+      <c r="P24" s="90"/>
+      <c r="Q24" s="90"/>
+      <c r="R24" s="91"/>
     </row>
     <row r="26" spans="2:18">
-      <c r="C26" s="139" t="s">
+      <c r="C26" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="139"/>
-      <c r="E26" s="139"/>
-      <c r="F26" s="139"/>
-      <c r="G26" s="139"/>
-      <c r="H26" s="139"/>
-      <c r="I26" s="139"/>
-      <c r="J26" s="139"/>
-      <c r="K26" s="138" t="s">
+      <c r="D26" s="85"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="85"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="L26" s="138"/>
-      <c r="M26" s="138"/>
-      <c r="N26" s="138"/>
-      <c r="O26" s="138"/>
-      <c r="P26" s="138"/>
-      <c r="Q26" s="138"/>
-      <c r="R26" s="138"/>
+      <c r="L26" s="84"/>
+      <c r="M26" s="84"/>
+      <c r="N26" s="84"/>
+      <c r="O26" s="84"/>
+      <c r="P26" s="84"/>
+      <c r="Q26" s="84"/>
+      <c r="R26" s="84"/>
     </row>
     <row r="28" spans="2:18">
       <c r="C28" t="s">
@@ -2517,7 +2547,29 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="32">
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="O11:R11"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="O14:R14"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="O9:R9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="O10:R10"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="O12:R12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="O13:R13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="K17:R17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="K18:R18"/>
     <mergeCell ref="K26:R26"/>
     <mergeCell ref="C26:J26"/>
     <mergeCell ref="K23:R23"/>
@@ -2528,26 +2580,6 @@
     <mergeCell ref="K22:R22"/>
     <mergeCell ref="C24:J24"/>
     <mergeCell ref="K24:L24"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="K17:R17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="K18:R18"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="O12:R12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="O13:R13"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="O9:R9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="O10:R10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="O11:R11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2557,60 +2589,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D8C36D-939B-444F-978B-726CF9EB90A8}">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16:Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:17" ht="16.2" thickBot="1">
-      <c r="A1" s="137"/>
-      <c r="B1" s="95">
+      <c r="A1" s="80"/>
+      <c r="B1" s="72">
         <v>0</v>
       </c>
-      <c r="C1" s="96">
+      <c r="C1" s="73">
         <v>1</v>
       </c>
-      <c r="D1" s="97">
+      <c r="D1" s="74">
         <v>2</v>
       </c>
-      <c r="E1" s="97">
+      <c r="E1" s="74">
         <v>3</v>
       </c>
-      <c r="F1" s="97">
+      <c r="F1" s="74">
         <v>4</v>
       </c>
-      <c r="G1" s="97">
+      <c r="G1" s="74">
         <v>5</v>
       </c>
-      <c r="H1" s="97">
-        <v>6</v>
-      </c>
-      <c r="I1" s="97">
+      <c r="H1" s="74">
+        <v>6</v>
+      </c>
+      <c r="I1" s="74">
         <v>7</v>
       </c>
-      <c r="J1" s="97">
+      <c r="J1" s="74">
         <v>8</v>
       </c>
-      <c r="K1" s="97">
+      <c r="K1" s="74">
         <v>9</v>
       </c>
-      <c r="L1" s="97" t="s">
+      <c r="L1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="97" t="s">
+      <c r="M1" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="97" t="s">
+      <c r="N1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="97" t="s">
+      <c r="O1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="97" t="s">
+      <c r="P1" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="98" t="s">
+      <c r="Q1" s="75" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2618,12 +2650,12 @@
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="111" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="117"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="113"/>
       <c r="F2" s="24" t="s">
         <v>6</v>
       </c>
@@ -2633,21 +2665,21 @@
       <c r="H2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="141" t="s">
+      <c r="I2" s="82" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="118" t="s">
+      <c r="J2" s="114" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="118"/>
-      <c r="L2" s="118"/>
-      <c r="M2" s="118"/>
-      <c r="N2" s="118" t="s">
+      <c r="K2" s="114"/>
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+      <c r="N2" s="114" t="s">
         <v>80</v>
       </c>
-      <c r="O2" s="118"/>
-      <c r="P2" s="118"/>
-      <c r="Q2" s="119"/>
+      <c r="O2" s="114"/>
+      <c r="P2" s="114"/>
+      <c r="Q2" s="115"/>
     </row>
     <row r="3" spans="1:17" ht="15.6">
       <c r="A3" s="14" t="s">
@@ -2677,29 +2709,29 @@
       <c r="I3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="120" t="s">
+      <c r="J3" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
-      <c r="N3" s="121" t="s">
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="116" t="s">
         <v>82</v>
       </c>
-      <c r="O3" s="121"/>
-      <c r="P3" s="121"/>
-      <c r="Q3" s="122"/>
+      <c r="O3" s="116"/>
+      <c r="P3" s="116"/>
+      <c r="Q3" s="117"/>
     </row>
     <row r="4" spans="1:17" ht="15.6">
       <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="113" t="s">
+      <c r="B4" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="114"/>
-      <c r="D4" s="114"/>
-      <c r="E4" s="114"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
       <c r="F4" s="24" t="s">
         <v>6</v>
       </c>
@@ -2712,18 +2744,18 @@
       <c r="I4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="120" t="s">
+      <c r="J4" s="96" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
-      <c r="M4" s="120"/>
-      <c r="N4" s="120" t="s">
+      <c r="K4" s="96"/>
+      <c r="L4" s="96"/>
+      <c r="M4" s="96"/>
+      <c r="N4" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="O4" s="120"/>
-      <c r="P4" s="120"/>
-      <c r="Q4" s="123"/>
+      <c r="O4" s="96"/>
+      <c r="P4" s="96"/>
+      <c r="Q4" s="97"/>
     </row>
     <row r="5" spans="1:17" ht="15.6">
       <c r="A5" s="11" t="s">
@@ -2753,58 +2785,58 @@
       <c r="I5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="124" t="s">
+      <c r="J5" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="K5" s="124"/>
-      <c r="L5" s="124"/>
-      <c r="M5" s="124"/>
-      <c r="N5" s="125" t="s">
+      <c r="K5" s="94"/>
+      <c r="L5" s="94"/>
+      <c r="M5" s="94"/>
+      <c r="N5" s="106" t="s">
         <v>86</v>
       </c>
-      <c r="O5" s="125"/>
-      <c r="P5" s="125"/>
-      <c r="Q5" s="126"/>
+      <c r="O5" s="106"/>
+      <c r="P5" s="106"/>
+      <c r="Q5" s="107"/>
     </row>
     <row r="6" spans="1:17" ht="15.6">
       <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="108" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110" t="s">
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="127" t="s">
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="110" t="s">
         <v>87</v>
       </c>
-      <c r="K6" s="127"/>
-      <c r="L6" s="127"/>
-      <c r="M6" s="127"/>
-      <c r="N6" s="120" t="s">
+      <c r="K6" s="110"/>
+      <c r="L6" s="110"/>
+      <c r="M6" s="110"/>
+      <c r="N6" s="96" t="s">
         <v>88</v>
       </c>
-      <c r="O6" s="120"/>
-      <c r="P6" s="120"/>
-      <c r="Q6" s="123"/>
+      <c r="O6" s="96"/>
+      <c r="P6" s="96"/>
+      <c r="Q6" s="97"/>
     </row>
     <row r="7" spans="1:17" ht="15.6">
       <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="111" t="s">
+      <c r="B7" s="101" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="102"/>
       <c r="F7" s="24" t="s">
         <v>6</v>
       </c>
@@ -2846,16 +2878,16 @@
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="107" t="s">
+      <c r="C8" s="76" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="107" t="s">
+      <c r="E8" s="76" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="24" t="s">
@@ -2870,10 +2902,10 @@
       <c r="I8" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="128" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="129" t="s">
+      <c r="J8" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="79" t="s">
         <v>6</v>
       </c>
       <c r="L8" s="24" t="s">
@@ -2952,61 +2984,61 @@
       <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="102" t="s">
+      <c r="B10" s="103" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="103"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="103"/>
-      <c r="F10" s="103" t="s">
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="104" t="s">
         <v>76</v>
       </c>
-      <c r="G10" s="103"/>
-      <c r="H10" s="103"/>
-      <c r="I10" s="104"/>
-      <c r="J10" s="120" t="s">
+      <c r="G10" s="104"/>
+      <c r="H10" s="104"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="96" t="s">
         <v>94</v>
       </c>
-      <c r="K10" s="120"/>
-      <c r="L10" s="120"/>
-      <c r="M10" s="120"/>
-      <c r="N10" s="120"/>
-      <c r="O10" s="120"/>
-      <c r="P10" s="120"/>
-      <c r="Q10" s="123"/>
+      <c r="K10" s="96"/>
+      <c r="L10" s="96"/>
+      <c r="M10" s="96"/>
+      <c r="N10" s="96"/>
+      <c r="O10" s="96"/>
+      <c r="P10" s="96"/>
+      <c r="Q10" s="97"/>
     </row>
     <row r="11" spans="1:17" ht="15.6">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="102" t="s">
+      <c r="B11" s="103" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="107" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="107" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="107" t="s">
-        <v>6</v>
-      </c>
-      <c r="I11" s="140" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="120" t="s">
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="104"/>
+      <c r="F11" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="96" t="s">
         <v>95</v>
       </c>
-      <c r="K11" s="120"/>
-      <c r="L11" s="120"/>
-      <c r="M11" s="120"/>
-      <c r="N11" s="120"/>
-      <c r="O11" s="120"/>
-      <c r="P11" s="120"/>
-      <c r="Q11" s="123"/>
+      <c r="K11" s="96"/>
+      <c r="L11" s="96"/>
+      <c r="M11" s="96"/>
+      <c r="N11" s="96"/>
+      <c r="O11" s="96"/>
+      <c r="P11" s="96"/>
+      <c r="Q11" s="97"/>
     </row>
     <row r="12" spans="1:17" ht="15.6">
       <c r="A12" s="6" t="s">
@@ -3036,16 +3068,16 @@
       <c r="I12" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="130" t="s">
+      <c r="J12" s="92" t="s">
         <v>96</v>
       </c>
-      <c r="K12" s="130"/>
-      <c r="L12" s="130"/>
-      <c r="M12" s="130"/>
-      <c r="N12" s="130"/>
-      <c r="O12" s="130"/>
-      <c r="P12" s="130"/>
-      <c r="Q12" s="131"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="92"/>
+      <c r="M12" s="92"/>
+      <c r="N12" s="92"/>
+      <c r="O12" s="92"/>
+      <c r="P12" s="92"/>
+      <c r="Q12" s="93"/>
     </row>
     <row r="13" spans="1:17" ht="15.6">
       <c r="A13" s="6" t="s">
@@ -3075,16 +3107,16 @@
       <c r="I13" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="124" t="s">
+      <c r="J13" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="K13" s="124"/>
-      <c r="L13" s="124"/>
-      <c r="M13" s="124"/>
-      <c r="N13" s="124"/>
-      <c r="O13" s="124"/>
-      <c r="P13" s="124"/>
-      <c r="Q13" s="132"/>
+      <c r="K13" s="94"/>
+      <c r="L13" s="94"/>
+      <c r="M13" s="94"/>
+      <c r="N13" s="94"/>
+      <c r="O13" s="94"/>
+      <c r="P13" s="94"/>
+      <c r="Q13" s="95"/>
     </row>
     <row r="14" spans="1:17" ht="15.6">
       <c r="A14" s="6" t="s">
@@ -3114,16 +3146,16 @@
       <c r="I14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J14" s="120" t="s">
+      <c r="J14" s="96" t="s">
         <v>98</v>
       </c>
-      <c r="K14" s="120"/>
-      <c r="L14" s="120"/>
-      <c r="M14" s="120"/>
-      <c r="N14" s="120"/>
-      <c r="O14" s="120"/>
-      <c r="P14" s="120"/>
-      <c r="Q14" s="123"/>
+      <c r="K14" s="96"/>
+      <c r="L14" s="96"/>
+      <c r="M14" s="96"/>
+      <c r="N14" s="96"/>
+      <c r="O14" s="96"/>
+      <c r="P14" s="96"/>
+      <c r="Q14" s="97"/>
     </row>
     <row r="15" spans="1:17" ht="15.6">
       <c r="A15" s="6" t="s">
@@ -3153,16 +3185,16 @@
       <c r="I15" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J15" s="124" t="s">
+      <c r="J15" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="K15" s="124"/>
-      <c r="L15" s="124"/>
-      <c r="M15" s="124"/>
-      <c r="N15" s="124"/>
-      <c r="O15" s="124"/>
-      <c r="P15" s="124"/>
-      <c r="Q15" s="132"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="94"/>
+      <c r="O15" s="94"/>
+      <c r="P15" s="94"/>
+      <c r="Q15" s="95"/>
     </row>
     <row r="16" spans="1:17" ht="15.6">
       <c r="A16" s="6" t="s">
@@ -3192,96 +3224,96 @@
       <c r="I16" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="133" t="s">
+      <c r="J16" s="86" t="s">
         <v>103</v>
       </c>
-      <c r="K16" s="143"/>
-      <c r="L16" s="143"/>
-      <c r="M16" s="143"/>
-      <c r="N16" s="143"/>
-      <c r="O16" s="143"/>
-      <c r="P16" s="143"/>
-      <c r="Q16" s="134"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="87"/>
+      <c r="N16" s="87"/>
+      <c r="O16" s="87"/>
+      <c r="P16" s="87"/>
+      <c r="Q16" s="88"/>
     </row>
     <row r="17" spans="1:17" ht="16.2" thickBot="1">
       <c r="A17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="99" t="s">
+      <c r="B17" s="98" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="100"/>
-      <c r="D17" s="100"/>
-      <c r="E17" s="100"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="100"/>
-      <c r="H17" s="100"/>
-      <c r="I17" s="101"/>
-      <c r="J17" s="133" t="s">
+      <c r="C17" s="99"/>
+      <c r="D17" s="99"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="99"/>
+      <c r="G17" s="99"/>
+      <c r="H17" s="99"/>
+      <c r="I17" s="100"/>
+      <c r="J17" s="86" t="s">
         <v>90</v>
       </c>
-      <c r="K17" s="134"/>
-      <c r="L17" s="135" t="s">
+      <c r="K17" s="88"/>
+      <c r="L17" s="120" t="s">
         <v>92</v>
       </c>
-      <c r="M17" s="135"/>
-      <c r="N17" s="135" t="s">
+      <c r="M17" s="120"/>
+      <c r="N17" s="120" t="s">
         <v>91</v>
       </c>
-      <c r="O17" s="135"/>
-      <c r="P17" s="135" t="s">
+      <c r="O17" s="120"/>
+      <c r="P17" s="120" t="s">
         <v>93</v>
       </c>
-      <c r="Q17" s="136"/>
+      <c r="Q17" s="121"/>
     </row>
     <row r="18" spans="1:17" ht="15" thickBot="1"/>
     <row r="19" spans="1:17" ht="16.2" thickBot="1">
-      <c r="B19" s="95">
+      <c r="B19" s="72">
         <v>0</v>
       </c>
-      <c r="C19" s="96">
+      <c r="C19" s="73">
         <v>1</v>
       </c>
-      <c r="D19" s="97">
+      <c r="D19" s="74">
         <v>2</v>
       </c>
-      <c r="E19" s="97">
+      <c r="E19" s="74">
         <v>3</v>
       </c>
-      <c r="F19" s="97">
+      <c r="F19" s="74">
         <v>4</v>
       </c>
-      <c r="G19" s="97">
+      <c r="G19" s="74">
         <v>5</v>
       </c>
-      <c r="H19" s="97">
-        <v>6</v>
-      </c>
-      <c r="I19" s="97">
+      <c r="H19" s="74">
+        <v>6</v>
+      </c>
+      <c r="I19" s="74">
         <v>7</v>
       </c>
-      <c r="J19" s="97">
+      <c r="J19" s="74">
         <v>8</v>
       </c>
-      <c r="K19" s="97">
+      <c r="K19" s="74">
         <v>9</v>
       </c>
-      <c r="L19" s="97" t="s">
+      <c r="L19" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="M19" s="97" t="s">
+      <c r="M19" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="N19" s="97" t="s">
+      <c r="N19" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="O19" s="97" t="s">
+      <c r="O19" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="P19" s="97" t="s">
+      <c r="P19" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="Q19" s="98" t="s">
+      <c r="Q19" s="75" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3289,30 +3321,30 @@
       <c r="A20" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="115">
+      <c r="B20" s="111">
         <v>33.299999999999997</v>
       </c>
-      <c r="C20" s="116"/>
-      <c r="D20" s="116"/>
-      <c r="E20" s="117"/>
+      <c r="C20" s="112"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="113"/>
       <c r="F20" s="24"/>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="141">
+      <c r="I20" s="82">
         <v>119</v>
       </c>
-      <c r="J20" s="118">
+      <c r="J20" s="114">
         <v>33.299999999999997</v>
       </c>
-      <c r="K20" s="118"/>
-      <c r="L20" s="118"/>
-      <c r="M20" s="118"/>
-      <c r="N20" s="118">
+      <c r="K20" s="114"/>
+      <c r="L20" s="114"/>
+      <c r="M20" s="114"/>
+      <c r="N20" s="114">
         <v>128.79</v>
       </c>
-      <c r="O20" s="118"/>
-      <c r="P20" s="118"/>
-      <c r="Q20" s="119"/>
+      <c r="O20" s="114"/>
+      <c r="P20" s="114"/>
+      <c r="Q20" s="115"/>
     </row>
     <row r="21" spans="1:17" ht="15.6">
       <c r="A21" s="14" t="s">
@@ -3326,116 +3358,116 @@
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
       <c r="I21" s="24"/>
-      <c r="J21" s="120">
+      <c r="J21" s="96">
         <v>28.79</v>
       </c>
-      <c r="K21" s="120"/>
-      <c r="L21" s="120"/>
-      <c r="M21" s="120"/>
-      <c r="N21" s="121">
+      <c r="K21" s="96"/>
+      <c r="L21" s="96"/>
+      <c r="M21" s="96"/>
+      <c r="N21" s="116">
         <v>100</v>
       </c>
-      <c r="O21" s="121"/>
-      <c r="P21" s="121"/>
-      <c r="Q21" s="122"/>
+      <c r="O21" s="116"/>
+      <c r="P21" s="116"/>
+      <c r="Q21" s="117"/>
     </row>
     <row r="22" spans="1:17" ht="15.6">
       <c r="A22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="113">
+      <c r="B22" s="118">
         <v>8.8888800000000003</v>
       </c>
-      <c r="C22" s="114"/>
-      <c r="D22" s="114"/>
-      <c r="E22" s="114"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
       <c r="F22" s="24"/>
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
       <c r="I22" s="24"/>
-      <c r="J22" s="120">
+      <c r="J22" s="96">
         <v>5.5</v>
       </c>
-      <c r="K22" s="120"/>
-      <c r="L22" s="120"/>
-      <c r="M22" s="120"/>
-      <c r="N22" s="120">
+      <c r="K22" s="96"/>
+      <c r="L22" s="96"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="96">
         <v>2.5</v>
       </c>
-      <c r="O22" s="120"/>
-      <c r="P22" s="120"/>
-      <c r="Q22" s="123"/>
+      <c r="O22" s="96"/>
+      <c r="P22" s="96"/>
+      <c r="Q22" s="97"/>
     </row>
     <row r="23" spans="1:17" ht="15.6">
       <c r="A23" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="93"/>
-      <c r="E23" s="93"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
       <c r="I23" s="27"/>
-      <c r="J23" s="124">
+      <c r="J23" s="94">
         <v>1.4</v>
       </c>
-      <c r="K23" s="124"/>
-      <c r="L23" s="124"/>
-      <c r="M23" s="124"/>
-      <c r="N23" s="125">
+      <c r="K23" s="94"/>
+      <c r="L23" s="94"/>
+      <c r="M23" s="94"/>
+      <c r="N23" s="106">
         <v>13.2</v>
       </c>
-      <c r="O23" s="125"/>
-      <c r="P23" s="125"/>
-      <c r="Q23" s="126"/>
+      <c r="O23" s="106"/>
+      <c r="P23" s="106"/>
+      <c r="Q23" s="107"/>
     </row>
     <row r="24" spans="1:17" ht="15.6">
       <c r="A24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="109">
+      <c r="B24" s="108">
         <v>0.15</v>
       </c>
-      <c r="C24" s="110"/>
-      <c r="D24" s="110"/>
-      <c r="E24" s="110"/>
-      <c r="F24" s="110">
+      <c r="C24" s="109"/>
+      <c r="D24" s="109"/>
+      <c r="E24" s="109"/>
+      <c r="F24" s="109">
         <v>11.7</v>
       </c>
-      <c r="G24" s="110"/>
-      <c r="H24" s="110"/>
-      <c r="I24" s="110"/>
-      <c r="J24" s="127">
+      <c r="G24" s="109"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="109"/>
+      <c r="J24" s="110">
         <v>0</v>
       </c>
-      <c r="K24" s="127"/>
-      <c r="L24" s="127"/>
-      <c r="M24" s="127"/>
-      <c r="N24" s="120">
+      <c r="K24" s="110"/>
+      <c r="L24" s="110"/>
+      <c r="M24" s="110"/>
+      <c r="N24" s="96">
         <v>8</v>
       </c>
-      <c r="O24" s="120"/>
-      <c r="P24" s="120"/>
-      <c r="Q24" s="123"/>
+      <c r="O24" s="96"/>
+      <c r="P24" s="96"/>
+      <c r="Q24" s="97"/>
     </row>
     <row r="25" spans="1:17" ht="15.6">
       <c r="A25" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="111">
+      <c r="B25" s="101">
         <v>125732</v>
       </c>
-      <c r="C25" s="112"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="112"/>
-      <c r="F25" s="93"/>
-      <c r="G25" s="93"/>
-      <c r="H25" s="93"/>
-      <c r="I25" s="93"/>
-      <c r="J25" s="93"/>
-      <c r="K25" s="93"/>
+      <c r="C25" s="102"/>
+      <c r="D25" s="102"/>
+      <c r="E25" s="102"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="70"/>
       <c r="L25" s="29"/>
       <c r="M25" s="29"/>
       <c r="N25" s="20"/>
@@ -3447,24 +3479,24 @@
       <c r="A26" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="108">
+      <c r="B26" s="77">
         <v>-1</v>
       </c>
-      <c r="C26" s="107">
+      <c r="C26" s="76">
         <v>0</v>
       </c>
       <c r="D26" s="20"/>
-      <c r="E26" s="107">
+      <c r="E26" s="76">
         <v>0</v>
       </c>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
-      <c r="J26" s="128">
+      <c r="J26" s="78">
         <v>0</v>
       </c>
-      <c r="K26" s="129">
+      <c r="K26" s="79">
         <v>0</v>
       </c>
       <c r="L26" s="29"/>
@@ -3499,55 +3531,55 @@
       <c r="A28" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="102">
+      <c r="B28" s="103">
         <v>0.1234</v>
       </c>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="103"/>
-      <c r="F28" s="103">
+      <c r="C28" s="104"/>
+      <c r="D28" s="104"/>
+      <c r="E28" s="104"/>
+      <c r="F28" s="104">
         <v>2.3216999999999999</v>
       </c>
-      <c r="G28" s="103"/>
-      <c r="H28" s="103"/>
-      <c r="I28" s="104"/>
-      <c r="J28" s="120">
+      <c r="G28" s="104"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="105"/>
+      <c r="J28" s="96">
         <v>0.12</v>
       </c>
-      <c r="K28" s="120"/>
-      <c r="L28" s="120"/>
-      <c r="M28" s="120"/>
-      <c r="N28" s="120"/>
-      <c r="O28" s="120"/>
-      <c r="P28" s="120"/>
-      <c r="Q28" s="123"/>
+      <c r="K28" s="96"/>
+      <c r="L28" s="96"/>
+      <c r="M28" s="96"/>
+      <c r="N28" s="96"/>
+      <c r="O28" s="96"/>
+      <c r="P28" s="96"/>
+      <c r="Q28" s="97"/>
     </row>
     <row r="29" spans="1:17" ht="15.6">
       <c r="A29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="102">
+      <c r="B29" s="103">
         <v>128.78800000000001</v>
       </c>
-      <c r="C29" s="103"/>
-      <c r="D29" s="103"/>
-      <c r="E29" s="103"/>
-      <c r="F29" s="107">
+      <c r="C29" s="104"/>
+      <c r="D29" s="104"/>
+      <c r="E29" s="104"/>
+      <c r="F29" s="76">
         <v>0</v>
       </c>
-      <c r="G29" s="107"/>
-      <c r="H29" s="107"/>
-      <c r="I29" s="140"/>
-      <c r="J29" s="120">
+      <c r="G29" s="76"/>
+      <c r="H29" s="76"/>
+      <c r="I29" s="81"/>
+      <c r="J29" s="96">
         <v>1</v>
       </c>
-      <c r="K29" s="120"/>
-      <c r="L29" s="120"/>
-      <c r="M29" s="120"/>
-      <c r="N29" s="120"/>
-      <c r="O29" s="120"/>
-      <c r="P29" s="120"/>
-      <c r="Q29" s="123"/>
+      <c r="K29" s="96"/>
+      <c r="L29" s="96"/>
+      <c r="M29" s="96"/>
+      <c r="N29" s="96"/>
+      <c r="O29" s="96"/>
+      <c r="P29" s="96"/>
+      <c r="Q29" s="97"/>
     </row>
     <row r="30" spans="1:17" ht="15.6">
       <c r="A30" s="6" t="s">
@@ -3561,16 +3593,16 @@
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
-      <c r="J30" s="130">
+      <c r="J30" s="92">
         <v>13.289020320000001</v>
       </c>
-      <c r="K30" s="130"/>
-      <c r="L30" s="130"/>
-      <c r="M30" s="130"/>
-      <c r="N30" s="130"/>
-      <c r="O30" s="130"/>
-      <c r="P30" s="130"/>
-      <c r="Q30" s="131"/>
+      <c r="K30" s="92"/>
+      <c r="L30" s="92"/>
+      <c r="M30" s="92"/>
+      <c r="N30" s="92"/>
+      <c r="O30" s="92"/>
+      <c r="P30" s="92"/>
+      <c r="Q30" s="93"/>
     </row>
     <row r="31" spans="1:17" ht="15.6">
       <c r="A31" s="6" t="s">
@@ -3584,16 +3616,16 @@
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
-      <c r="J31" s="124">
+      <c r="J31" s="94">
         <v>0.11111111110000001</v>
       </c>
-      <c r="K31" s="124"/>
-      <c r="L31" s="124"/>
-      <c r="M31" s="124"/>
-      <c r="N31" s="124"/>
-      <c r="O31" s="124"/>
-      <c r="P31" s="124"/>
-      <c r="Q31" s="132"/>
+      <c r="K31" s="94"/>
+      <c r="L31" s="94"/>
+      <c r="M31" s="94"/>
+      <c r="N31" s="94"/>
+      <c r="O31" s="94"/>
+      <c r="P31" s="94"/>
+      <c r="Q31" s="95"/>
     </row>
     <row r="32" spans="1:17" ht="15.6">
       <c r="A32" s="6" t="s">
@@ -3607,16 +3639,16 @@
       <c r="G32" s="38"/>
       <c r="H32" s="38"/>
       <c r="I32" s="38"/>
-      <c r="J32" s="120">
+      <c r="J32" s="96">
         <v>0</v>
       </c>
-      <c r="K32" s="120"/>
-      <c r="L32" s="120"/>
-      <c r="M32" s="120"/>
-      <c r="N32" s="120"/>
-      <c r="O32" s="120"/>
-      <c r="P32" s="120"/>
-      <c r="Q32" s="123"/>
+      <c r="K32" s="96"/>
+      <c r="L32" s="96"/>
+      <c r="M32" s="96"/>
+      <c r="N32" s="96"/>
+      <c r="O32" s="96"/>
+      <c r="P32" s="96"/>
+      <c r="Q32" s="97"/>
     </row>
     <row r="33" spans="1:17" ht="15.6">
       <c r="A33" s="6" t="s">
@@ -3630,16 +3662,16 @@
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
-      <c r="J33" s="124">
+      <c r="J33" s="94">
         <v>1010101</v>
       </c>
-      <c r="K33" s="124"/>
-      <c r="L33" s="124"/>
-      <c r="M33" s="124"/>
-      <c r="N33" s="124"/>
-      <c r="O33" s="124"/>
-      <c r="P33" s="124"/>
-      <c r="Q33" s="132"/>
+      <c r="K33" s="94"/>
+      <c r="L33" s="94"/>
+      <c r="M33" s="94"/>
+      <c r="N33" s="94"/>
+      <c r="O33" s="94"/>
+      <c r="P33" s="94"/>
+      <c r="Q33" s="95"/>
     </row>
     <row r="34" spans="1:17" ht="15.6">
       <c r="A34" s="6" t="s">
@@ -3653,77 +3685,70 @@
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
-      <c r="J34" s="133" t="s">
+      <c r="J34" s="86" t="s">
         <v>101</v>
       </c>
-      <c r="K34" s="143"/>
-      <c r="L34" s="143"/>
-      <c r="M34" s="143"/>
-      <c r="N34" s="143"/>
-      <c r="O34" s="143"/>
-      <c r="P34" s="143"/>
-      <c r="Q34" s="134"/>
+      <c r="K34" s="87"/>
+      <c r="L34" s="87"/>
+      <c r="M34" s="87"/>
+      <c r="N34" s="87"/>
+      <c r="O34" s="87"/>
+      <c r="P34" s="87"/>
+      <c r="Q34" s="88"/>
     </row>
     <row r="35" spans="1:17" ht="16.2" thickBot="1">
       <c r="A35" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="99" t="s">
+      <c r="B35" s="98" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="100"/>
-      <c r="D35" s="100"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="100"/>
-      <c r="G35" s="100"/>
-      <c r="H35" s="100"/>
-      <c r="I35" s="101"/>
-      <c r="J35" s="133">
+      <c r="C35" s="99"/>
+      <c r="D35" s="99"/>
+      <c r="E35" s="99"/>
+      <c r="F35" s="99"/>
+      <c r="G35" s="99"/>
+      <c r="H35" s="99"/>
+      <c r="I35" s="100"/>
+      <c r="J35" s="86">
         <v>2021</v>
       </c>
-      <c r="K35" s="134"/>
-      <c r="L35" s="135">
+      <c r="K35" s="88"/>
+      <c r="L35" s="120">
         <v>1</v>
       </c>
-      <c r="M35" s="135"/>
-      <c r="N35" s="135">
+      <c r="M35" s="120"/>
+      <c r="N35" s="120">
         <v>8</v>
       </c>
-      <c r="O35" s="135"/>
-      <c r="P35" s="135">
+      <c r="O35" s="120"/>
+      <c r="P35" s="120">
         <v>23</v>
       </c>
-      <c r="Q35" s="136"/>
+      <c r="Q35" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="J30:Q30"/>
-    <mergeCell ref="J31:Q31"/>
-    <mergeCell ref="J32:Q32"/>
-    <mergeCell ref="J33:Q33"/>
-    <mergeCell ref="J34:Q34"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="P35:Q35"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="J28:Q28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="J29:Q29"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="N23:Q23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="N24:Q24"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="N21:Q21"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="J10:Q10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="J11:Q11"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="J22:M22"/>
     <mergeCell ref="N22:Q22"/>
@@ -3737,26 +3762,33 @@
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="N17:O17"/>
     <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="J10:Q10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="J11:Q11"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="N21:Q21"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="N23:Q23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="N24:Q24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="J28:Q28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="J29:Q29"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="J30:Q30"/>
+    <mergeCell ref="J31:Q31"/>
+    <mergeCell ref="J32:Q32"/>
+    <mergeCell ref="J33:Q33"/>
+    <mergeCell ref="J34:Q34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3838,18 +3870,18 @@
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65" t="s">
+      <c r="D8" s="137"/>
+      <c r="E8" s="137"/>
+      <c r="F8" s="137"/>
+      <c r="G8" s="137" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
+      <c r="H8" s="137"/>
+      <c r="I8" s="137"/>
+      <c r="J8" s="137"/>
       <c r="K8" s="16"/>
       <c r="L8" s="17"/>
       <c r="M8" s="46"/>
@@ -3858,36 +3890,36 @@
       <c r="P8" s="46"/>
       <c r="Q8" s="18"/>
       <c r="R8" s="19"/>
-      <c r="S8" s="50" t="s">
+      <c r="S8" s="124" t="s">
         <v>7</v>
       </c>
-      <c r="T8" s="51"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="51"/>
+      <c r="T8" s="125"/>
+      <c r="U8" s="125"/>
+      <c r="V8" s="125"/>
+      <c r="W8" s="125"/>
     </row>
     <row r="9" spans="1:23" ht="26.4" customHeight="1">
       <c r="B9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="60" t="s">
+      <c r="D9" s="130"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="130"/>
+      <c r="G9" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="54" t="s">
+      <c r="H9" s="134"/>
+      <c r="I9" s="134"/>
+      <c r="J9" s="134"/>
+      <c r="K9" s="128" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="54"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="54"/>
+      <c r="L9" s="128"/>
+      <c r="M9" s="128"/>
+      <c r="N9" s="128"/>
       <c r="O9" s="47" t="s">
         <v>30</v>
       </c>
@@ -3900,70 +3932,70 @@
       <c r="R9" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="S9" s="50"/>
-      <c r="T9" s="51"/>
-      <c r="U9" s="51"/>
-      <c r="V9" s="51"/>
-      <c r="W9" s="51"/>
+      <c r="S9" s="124"/>
+      <c r="T9" s="125"/>
+      <c r="U9" s="125"/>
+      <c r="V9" s="125"/>
+      <c r="W9" s="125"/>
     </row>
     <row r="10" spans="1:23" ht="22.8" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="129" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56" t="s">
+      <c r="D10" s="130"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="130"/>
+      <c r="G10" s="130"/>
+      <c r="H10" s="130"/>
+      <c r="I10" s="130"/>
+      <c r="J10" s="130"/>
+      <c r="K10" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="57"/>
-      <c r="S10" s="52" t="s">
+      <c r="L10" s="130"/>
+      <c r="M10" s="130"/>
+      <c r="N10" s="130"/>
+      <c r="O10" s="130"/>
+      <c r="P10" s="130"/>
+      <c r="Q10" s="130"/>
+      <c r="R10" s="131"/>
+      <c r="S10" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="T10" s="52"/>
-      <c r="U10" s="52"/>
-      <c r="V10" s="52"/>
-      <c r="W10" s="52"/>
+      <c r="T10" s="126"/>
+      <c r="U10" s="126"/>
+      <c r="V10" s="126"/>
+      <c r="W10" s="126"/>
     </row>
     <row r="11" spans="1:23" ht="22.8" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="132" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="60" t="s">
+      <c r="D11" s="133"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="133"/>
+      <c r="G11" s="133"/>
+      <c r="H11" s="133"/>
+      <c r="I11" s="133"/>
+      <c r="J11" s="133"/>
+      <c r="K11" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="60"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="60"/>
-      <c r="R11" s="61"/>
+      <c r="L11" s="134"/>
+      <c r="M11" s="134"/>
+      <c r="N11" s="134"/>
+      <c r="O11" s="134"/>
+      <c r="P11" s="134"/>
+      <c r="Q11" s="134"/>
+      <c r="R11" s="135"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
@@ -3975,26 +4007,26 @@
       <c r="B12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="129" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="60" t="s">
+      <c r="D12" s="130"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="130"/>
+      <c r="K12" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="60"/>
-      <c r="O12" s="60"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="60"/>
-      <c r="R12" s="61"/>
+      <c r="L12" s="134"/>
+      <c r="M12" s="134"/>
+      <c r="N12" s="134"/>
+      <c r="O12" s="134"/>
+      <c r="P12" s="134"/>
+      <c r="Q12" s="134"/>
+      <c r="R12" s="135"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
@@ -4022,13 +4054,13 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="21"/>
       <c r="R13" s="34"/>
-      <c r="S13" s="52" t="s">
+      <c r="S13" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="T13" s="53"/>
-      <c r="U13" s="53"/>
-      <c r="V13" s="53"/>
-      <c r="W13" s="53"/>
+      <c r="T13" s="127"/>
+      <c r="U13" s="127"/>
+      <c r="V13" s="127"/>
+      <c r="W13" s="127"/>
     </row>
     <row r="14" spans="1:23" ht="15.6">
       <c r="A14" s="1"/>
@@ -4089,26 +4121,26 @@
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="62" t="s">
+      <c r="C16" s="122" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63" t="s">
+      <c r="D16" s="123"/>
+      <c r="E16" s="123" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63" t="s">
+      <c r="F16" s="123"/>
+      <c r="G16" s="123" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63" t="s">
+      <c r="H16" s="123"/>
+      <c r="I16" s="123" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="63"/>
-      <c r="K16" s="63" t="s">
+      <c r="J16" s="123"/>
+      <c r="K16" s="123" t="s">
         <v>44</v>
       </c>
-      <c r="L16" s="63"/>
+      <c r="L16" s="123"/>
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
       <c r="O16" s="20"/>
@@ -4312,11 +4344,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
     <mergeCell ref="S8:W9"/>
     <mergeCell ref="S13:W13"/>
     <mergeCell ref="S10:W10"/>
@@ -4331,6 +4358,11 @@
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="G9:J9"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4348,14 +4380,14 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:38" ht="15" thickBot="1">
-      <c r="A1" s="64"/>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
+      <c r="A1" s="136"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
       <c r="I1" s="16"/>
       <c r="J1" s="17"/>
       <c r="K1" s="46"/>
@@ -4366,18 +4398,18 @@
       <c r="P1" s="19"/>
     </row>
     <row r="2" spans="1:38" ht="16.2" thickBot="1">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
+      <c r="A2" s="129"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
       <c r="M2" s="47"/>
       <c r="N2" s="48"/>
       <c r="O2" s="47"/>
@@ -4433,57 +4465,57 @@
       </c>
     </row>
     <row r="3" spans="1:38">
-      <c r="A3" s="55"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="57"/>
-      <c r="W3" s="76"/>
-      <c r="X3" s="77"/>
-      <c r="Y3" s="77"/>
-      <c r="Z3" s="77"/>
-      <c r="AA3" s="77"/>
-      <c r="AB3" s="77"/>
-      <c r="AC3" s="77"/>
-      <c r="AD3" s="77"/>
-      <c r="AE3" s="77"/>
-      <c r="AF3" s="77"/>
-      <c r="AG3" s="77"/>
-      <c r="AH3" s="77"/>
-      <c r="AI3" s="77"/>
-      <c r="AJ3" s="77"/>
-      <c r="AK3" s="77"/>
-      <c r="AL3" s="78"/>
+      <c r="A3" s="129"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="130"/>
+      <c r="M3" s="130"/>
+      <c r="N3" s="130"/>
+      <c r="O3" s="130"/>
+      <c r="P3" s="131"/>
+      <c r="W3" s="53"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
+      <c r="AB3" s="54"/>
+      <c r="AC3" s="54"/>
+      <c r="AD3" s="54"/>
+      <c r="AE3" s="54"/>
+      <c r="AF3" s="54"/>
+      <c r="AG3" s="54"/>
+      <c r="AH3" s="54"/>
+      <c r="AI3" s="54"/>
+      <c r="AJ3" s="54"/>
+      <c r="AK3" s="54"/>
+      <c r="AL3" s="55"/>
     </row>
     <row r="4" spans="1:38">
-      <c r="A4" s="58"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="61"/>
-      <c r="W4" s="79"/>
+      <c r="A4" s="132"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="133"/>
+      <c r="D4" s="133"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
+      <c r="H4" s="133"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="134"/>
+      <c r="L4" s="134"/>
+      <c r="M4" s="134"/>
+      <c r="N4" s="134"/>
+      <c r="O4" s="134"/>
+      <c r="P4" s="135"/>
+      <c r="W4" s="56"/>
       <c r="X4" s="24"/>
       <c r="Y4" s="24"/>
       <c r="Z4" s="24"/>
@@ -4491,33 +4523,33 @@
       <c r="AB4" s="24"/>
       <c r="AC4" s="24"/>
       <c r="AD4" s="24"/>
-      <c r="AE4" s="75"/>
-      <c r="AF4" s="75"/>
-      <c r="AG4" s="75"/>
-      <c r="AH4" s="75"/>
-      <c r="AI4" s="75"/>
-      <c r="AJ4" s="75"/>
-      <c r="AK4" s="75"/>
-      <c r="AL4" s="80"/>
+      <c r="AE4" s="52"/>
+      <c r="AF4" s="52"/>
+      <c r="AG4" s="52"/>
+      <c r="AH4" s="52"/>
+      <c r="AI4" s="52"/>
+      <c r="AJ4" s="52"/>
+      <c r="AK4" s="52"/>
+      <c r="AL4" s="57"/>
     </row>
     <row r="5" spans="1:38">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
-      <c r="P5" s="61"/>
-      <c r="W5" s="79"/>
+      <c r="A5" s="129"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="134"/>
+      <c r="L5" s="134"/>
+      <c r="M5" s="134"/>
+      <c r="N5" s="134"/>
+      <c r="O5" s="134"/>
+      <c r="P5" s="135"/>
+      <c r="W5" s="56"/>
       <c r="X5" s="24"/>
       <c r="Y5" s="24"/>
       <c r="Z5" s="24"/>
@@ -4532,7 +4564,7 @@
       <c r="AI5" s="24"/>
       <c r="AJ5" s="24"/>
       <c r="AK5" s="24"/>
-      <c r="AL5" s="81"/>
+      <c r="AL5" s="58"/>
     </row>
     <row r="6" spans="1:38">
       <c r="A6" s="33"/>
@@ -4551,7 +4583,7 @@
       <c r="N6" s="21"/>
       <c r="O6" s="21"/>
       <c r="P6" s="34"/>
-      <c r="W6" s="82"/>
+      <c r="W6" s="59"/>
       <c r="X6" s="27"/>
       <c r="Y6" s="27"/>
       <c r="Z6" s="27"/>
@@ -4566,7 +4598,7 @@
       <c r="AI6" s="44"/>
       <c r="AJ6" s="44"/>
       <c r="AK6" s="44"/>
-      <c r="AL6" s="83"/>
+      <c r="AL6" s="60"/>
     </row>
     <row r="7" spans="1:38">
       <c r="A7" s="31"/>
@@ -4585,7 +4617,7 @@
       <c r="N7" s="29"/>
       <c r="O7" s="29"/>
       <c r="P7" s="30"/>
-      <c r="W7" s="79"/>
+      <c r="W7" s="56"/>
       <c r="X7" s="24"/>
       <c r="Y7" s="24"/>
       <c r="Z7" s="24"/>
@@ -4600,7 +4632,7 @@
       <c r="AI7" s="44"/>
       <c r="AJ7" s="44"/>
       <c r="AK7" s="44"/>
-      <c r="AL7" s="83"/>
+      <c r="AL7" s="60"/>
     </row>
     <row r="8" spans="1:38">
       <c r="A8" s="35"/>
@@ -4619,7 +4651,7 @@
       <c r="N8" s="32"/>
       <c r="O8" s="20"/>
       <c r="P8" s="22"/>
-      <c r="W8" s="84"/>
+      <c r="W8" s="61"/>
       <c r="X8" s="20"/>
       <c r="Y8" s="20"/>
       <c r="Z8" s="20"/>
@@ -4634,26 +4666,26 @@
       <c r="AI8" s="20"/>
       <c r="AJ8" s="21"/>
       <c r="AK8" s="21"/>
-      <c r="AL8" s="85"/>
+      <c r="AL8" s="62"/>
     </row>
     <row r="9" spans="1:38">
-      <c r="A9" s="62"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
+      <c r="A9" s="122"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="123"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="123"/>
+      <c r="J9" s="123"/>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
       <c r="N9" s="20"/>
       <c r="O9" s="20"/>
       <c r="P9" s="22"/>
-      <c r="W9" s="86"/>
+      <c r="W9" s="63"/>
       <c r="X9" s="28"/>
       <c r="Y9" s="28"/>
       <c r="Z9" s="28"/>
@@ -4668,7 +4700,7 @@
       <c r="AI9" s="29"/>
       <c r="AJ9" s="29"/>
       <c r="AK9" s="29"/>
-      <c r="AL9" s="87"/>
+      <c r="AL9" s="64"/>
     </row>
     <row r="10" spans="1:38">
       <c r="A10" s="37"/>
@@ -4687,7 +4719,7 @@
       <c r="N10" s="20"/>
       <c r="O10" s="20"/>
       <c r="P10" s="22"/>
-      <c r="W10" s="88"/>
+      <c r="W10" s="65"/>
       <c r="X10" s="36"/>
       <c r="Y10" s="20"/>
       <c r="Z10" s="20"/>
@@ -4702,7 +4734,7 @@
       <c r="AI10" s="32"/>
       <c r="AJ10" s="32"/>
       <c r="AK10" s="20"/>
-      <c r="AL10" s="89"/>
+      <c r="AL10" s="66"/>
     </row>
     <row r="11" spans="1:38">
       <c r="A11" s="35"/>
@@ -4721,7 +4753,7 @@
       <c r="N11" s="32"/>
       <c r="O11" s="20"/>
       <c r="P11" s="22"/>
-      <c r="W11" s="84"/>
+      <c r="W11" s="61"/>
       <c r="X11" s="20"/>
       <c r="Y11" s="20"/>
       <c r="Z11" s="20"/>
@@ -4736,7 +4768,7 @@
       <c r="AI11" s="20"/>
       <c r="AJ11" s="20"/>
       <c r="AK11" s="20"/>
-      <c r="AL11" s="89"/>
+      <c r="AL11" s="66"/>
     </row>
     <row r="12" spans="1:38">
       <c r="A12" s="33"/>
@@ -4755,7 +4787,7 @@
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
       <c r="P12" s="22"/>
-      <c r="W12" s="90"/>
+      <c r="W12" s="67"/>
       <c r="X12" s="38"/>
       <c r="Y12" s="38"/>
       <c r="Z12" s="38"/>
@@ -4770,7 +4802,7 @@
       <c r="AI12" s="20"/>
       <c r="AJ12" s="20"/>
       <c r="AK12" s="20"/>
-      <c r="AL12" s="89"/>
+      <c r="AL12" s="66"/>
     </row>
     <row r="13" spans="1:38">
       <c r="A13" s="37"/>
@@ -4789,7 +4821,7 @@
       <c r="N13" s="20"/>
       <c r="O13" s="20"/>
       <c r="P13" s="22"/>
-      <c r="W13" s="88"/>
+      <c r="W13" s="65"/>
       <c r="X13" s="36"/>
       <c r="Y13" s="20"/>
       <c r="Z13" s="20"/>
@@ -4804,7 +4836,7 @@
       <c r="AI13" s="32"/>
       <c r="AJ13" s="32"/>
       <c r="AK13" s="20"/>
-      <c r="AL13" s="89"/>
+      <c r="AL13" s="66"/>
     </row>
     <row r="14" spans="1:38">
       <c r="A14" s="35"/>
@@ -4823,7 +4855,7 @@
       <c r="N14" s="32"/>
       <c r="O14" s="20"/>
       <c r="P14" s="22"/>
-      <c r="W14" s="84"/>
+      <c r="W14" s="61"/>
       <c r="X14" s="20"/>
       <c r="Y14" s="20"/>
       <c r="Z14" s="20"/>
@@ -4838,7 +4870,7 @@
       <c r="AI14" s="20"/>
       <c r="AJ14" s="20"/>
       <c r="AK14" s="20"/>
-      <c r="AL14" s="89"/>
+      <c r="AL14" s="66"/>
     </row>
     <row r="15" spans="1:38">
       <c r="A15" s="33"/>
@@ -4857,7 +4889,7 @@
       <c r="N15" s="20"/>
       <c r="O15" s="20"/>
       <c r="P15" s="22"/>
-      <c r="W15" s="90"/>
+      <c r="W15" s="67"/>
       <c r="X15" s="38"/>
       <c r="Y15" s="38"/>
       <c r="Z15" s="38"/>
@@ -4872,7 +4904,7 @@
       <c r="AI15" s="20"/>
       <c r="AJ15" s="20"/>
       <c r="AK15" s="20"/>
-      <c r="AL15" s="89"/>
+      <c r="AL15" s="66"/>
     </row>
     <row r="16" spans="1:38" ht="15" thickBot="1">
       <c r="A16" s="40"/>
@@ -4891,7 +4923,7 @@
       <c r="N16" s="42"/>
       <c r="O16" s="42"/>
       <c r="P16" s="43"/>
-      <c r="W16" s="88"/>
+      <c r="W16" s="65"/>
       <c r="X16" s="36"/>
       <c r="Y16" s="20"/>
       <c r="Z16" s="20"/>
@@ -4906,26 +4938,26 @@
       <c r="AI16" s="32"/>
       <c r="AJ16" s="32"/>
       <c r="AK16" s="20"/>
-      <c r="AL16" s="89"/>
+      <c r="AL16" s="66"/>
     </row>
     <row r="17" spans="1:38">
-      <c r="A17" s="64"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="69"/>
-      <c r="N17" s="69"/>
-      <c r="O17" s="69"/>
-      <c r="P17" s="70"/>
-      <c r="W17" s="84"/>
+      <c r="A17" s="136"/>
+      <c r="B17" s="137"/>
+      <c r="C17" s="137"/>
+      <c r="D17" s="137"/>
+      <c r="E17" s="137"/>
+      <c r="F17" s="137"/>
+      <c r="G17" s="137"/>
+      <c r="H17" s="137"/>
+      <c r="I17" s="137"/>
+      <c r="J17" s="137"/>
+      <c r="K17" s="137"/>
+      <c r="L17" s="137"/>
+      <c r="M17" s="143"/>
+      <c r="N17" s="143"/>
+      <c r="O17" s="143"/>
+      <c r="P17" s="144"/>
+      <c r="W17" s="61"/>
       <c r="X17" s="20"/>
       <c r="Y17" s="20"/>
       <c r="Z17" s="20"/>
@@ -4940,69 +4972,69 @@
       <c r="AI17" s="20"/>
       <c r="AJ17" s="20"/>
       <c r="AK17" s="20"/>
-      <c r="AL17" s="89"/>
+      <c r="AL17" s="66"/>
     </row>
     <row r="18" spans="1:38">
-      <c r="A18" s="55"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
+      <c r="A18" s="129"/>
+      <c r="B18" s="130"/>
+      <c r="C18" s="130"/>
+      <c r="D18" s="130"/>
+      <c r="E18" s="134"/>
+      <c r="F18" s="134"/>
+      <c r="G18" s="134"/>
+      <c r="H18" s="134"/>
+      <c r="I18" s="128"/>
+      <c r="J18" s="128"/>
+      <c r="K18" s="128"/>
+      <c r="L18" s="128"/>
       <c r="M18" s="20"/>
       <c r="N18" s="21"/>
       <c r="O18" s="20"/>
       <c r="P18" s="22"/>
-      <c r="W18" s="91"/>
-      <c r="X18" s="73"/>
-      <c r="Y18" s="73"/>
-      <c r="Z18" s="73"/>
-      <c r="AA18" s="73"/>
-      <c r="AB18" s="73"/>
-      <c r="AC18" s="73"/>
-      <c r="AD18" s="73"/>
-      <c r="AE18" s="73"/>
-      <c r="AF18" s="73"/>
-      <c r="AG18" s="74"/>
-      <c r="AH18" s="74"/>
-      <c r="AI18" s="74"/>
-      <c r="AJ18" s="74"/>
-      <c r="AK18" s="74"/>
-      <c r="AL18" s="92"/>
+      <c r="W18" s="68"/>
+      <c r="X18" s="50"/>
+      <c r="Y18" s="50"/>
+      <c r="Z18" s="50"/>
+      <c r="AA18" s="50"/>
+      <c r="AB18" s="50"/>
+      <c r="AC18" s="50"/>
+      <c r="AD18" s="50"/>
+      <c r="AE18" s="50"/>
+      <c r="AF18" s="50"/>
+      <c r="AG18" s="51"/>
+      <c r="AH18" s="51"/>
+      <c r="AI18" s="51"/>
+      <c r="AJ18" s="51"/>
+      <c r="AK18" s="51"/>
+      <c r="AL18" s="69"/>
     </row>
     <row r="19" spans="1:38" ht="15" thickBot="1">
-      <c r="A19" s="55"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
+      <c r="A19" s="129"/>
+      <c r="B19" s="130"/>
+      <c r="C19" s="130"/>
+      <c r="D19" s="130"/>
+      <c r="E19" s="130"/>
+      <c r="F19" s="130"/>
+      <c r="G19" s="130"/>
+      <c r="H19" s="130"/>
+      <c r="I19" s="130"/>
+      <c r="J19" s="130"/>
+      <c r="K19" s="130"/>
+      <c r="L19" s="130"/>
       <c r="M19" s="24"/>
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
       <c r="P19" s="25"/>
     </row>
     <row r="20" spans="1:38" ht="16.2" thickBot="1">
-      <c r="A20" s="58"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="59"/>
+      <c r="A20" s="132"/>
+      <c r="B20" s="133"/>
+      <c r="C20" s="133"/>
+      <c r="D20" s="133"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="133"/>
+      <c r="G20" s="133"/>
+      <c r="H20" s="133"/>
       <c r="I20" s="44"/>
       <c r="J20" s="44"/>
       <c r="K20" s="44"/>
@@ -5011,53 +5043,53 @@
       <c r="N20" s="44"/>
       <c r="O20" s="44"/>
       <c r="P20" s="45"/>
-      <c r="V20" s="137"/>
-      <c r="W20" s="95">
+      <c r="V20" s="80"/>
+      <c r="W20" s="72">
         <v>0</v>
       </c>
-      <c r="X20" s="96">
+      <c r="X20" s="73">
         <v>1</v>
       </c>
-      <c r="Y20" s="97">
+      <c r="Y20" s="74">
         <v>2</v>
       </c>
-      <c r="Z20" s="97">
+      <c r="Z20" s="74">
         <v>3</v>
       </c>
-      <c r="AA20" s="97">
+      <c r="AA20" s="74">
         <v>4</v>
       </c>
-      <c r="AB20" s="97">
+      <c r="AB20" s="74">
         <v>5</v>
       </c>
-      <c r="AC20" s="97">
-        <v>6</v>
-      </c>
-      <c r="AD20" s="97">
+      <c r="AC20" s="74">
+        <v>6</v>
+      </c>
+      <c r="AD20" s="74">
         <v>7</v>
       </c>
-      <c r="AE20" s="97">
+      <c r="AE20" s="74">
         <v>8</v>
       </c>
-      <c r="AF20" s="97">
+      <c r="AF20" s="74">
         <v>9</v>
       </c>
-      <c r="AG20" s="97" t="s">
+      <c r="AG20" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="AH20" s="97" t="s">
+      <c r="AH20" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="AI20" s="97" t="s">
+      <c r="AI20" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="AJ20" s="97" t="s">
+      <c r="AJ20" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="AK20" s="97" t="s">
+      <c r="AK20" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="AL20" s="98" t="s">
+      <c r="AL20" s="75" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5081,28 +5113,28 @@
       <c r="V21" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="W21" s="115" t="s">
+      <c r="W21" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="X21" s="116"/>
-      <c r="Y21" s="116"/>
-      <c r="Z21" s="117"/>
+      <c r="X21" s="112"/>
+      <c r="Y21" s="112"/>
+      <c r="Z21" s="113"/>
       <c r="AA21" s="24"/>
       <c r="AB21" s="24"/>
       <c r="AC21" s="24"/>
       <c r="AD21" s="24"/>
-      <c r="AE21" s="118" t="s">
+      <c r="AE21" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="AF21" s="118"/>
-      <c r="AG21" s="118"/>
-      <c r="AH21" s="118"/>
-      <c r="AI21" s="118" t="s">
+      <c r="AF21" s="114"/>
+      <c r="AG21" s="114"/>
+      <c r="AH21" s="114"/>
+      <c r="AI21" s="114" t="s">
         <v>48</v>
       </c>
-      <c r="AJ21" s="118"/>
-      <c r="AK21" s="118"/>
-      <c r="AL21" s="119"/>
+      <c r="AJ21" s="114"/>
+      <c r="AK21" s="114"/>
+      <c r="AL21" s="115"/>
     </row>
     <row r="22" spans="1:38" ht="15.6">
       <c r="A22" s="33"/>
@@ -5132,18 +5164,18 @@
       <c r="AB22" s="24"/>
       <c r="AC22" s="24"/>
       <c r="AD22" s="24"/>
-      <c r="AE22" s="120" t="s">
+      <c r="AE22" s="96" t="s">
         <v>46</v>
       </c>
-      <c r="AF22" s="120"/>
-      <c r="AG22" s="120"/>
-      <c r="AH22" s="120"/>
-      <c r="AI22" s="121" t="s">
+      <c r="AF22" s="96"/>
+      <c r="AG22" s="96"/>
+      <c r="AH22" s="96"/>
+      <c r="AI22" s="116" t="s">
         <v>47</v>
       </c>
-      <c r="AJ22" s="121"/>
-      <c r="AK22" s="121"/>
-      <c r="AL22" s="122"/>
+      <c r="AJ22" s="116"/>
+      <c r="AK22" s="116"/>
+      <c r="AL22" s="117"/>
     </row>
     <row r="23" spans="1:38" ht="15.6">
       <c r="A23" s="31"/>
@@ -5165,28 +5197,28 @@
       <c r="V23" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="W23" s="113" t="s">
+      <c r="W23" s="118" t="s">
         <v>51</v>
       </c>
-      <c r="X23" s="114"/>
-      <c r="Y23" s="114"/>
-      <c r="Z23" s="114"/>
+      <c r="X23" s="119"/>
+      <c r="Y23" s="119"/>
+      <c r="Z23" s="119"/>
       <c r="AA23" s="24"/>
       <c r="AB23" s="24"/>
       <c r="AC23" s="24"/>
       <c r="AD23" s="24"/>
-      <c r="AE23" s="120" t="s">
+      <c r="AE23" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="AF23" s="120"/>
-      <c r="AG23" s="120"/>
-      <c r="AH23" s="120"/>
-      <c r="AI23" s="120" t="s">
+      <c r="AF23" s="96"/>
+      <c r="AG23" s="96"/>
+      <c r="AH23" s="96"/>
+      <c r="AI23" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="AJ23" s="120"/>
-      <c r="AK23" s="120"/>
-      <c r="AL23" s="123"/>
+      <c r="AJ23" s="96"/>
+      <c r="AK23" s="96"/>
+      <c r="AL23" s="97"/>
     </row>
     <row r="24" spans="1:38" ht="15.6">
       <c r="A24" s="35"/>
@@ -5208,32 +5240,32 @@
       <c r="V24" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="W24" s="94"/>
-      <c r="X24" s="93"/>
-      <c r="Y24" s="93"/>
-      <c r="Z24" s="93"/>
+      <c r="W24" s="71"/>
+      <c r="X24" s="70"/>
+      <c r="Y24" s="70"/>
+      <c r="Z24" s="70"/>
       <c r="AA24" s="27"/>
       <c r="AB24" s="27"/>
       <c r="AC24" s="27"/>
       <c r="AD24" s="27"/>
-      <c r="AE24" s="124" t="s">
+      <c r="AE24" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="AF24" s="124"/>
-      <c r="AG24" s="124"/>
-      <c r="AH24" s="124"/>
-      <c r="AI24" s="125" t="s">
+      <c r="AF24" s="94"/>
+      <c r="AG24" s="94"/>
+      <c r="AH24" s="94"/>
+      <c r="AI24" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="AJ24" s="125"/>
-      <c r="AK24" s="125"/>
-      <c r="AL24" s="126"/>
+      <c r="AJ24" s="106"/>
+      <c r="AK24" s="106"/>
+      <c r="AL24" s="107"/>
     </row>
     <row r="25" spans="1:38" ht="15.6">
-      <c r="A25" s="62"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="63"/>
+      <c r="A25" s="122"/>
+      <c r="B25" s="123"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="123"/>
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
       <c r="G25" s="47"/>
@@ -5249,30 +5281,30 @@
       <c r="V25" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="W25" s="109" t="s">
+      <c r="W25" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="X25" s="110"/>
-      <c r="Y25" s="110"/>
-      <c r="Z25" s="110"/>
-      <c r="AA25" s="110" t="s">
+      <c r="X25" s="109"/>
+      <c r="Y25" s="109"/>
+      <c r="Z25" s="109"/>
+      <c r="AA25" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="AB25" s="110"/>
-      <c r="AC25" s="110"/>
-      <c r="AD25" s="110"/>
-      <c r="AE25" s="127" t="s">
+      <c r="AB25" s="109"/>
+      <c r="AC25" s="109"/>
+      <c r="AD25" s="109"/>
+      <c r="AE25" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="AF25" s="127"/>
-      <c r="AG25" s="127"/>
-      <c r="AH25" s="127"/>
-      <c r="AI25" s="120" t="s">
+      <c r="AF25" s="110"/>
+      <c r="AG25" s="110"/>
+      <c r="AH25" s="110"/>
+      <c r="AI25" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="AJ25" s="120"/>
-      <c r="AK25" s="120"/>
-      <c r="AL25" s="123"/>
+      <c r="AJ25" s="96"/>
+      <c r="AK25" s="96"/>
+      <c r="AL25" s="97"/>
     </row>
     <row r="26" spans="1:38" ht="15.6">
       <c r="A26" s="37"/>
@@ -5294,18 +5326,18 @@
       <c r="V26" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="W26" s="111" t="s">
+      <c r="W26" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="X26" s="112"/>
-      <c r="Y26" s="112"/>
-      <c r="Z26" s="112"/>
-      <c r="AA26" s="93"/>
-      <c r="AB26" s="93"/>
-      <c r="AC26" s="93"/>
-      <c r="AD26" s="93"/>
-      <c r="AE26" s="93"/>
-      <c r="AF26" s="93"/>
+      <c r="X26" s="102"/>
+      <c r="Y26" s="102"/>
+      <c r="Z26" s="102"/>
+      <c r="AA26" s="70"/>
+      <c r="AB26" s="70"/>
+      <c r="AC26" s="70"/>
+      <c r="AD26" s="70"/>
+      <c r="AE26" s="70"/>
+      <c r="AF26" s="70"/>
       <c r="AG26" s="29"/>
       <c r="AH26" s="29"/>
       <c r="AI26" s="20"/>
@@ -5333,10 +5365,10 @@
       <c r="V27" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="W27" s="108" t="s">
+      <c r="W27" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="X27" s="107" t="s">
+      <c r="X27" s="76" t="s">
         <v>57</v>
       </c>
       <c r="Y27" s="20"/>
@@ -5345,10 +5377,10 @@
       <c r="AB27" s="20"/>
       <c r="AC27" s="20"/>
       <c r="AD27" s="20"/>
-      <c r="AE27" s="128" t="s">
+      <c r="AE27" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="AF27" s="129" t="s">
+      <c r="AF27" s="79" t="s">
         <v>58</v>
       </c>
       <c r="AG27" s="29"/>
@@ -5396,55 +5428,55 @@
       <c r="AL28" s="22"/>
     </row>
     <row r="29" spans="1:38" ht="15.6">
-      <c r="A29" s="68" t="s">
+      <c r="A29" s="140" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="66"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66" t="s">
+      <c r="B29" s="141"/>
+      <c r="C29" s="141"/>
+      <c r="D29" s="141"/>
+      <c r="E29" s="141" t="s">
         <v>60</v>
       </c>
-      <c r="F29" s="66"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="66" t="s">
+      <c r="F29" s="141"/>
+      <c r="G29" s="141"/>
+      <c r="H29" s="141"/>
+      <c r="I29" s="141" t="s">
         <v>61</v>
       </c>
-      <c r="J29" s="66"/>
-      <c r="K29" s="66"/>
-      <c r="L29" s="66"/>
-      <c r="M29" s="63" t="s">
+      <c r="J29" s="141"/>
+      <c r="K29" s="141"/>
+      <c r="L29" s="141"/>
+      <c r="M29" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="N29" s="63"/>
-      <c r="O29" s="63"/>
-      <c r="P29" s="67"/>
+      <c r="N29" s="123"/>
+      <c r="O29" s="123"/>
+      <c r="P29" s="142"/>
       <c r="V29" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="W29" s="102" t="s">
+      <c r="W29" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="X29" s="103"/>
-      <c r="Y29" s="103"/>
-      <c r="Z29" s="103"/>
-      <c r="AA29" s="103" t="s">
+      <c r="X29" s="104"/>
+      <c r="Y29" s="104"/>
+      <c r="Z29" s="104"/>
+      <c r="AA29" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="AB29" s="103"/>
-      <c r="AC29" s="103"/>
-      <c r="AD29" s="104"/>
-      <c r="AE29" s="120" t="s">
+      <c r="AB29" s="104"/>
+      <c r="AC29" s="104"/>
+      <c r="AD29" s="105"/>
+      <c r="AE29" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="AF29" s="120"/>
-      <c r="AG29" s="120"/>
-      <c r="AH29" s="120"/>
-      <c r="AI29" s="120"/>
-      <c r="AJ29" s="120"/>
-      <c r="AK29" s="120"/>
-      <c r="AL29" s="123"/>
+      <c r="AF29" s="96"/>
+      <c r="AG29" s="96"/>
+      <c r="AH29" s="96"/>
+      <c r="AI29" s="96"/>
+      <c r="AJ29" s="96"/>
+      <c r="AK29" s="96"/>
+      <c r="AL29" s="97"/>
     </row>
     <row r="30" spans="1:38" ht="15.6">
       <c r="A30" s="35"/>
@@ -5466,28 +5498,28 @@
       <c r="V30" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="W30" s="102" t="s">
+      <c r="W30" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="X30" s="103"/>
-      <c r="Y30" s="103"/>
-      <c r="Z30" s="103"/>
-      <c r="AA30" s="105" t="s">
+      <c r="X30" s="104"/>
+      <c r="Y30" s="104"/>
+      <c r="Z30" s="104"/>
+      <c r="AA30" s="138" t="s">
         <v>62</v>
       </c>
-      <c r="AB30" s="105"/>
-      <c r="AC30" s="105"/>
-      <c r="AD30" s="106"/>
-      <c r="AE30" s="120" t="s">
+      <c r="AB30" s="138"/>
+      <c r="AC30" s="138"/>
+      <c r="AD30" s="139"/>
+      <c r="AE30" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="AF30" s="120"/>
-      <c r="AG30" s="120"/>
-      <c r="AH30" s="120"/>
-      <c r="AI30" s="120"/>
-      <c r="AJ30" s="120"/>
-      <c r="AK30" s="120"/>
-      <c r="AL30" s="123"/>
+      <c r="AF30" s="96"/>
+      <c r="AG30" s="96"/>
+      <c r="AH30" s="96"/>
+      <c r="AI30" s="96"/>
+      <c r="AJ30" s="96"/>
+      <c r="AK30" s="96"/>
+      <c r="AL30" s="97"/>
     </row>
     <row r="31" spans="1:38" ht="15.6">
       <c r="A31" s="33"/>
@@ -5517,16 +5549,16 @@
       <c r="AB31" s="20"/>
       <c r="AC31" s="20"/>
       <c r="AD31" s="20"/>
-      <c r="AE31" s="130" t="s">
+      <c r="AE31" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="AF31" s="130"/>
-      <c r="AG31" s="130"/>
-      <c r="AH31" s="130"/>
-      <c r="AI31" s="130"/>
-      <c r="AJ31" s="130"/>
-      <c r="AK31" s="130"/>
-      <c r="AL31" s="131"/>
+      <c r="AF31" s="92"/>
+      <c r="AG31" s="92"/>
+      <c r="AH31" s="92"/>
+      <c r="AI31" s="92"/>
+      <c r="AJ31" s="92"/>
+      <c r="AK31" s="92"/>
+      <c r="AL31" s="93"/>
     </row>
     <row r="32" spans="1:38" ht="15.6">
       <c r="A32" s="35"/>
@@ -5556,34 +5588,34 @@
       <c r="AB32" s="20"/>
       <c r="AC32" s="20"/>
       <c r="AD32" s="20"/>
-      <c r="AE32" s="124" t="s">
+      <c r="AE32" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="AF32" s="124"/>
-      <c r="AG32" s="124"/>
-      <c r="AH32" s="124"/>
-      <c r="AI32" s="124"/>
-      <c r="AJ32" s="124"/>
-      <c r="AK32" s="124"/>
-      <c r="AL32" s="132"/>
+      <c r="AF32" s="94"/>
+      <c r="AG32" s="94"/>
+      <c r="AH32" s="94"/>
+      <c r="AI32" s="94"/>
+      <c r="AJ32" s="94"/>
+      <c r="AK32" s="94"/>
+      <c r="AL32" s="95"/>
     </row>
     <row r="33" spans="1:38" ht="15.6">
-      <c r="A33" s="76"/>
-      <c r="B33" s="77"/>
-      <c r="C33" s="77"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="77"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="77"/>
-      <c r="J33" s="77"/>
-      <c r="K33" s="77"/>
-      <c r="L33" s="77"/>
-      <c r="M33" s="77"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="77"/>
-      <c r="P33" s="78"/>
+      <c r="A33" s="53"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="54"/>
+      <c r="L33" s="54"/>
+      <c r="M33" s="54"/>
+      <c r="N33" s="54"/>
+      <c r="O33" s="54"/>
+      <c r="P33" s="55"/>
       <c r="V33" s="6" t="s">
         <v>21</v>
       </c>
@@ -5595,19 +5627,19 @@
       <c r="AB33" s="38"/>
       <c r="AC33" s="38"/>
       <c r="AD33" s="38"/>
-      <c r="AE33" s="120" t="s">
+      <c r="AE33" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="AF33" s="120"/>
-      <c r="AG33" s="120"/>
-      <c r="AH33" s="120"/>
-      <c r="AI33" s="120"/>
-      <c r="AJ33" s="120"/>
-      <c r="AK33" s="120"/>
-      <c r="AL33" s="123"/>
+      <c r="AF33" s="96"/>
+      <c r="AG33" s="96"/>
+      <c r="AH33" s="96"/>
+      <c r="AI33" s="96"/>
+      <c r="AJ33" s="96"/>
+      <c r="AK33" s="96"/>
+      <c r="AL33" s="97"/>
     </row>
     <row r="34" spans="1:38" ht="15.6">
-      <c r="A34" s="79"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="24"/>
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
@@ -5615,14 +5647,14 @@
       <c r="F34" s="24"/>
       <c r="G34" s="24"/>
       <c r="H34" s="24"/>
-      <c r="I34" s="75"/>
-      <c r="J34" s="75"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="75"/>
-      <c r="M34" s="75"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="75"/>
-      <c r="P34" s="80"/>
+      <c r="I34" s="52"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="52"/>
+      <c r="L34" s="52"/>
+      <c r="M34" s="52"/>
+      <c r="N34" s="52"/>
+      <c r="O34" s="52"/>
+      <c r="P34" s="57"/>
       <c r="V34" s="6" t="s">
         <v>22</v>
       </c>
@@ -5634,19 +5666,19 @@
       <c r="AB34" s="20"/>
       <c r="AC34" s="20"/>
       <c r="AD34" s="20"/>
-      <c r="AE34" s="124" t="s">
+      <c r="AE34" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="AF34" s="124"/>
-      <c r="AG34" s="124"/>
-      <c r="AH34" s="124"/>
-      <c r="AI34" s="124"/>
-      <c r="AJ34" s="124"/>
-      <c r="AK34" s="124"/>
-      <c r="AL34" s="132"/>
+      <c r="AF34" s="94"/>
+      <c r="AG34" s="94"/>
+      <c r="AH34" s="94"/>
+      <c r="AI34" s="94"/>
+      <c r="AJ34" s="94"/>
+      <c r="AK34" s="94"/>
+      <c r="AL34" s="95"/>
     </row>
     <row r="35" spans="1:38" ht="15.6">
-      <c r="A35" s="79"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="24"/>
       <c r="C35" s="24"/>
       <c r="D35" s="24"/>
@@ -5661,7 +5693,7 @@
       <c r="M35" s="24"/>
       <c r="N35" s="24"/>
       <c r="O35" s="24"/>
-      <c r="P35" s="81"/>
+      <c r="P35" s="58"/>
       <c r="V35" s="6" t="s">
         <v>23</v>
       </c>
@@ -5679,13 +5711,13 @@
       <c r="AH35" s="20"/>
       <c r="AI35" s="20"/>
       <c r="AJ35" s="20"/>
-      <c r="AK35" s="133" t="s">
+      <c r="AK35" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="AL35" s="134"/>
+      <c r="AL35" s="88"/>
     </row>
     <row r="36" spans="1:38" ht="16.2" thickBot="1">
-      <c r="A36" s="82"/>
+      <c r="A36" s="59"/>
       <c r="B36" s="27"/>
       <c r="C36" s="27"/>
       <c r="D36" s="27"/>
@@ -5700,39 +5732,39 @@
       <c r="M36" s="44"/>
       <c r="N36" s="44"/>
       <c r="O36" s="44"/>
-      <c r="P36" s="83"/>
+      <c r="P36" s="60"/>
       <c r="V36" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="W36" s="99" t="s">
+      <c r="W36" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="X36" s="100"/>
-      <c r="Y36" s="100"/>
-      <c r="Z36" s="100"/>
-      <c r="AA36" s="100"/>
-      <c r="AB36" s="100"/>
-      <c r="AC36" s="100"/>
-      <c r="AD36" s="101"/>
-      <c r="AE36" s="135" t="s">
+      <c r="X36" s="99"/>
+      <c r="Y36" s="99"/>
+      <c r="Z36" s="99"/>
+      <c r="AA36" s="99"/>
+      <c r="AB36" s="99"/>
+      <c r="AC36" s="99"/>
+      <c r="AD36" s="100"/>
+      <c r="AE36" s="120" t="s">
         <v>40</v>
       </c>
-      <c r="AF36" s="135"/>
-      <c r="AG36" s="135" t="s">
+      <c r="AF36" s="120"/>
+      <c r="AG36" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="AH36" s="135"/>
-      <c r="AI36" s="135" t="s">
+      <c r="AH36" s="120"/>
+      <c r="AI36" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AJ36" s="135"/>
-      <c r="AK36" s="135" t="s">
+      <c r="AJ36" s="120"/>
+      <c r="AK36" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="AL36" s="136"/>
+      <c r="AL36" s="121"/>
     </row>
     <row r="37" spans="1:38">
-      <c r="A37" s="79"/>
+      <c r="A37" s="56"/>
       <c r="B37" s="24"/>
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
@@ -5747,10 +5779,10 @@
       <c r="M37" s="44"/>
       <c r="N37" s="44"/>
       <c r="O37" s="44"/>
-      <c r="P37" s="83"/>
+      <c r="P37" s="60"/>
     </row>
     <row r="38" spans="1:38">
-      <c r="A38" s="84"/>
+      <c r="A38" s="61"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
@@ -5765,10 +5797,10 @@
       <c r="M38" s="20"/>
       <c r="N38" s="21"/>
       <c r="O38" s="21"/>
-      <c r="P38" s="85"/>
+      <c r="P38" s="62"/>
     </row>
     <row r="39" spans="1:38">
-      <c r="A39" s="86"/>
+      <c r="A39" s="63"/>
       <c r="B39" s="28"/>
       <c r="C39" s="28"/>
       <c r="D39" s="28"/>
@@ -5783,10 +5815,10 @@
       <c r="M39" s="29"/>
       <c r="N39" s="29"/>
       <c r="O39" s="29"/>
-      <c r="P39" s="87"/>
+      <c r="P39" s="64"/>
     </row>
     <row r="40" spans="1:38">
-      <c r="A40" s="88"/>
+      <c r="A40" s="65"/>
       <c r="B40" s="36"/>
       <c r="C40" s="20"/>
       <c r="D40" s="20"/>
@@ -5801,10 +5833,10 @@
       <c r="M40" s="32"/>
       <c r="N40" s="32"/>
       <c r="O40" s="20"/>
-      <c r="P40" s="89"/>
+      <c r="P40" s="66"/>
     </row>
     <row r="41" spans="1:38">
-      <c r="A41" s="84"/>
+      <c r="A41" s="61"/>
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
       <c r="D41" s="20"/>
@@ -5819,10 +5851,10 @@
       <c r="M41" s="20"/>
       <c r="N41" s="20"/>
       <c r="O41" s="20"/>
-      <c r="P41" s="89"/>
+      <c r="P41" s="66"/>
     </row>
     <row r="42" spans="1:38">
-      <c r="A42" s="90"/>
+      <c r="A42" s="67"/>
       <c r="B42" s="38"/>
       <c r="C42" s="38"/>
       <c r="D42" s="38"/>
@@ -5837,10 +5869,10 @@
       <c r="M42" s="20"/>
       <c r="N42" s="20"/>
       <c r="O42" s="20"/>
-      <c r="P42" s="89"/>
+      <c r="P42" s="66"/>
     </row>
     <row r="43" spans="1:38">
-      <c r="A43" s="88"/>
+      <c r="A43" s="65"/>
       <c r="B43" s="36"/>
       <c r="C43" s="20"/>
       <c r="D43" s="20"/>
@@ -5855,10 +5887,10 @@
       <c r="M43" s="32"/>
       <c r="N43" s="32"/>
       <c r="O43" s="20"/>
-      <c r="P43" s="89"/>
+      <c r="P43" s="66"/>
     </row>
     <row r="44" spans="1:38">
-      <c r="A44" s="84"/>
+      <c r="A44" s="61"/>
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
       <c r="D44" s="20"/>
@@ -5873,10 +5905,10 @@
       <c r="M44" s="20"/>
       <c r="N44" s="20"/>
       <c r="O44" s="20"/>
-      <c r="P44" s="89"/>
+      <c r="P44" s="66"/>
     </row>
     <row r="45" spans="1:38">
-      <c r="A45" s="90"/>
+      <c r="A45" s="67"/>
       <c r="B45" s="38"/>
       <c r="C45" s="38"/>
       <c r="D45" s="38"/>
@@ -5891,10 +5923,10 @@
       <c r="M45" s="20"/>
       <c r="N45" s="20"/>
       <c r="O45" s="20"/>
-      <c r="P45" s="89"/>
+      <c r="P45" s="66"/>
     </row>
     <row r="46" spans="1:38">
-      <c r="A46" s="88"/>
+      <c r="A46" s="65"/>
       <c r="B46" s="36"/>
       <c r="C46" s="20"/>
       <c r="D46" s="20"/>
@@ -5909,10 +5941,10 @@
       <c r="M46" s="32"/>
       <c r="N46" s="32"/>
       <c r="O46" s="20"/>
-      <c r="P46" s="89"/>
+      <c r="P46" s="66"/>
     </row>
     <row r="47" spans="1:38">
-      <c r="A47" s="84"/>
+      <c r="A47" s="61"/>
       <c r="B47" s="20"/>
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
@@ -5927,28 +5959,77 @@
       <c r="M47" s="20"/>
       <c r="N47" s="20"/>
       <c r="O47" s="20"/>
-      <c r="P47" s="89"/>
+      <c r="P47" s="66"/>
     </row>
     <row r="48" spans="1:38">
-      <c r="A48" s="91"/>
-      <c r="B48" s="73"/>
-      <c r="C48" s="73"/>
-      <c r="D48" s="73"/>
-      <c r="E48" s="73"/>
-      <c r="F48" s="73"/>
-      <c r="G48" s="73"/>
-      <c r="H48" s="73"/>
-      <c r="I48" s="73"/>
-      <c r="J48" s="73"/>
-      <c r="K48" s="74"/>
-      <c r="L48" s="74"/>
-      <c r="M48" s="74"/>
-      <c r="N48" s="74"/>
-      <c r="O48" s="74"/>
-      <c r="P48" s="92"/>
+      <c r="A48" s="68"/>
+      <c r="B48" s="50"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="50"/>
+      <c r="H48" s="50"/>
+      <c r="I48" s="50"/>
+      <c r="J48" s="50"/>
+      <c r="K48" s="51"/>
+      <c r="L48" s="51"/>
+      <c r="M48" s="51"/>
+      <c r="N48" s="51"/>
+      <c r="O48" s="51"/>
+      <c r="P48" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:P3"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="I4:P4"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="I5:P5"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="W26:Z26"/>
+    <mergeCell ref="W29:Z29"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="M29:P29"/>
+    <mergeCell ref="AI24:AL24"/>
+    <mergeCell ref="AI21:AL21"/>
+    <mergeCell ref="W25:Z25"/>
+    <mergeCell ref="AA25:AD25"/>
+    <mergeCell ref="AE25:AH25"/>
+    <mergeCell ref="AI25:AL25"/>
+    <mergeCell ref="AE21:AH21"/>
+    <mergeCell ref="AE22:AH22"/>
+    <mergeCell ref="AI22:AL22"/>
+    <mergeCell ref="AE23:AH23"/>
+    <mergeCell ref="AI23:AL23"/>
+    <mergeCell ref="AE24:AH24"/>
+    <mergeCell ref="W21:Z21"/>
+    <mergeCell ref="W23:Z23"/>
     <mergeCell ref="AA29:AD29"/>
     <mergeCell ref="W30:Z30"/>
     <mergeCell ref="AA30:AD30"/>
@@ -5960,59 +6041,10 @@
     <mergeCell ref="AE32:AL32"/>
     <mergeCell ref="AE33:AL33"/>
     <mergeCell ref="AE34:AL34"/>
-    <mergeCell ref="AI24:AL24"/>
-    <mergeCell ref="AI21:AL21"/>
-    <mergeCell ref="W25:Z25"/>
-    <mergeCell ref="AA25:AD25"/>
-    <mergeCell ref="AE25:AH25"/>
-    <mergeCell ref="AI25:AL25"/>
     <mergeCell ref="AE36:AF36"/>
     <mergeCell ref="AG36:AH36"/>
     <mergeCell ref="AI36:AJ36"/>
     <mergeCell ref="AK36:AL36"/>
-    <mergeCell ref="AE21:AH21"/>
-    <mergeCell ref="AE22:AH22"/>
-    <mergeCell ref="AI22:AL22"/>
-    <mergeCell ref="AE23:AH23"/>
-    <mergeCell ref="AI23:AL23"/>
-    <mergeCell ref="AE24:AH24"/>
-    <mergeCell ref="W21:Z21"/>
-    <mergeCell ref="W23:Z23"/>
-    <mergeCell ref="W26:Z26"/>
-    <mergeCell ref="W29:Z29"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="I29:L29"/>
-    <mergeCell ref="M29:P29"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="I4:P4"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="I5:P5"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6095,122 +6127,122 @@
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="136" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65" t="s">
+      <c r="D8" s="137"/>
+      <c r="E8" s="137"/>
+      <c r="F8" s="137"/>
+      <c r="G8" s="137" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65" t="s">
+      <c r="H8" s="137"/>
+      <c r="I8" s="137"/>
+      <c r="J8" s="137"/>
+      <c r="K8" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="65"/>
-      <c r="O8" s="69" t="s">
+      <c r="L8" s="137"/>
+      <c r="M8" s="137"/>
+      <c r="N8" s="137"/>
+      <c r="O8" s="143" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="70"/>
-      <c r="S8" s="50" t="s">
+      <c r="P8" s="143"/>
+      <c r="Q8" s="143"/>
+      <c r="R8" s="144"/>
+      <c r="S8" s="124" t="s">
         <v>7</v>
       </c>
-      <c r="T8" s="51"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="51"/>
+      <c r="T8" s="125"/>
+      <c r="U8" s="125"/>
+      <c r="V8" s="125"/>
+      <c r="W8" s="125"/>
     </row>
     <row r="9" spans="1:23" ht="26.4" customHeight="1">
       <c r="B9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="129" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="60" t="s">
+      <c r="D9" s="130"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="130"/>
+      <c r="G9" s="134" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="54" t="s">
+      <c r="H9" s="134"/>
+      <c r="I9" s="134"/>
+      <c r="J9" s="134"/>
+      <c r="K9" s="128" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="54"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="54"/>
+      <c r="L9" s="128"/>
+      <c r="M9" s="128"/>
+      <c r="N9" s="128"/>
       <c r="O9" s="20"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="20"/>
       <c r="R9" s="22"/>
-      <c r="S9" s="50"/>
-      <c r="T9" s="51"/>
-      <c r="U9" s="51"/>
-      <c r="V9" s="51"/>
-      <c r="W9" s="51"/>
+      <c r="S9" s="124"/>
+      <c r="T9" s="125"/>
+      <c r="U9" s="125"/>
+      <c r="V9" s="125"/>
+      <c r="W9" s="125"/>
     </row>
     <row r="10" spans="1:23" ht="22.8" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="129" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56" t="s">
+      <c r="D10" s="130"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="130"/>
+      <c r="G10" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56" t="s">
+      <c r="H10" s="130"/>
+      <c r="I10" s="130"/>
+      <c r="J10" s="130"/>
+      <c r="K10" s="130" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
+      <c r="L10" s="130"/>
+      <c r="M10" s="130"/>
+      <c r="N10" s="130"/>
       <c r="O10" s="24"/>
       <c r="P10" s="24"/>
       <c r="Q10" s="24"/>
       <c r="R10" s="25"/>
-      <c r="S10" s="52" t="s">
+      <c r="S10" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="T10" s="52"/>
-      <c r="U10" s="52"/>
-      <c r="V10" s="52"/>
-      <c r="W10" s="52"/>
+      <c r="T10" s="126"/>
+      <c r="U10" s="126"/>
+      <c r="V10" s="126"/>
+      <c r="W10" s="126"/>
     </row>
     <row r="11" spans="1:23" ht="22.8" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="132" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59" t="s">
+      <c r="D11" s="133"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="133"/>
+      <c r="G11" s="133" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
+      <c r="H11" s="133"/>
+      <c r="I11" s="133"/>
+      <c r="J11" s="133"/>
       <c r="K11" s="44"/>
       <c r="L11" s="44"/>
       <c r="M11" s="44"/>
@@ -6273,13 +6305,13 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="21"/>
       <c r="R13" s="34"/>
-      <c r="S13" s="52" t="s">
+      <c r="S13" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="T13" s="53"/>
-      <c r="U13" s="53"/>
-      <c r="V13" s="53"/>
-      <c r="W13" s="53"/>
+      <c r="T13" s="127"/>
+      <c r="U13" s="127"/>
+      <c r="V13" s="127"/>
+      <c r="W13" s="127"/>
     </row>
     <row r="14" spans="1:23" ht="15.6">
       <c r="A14" s="1"/>
@@ -6340,12 +6372,12 @@
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="62" t="s">
+      <c r="C16" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
+      <c r="D16" s="123"/>
+      <c r="E16" s="123"/>
+      <c r="F16" s="123"/>
       <c r="G16" s="47" t="s">
         <v>56</v>
       </c>
@@ -6458,30 +6490,30 @@
       <c r="B20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="68" t="s">
+      <c r="C20" s="140" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66"/>
-      <c r="G20" s="66" t="s">
+      <c r="D20" s="141"/>
+      <c r="E20" s="141"/>
+      <c r="F20" s="141"/>
+      <c r="G20" s="141" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="66"/>
-      <c r="I20" s="66"/>
-      <c r="J20" s="66"/>
-      <c r="K20" s="66" t="s">
+      <c r="H20" s="141"/>
+      <c r="I20" s="141"/>
+      <c r="J20" s="141"/>
+      <c r="K20" s="141" t="s">
         <v>61</v>
       </c>
-      <c r="L20" s="66"/>
-      <c r="M20" s="66"/>
-      <c r="N20" s="66"/>
-      <c r="O20" s="63" t="s">
+      <c r="L20" s="141"/>
+      <c r="M20" s="141"/>
+      <c r="N20" s="141"/>
+      <c r="O20" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="P20" s="63"/>
-      <c r="Q20" s="63"/>
-      <c r="R20" s="67"/>
+      <c r="P20" s="123"/>
+      <c r="Q20" s="123"/>
+      <c r="R20" s="142"/>
       <c r="S20" s="5"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
@@ -6571,6 +6603,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="S13:W13"/>
+    <mergeCell ref="S10:W10"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="S8:W9"/>
@@ -6579,18 +6623,6 @@
     <mergeCell ref="K9:N9"/>
     <mergeCell ref="K8:N8"/>
     <mergeCell ref="O8:R8"/>
-    <mergeCell ref="S13:W13"/>
-    <mergeCell ref="S10:W10"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6671,96 +6703,96 @@
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="136" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65" t="s">
+      <c r="D8" s="137"/>
+      <c r="E8" s="137"/>
+      <c r="F8" s="137"/>
+      <c r="G8" s="137"/>
+      <c r="H8" s="137"/>
+      <c r="I8" s="137"/>
+      <c r="J8" s="137"/>
+      <c r="K8" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="65"/>
-      <c r="O8" s="65"/>
-      <c r="P8" s="65"/>
-      <c r="Q8" s="65"/>
-      <c r="R8" s="71"/>
-      <c r="S8" s="50" t="s">
+      <c r="L8" s="137"/>
+      <c r="M8" s="137"/>
+      <c r="N8" s="137"/>
+      <c r="O8" s="137"/>
+      <c r="P8" s="137"/>
+      <c r="Q8" s="137"/>
+      <c r="R8" s="145"/>
+      <c r="S8" s="124" t="s">
         <v>7</v>
       </c>
-      <c r="T8" s="51"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="51"/>
+      <c r="T8" s="125"/>
+      <c r="U8" s="125"/>
+      <c r="V8" s="125"/>
+      <c r="W8" s="125"/>
     </row>
     <row r="9" spans="1:23" ht="26.4" customHeight="1">
       <c r="B9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="54" t="s">
+      <c r="D9" s="130"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="130"/>
+      <c r="G9" s="130"/>
+      <c r="H9" s="130"/>
+      <c r="I9" s="130"/>
+      <c r="J9" s="130"/>
+      <c r="K9" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="54"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="54"/>
-      <c r="P9" s="54"/>
-      <c r="Q9" s="54"/>
-      <c r="R9" s="72"/>
-      <c r="S9" s="50"/>
-      <c r="T9" s="51"/>
-      <c r="U9" s="51"/>
-      <c r="V9" s="51"/>
-      <c r="W9" s="51"/>
+      <c r="L9" s="128"/>
+      <c r="M9" s="128"/>
+      <c r="N9" s="128"/>
+      <c r="O9" s="128"/>
+      <c r="P9" s="128"/>
+      <c r="Q9" s="128"/>
+      <c r="R9" s="146"/>
+      <c r="S9" s="124"/>
+      <c r="T9" s="125"/>
+      <c r="U9" s="125"/>
+      <c r="V9" s="125"/>
+      <c r="W9" s="125"/>
     </row>
     <row r="10" spans="1:23" ht="22.8" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="129" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56" t="s">
+      <c r="D10" s="130"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="130"/>
+      <c r="G10" s="130"/>
+      <c r="H10" s="130"/>
+      <c r="I10" s="130"/>
+      <c r="J10" s="130"/>
+      <c r="K10" s="130" t="s">
         <v>39</v>
       </c>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="57"/>
-      <c r="S10" s="52" t="s">
+      <c r="L10" s="130"/>
+      <c r="M10" s="130"/>
+      <c r="N10" s="130"/>
+      <c r="O10" s="130"/>
+      <c r="P10" s="130"/>
+      <c r="Q10" s="130"/>
+      <c r="R10" s="131"/>
+      <c r="S10" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="T10" s="52"/>
-      <c r="U10" s="52"/>
-      <c r="V10" s="52"/>
-      <c r="W10" s="52"/>
+      <c r="T10" s="126"/>
+      <c r="U10" s="126"/>
+      <c r="V10" s="126"/>
+      <c r="W10" s="126"/>
     </row>
     <row r="11" spans="1:23" ht="22.8" customHeight="1">
       <c r="A11" s="4"/>
@@ -6837,13 +6869,13 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="21"/>
       <c r="R13" s="34"/>
-      <c r="S13" s="52" t="s">
+      <c r="S13" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="T13" s="53"/>
-      <c r="U13" s="53"/>
-      <c r="V13" s="53"/>
-      <c r="W13" s="53"/>
+      <c r="T13" s="127"/>
+      <c r="U13" s="127"/>
+      <c r="V13" s="127"/>
+      <c r="W13" s="127"/>
     </row>
     <row r="14" spans="1:23" ht="15.6">
       <c r="A14" s="1"/>

</xml_diff>

<commit_message>
Console commands and memory call updates
</commit_message>
<xml_diff>
--- a/Documentation/Memory Map/MemoryMap.xlsx
+++ b/Documentation/Memory Map/MemoryMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\version-control\EDD-LCP_PistonDriver\Documentation\Memory Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D13B096-480F-4AC3-A07E-15566474BB41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB158BB-E736-4CAE-9C3D-2E5DDE30D98F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{9A36670B-9FAC-4E7D-BCC1-D5C646D37D72}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="108">
   <si>
     <t>A</t>
   </si>
@@ -346,6 +346,15 @@
   </si>
   <si>
     <t>LEN_TOTAL_IN</t>
+  </si>
+  <si>
+    <t>VOL_HOUSING_IN3</t>
+  </si>
+  <si>
+    <t>TRV_FULL</t>
+  </si>
+  <si>
+    <t>TRV_MIN</t>
   </si>
 </sst>
 </file>
@@ -1494,18 +1503,93 @@
     <xf numFmtId="0" fontId="20" fillId="7" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1524,18 +1608,9 @@
     <xf numFmtId="0" fontId="23" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1545,115 +1620,76 @@
     <xf numFmtId="0" fontId="20" fillId="6" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1662,37 +1698,10 @@
     <xf numFmtId="0" fontId="20" fillId="6" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2050,7 +2059,7 @@
   <dimension ref="B7:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:N11"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2111,30 +2120,30 @@
       <c r="B9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="111" t="s">
+      <c r="C9" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="113"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="96"/>
       <c r="G9" s="24"/>
       <c r="H9" s="24"/>
       <c r="I9" s="24"/>
       <c r="J9" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="114" t="s">
+      <c r="K9" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="114"/>
-      <c r="M9" s="114"/>
-      <c r="N9" s="114"/>
-      <c r="O9" s="114" t="s">
-        <v>48</v>
-      </c>
-      <c r="P9" s="114"/>
-      <c r="Q9" s="114"/>
-      <c r="R9" s="115"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="97"/>
+      <c r="O9" s="97" t="s">
+        <v>105</v>
+      </c>
+      <c r="P9" s="97"/>
+      <c r="Q9" s="97"/>
+      <c r="R9" s="98"/>
     </row>
     <row r="10" spans="2:18" ht="15.6">
       <c r="B10" s="14" t="s">
@@ -2148,43 +2157,43 @@
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
-      <c r="K10" s="96" t="s">
+      <c r="K10" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="96"/>
-      <c r="M10" s="96"/>
-      <c r="N10" s="96"/>
-      <c r="O10" s="116" t="s">
+      <c r="L10" s="86"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="P10" s="116"/>
-      <c r="Q10" s="116"/>
-      <c r="R10" s="117"/>
+      <c r="P10" s="99"/>
+      <c r="Q10" s="99"/>
+      <c r="R10" s="100"/>
     </row>
     <row r="11" spans="2:18" ht="15.6">
       <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="118" t="s">
+      <c r="C11" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="119"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
       <c r="J11" s="24"/>
-      <c r="K11" s="96" t="s">
+      <c r="K11" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="L11" s="96"/>
-      <c r="M11" s="96"/>
-      <c r="N11" s="96"/>
-      <c r="O11" s="96"/>
-      <c r="P11" s="96"/>
-      <c r="Q11" s="96"/>
-      <c r="R11" s="97"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="87"/>
     </row>
     <row r="12" spans="2:18" ht="15.6">
       <c r="B12" s="11" t="s">
@@ -2198,74 +2207,74 @@
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
-      <c r="K12" s="96" t="s">
+      <c r="K12" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="L12" s="96"/>
-      <c r="M12" s="96"/>
-      <c r="N12" s="96"/>
-      <c r="O12" s="96" t="s">
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="P12" s="96"/>
-      <c r="Q12" s="96"/>
-      <c r="R12" s="97"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="87"/>
     </row>
     <row r="13" spans="2:18" ht="15.6" customHeight="1">
       <c r="B13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="108" t="s">
+      <c r="C13" s="101" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="109"/>
-      <c r="E13" s="109"/>
-      <c r="F13" s="109"/>
-      <c r="G13" s="109" t="s">
+      <c r="D13" s="102"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="109"/>
-      <c r="K13" s="94" t="s">
+      <c r="H13" s="102"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="L13" s="94"/>
-      <c r="M13" s="94"/>
-      <c r="N13" s="94"/>
-      <c r="O13" s="106" t="s">
+      <c r="L13" s="103"/>
+      <c r="M13" s="103"/>
+      <c r="N13" s="103"/>
+      <c r="O13" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="P13" s="106"/>
-      <c r="Q13" s="106"/>
-      <c r="R13" s="107"/>
+      <c r="P13" s="104"/>
+      <c r="Q13" s="104"/>
+      <c r="R13" s="105"/>
     </row>
     <row r="14" spans="2:18" ht="22.8" customHeight="1">
       <c r="B14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="101" t="s">
+      <c r="C14" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="102"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="102"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="107"/>
+      <c r="F14" s="107"/>
       <c r="G14" s="70"/>
       <c r="H14" s="70"/>
       <c r="I14" s="70"/>
       <c r="J14" s="70"/>
-      <c r="K14" s="86" t="s">
+      <c r="K14" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="L14" s="87"/>
-      <c r="M14" s="87"/>
-      <c r="N14" s="147"/>
-      <c r="O14" s="148" t="s">
+      <c r="L14" s="89"/>
+      <c r="M14" s="89"/>
+      <c r="N14" s="90"/>
+      <c r="O14" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="P14" s="149"/>
-      <c r="Q14" s="149"/>
-      <c r="R14" s="150"/>
+      <c r="P14" s="92"/>
+      <c r="Q14" s="92"/>
+      <c r="R14" s="93"/>
     </row>
     <row r="15" spans="2:18" ht="22.8">
       <c r="B15" s="6" t="s">
@@ -2289,10 +2298,14 @@
         <v>32</v>
       </c>
       <c r="L15" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="M15" s="78" t="s">
+        <v>107</v>
+      </c>
+      <c r="N15" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
       <c r="O15" s="29"/>
       <c r="P15" s="29"/>
       <c r="Q15" s="29"/>
@@ -2323,55 +2336,55 @@
       <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="103" t="s">
+      <c r="C17" s="108" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="104"/>
-      <c r="E17" s="104"/>
-      <c r="F17" s="104"/>
-      <c r="G17" s="104" t="s">
+      <c r="D17" s="109"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="109"/>
+      <c r="G17" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="104"/>
-      <c r="I17" s="104"/>
-      <c r="J17" s="105"/>
-      <c r="K17" s="96" t="s">
+      <c r="H17" s="109"/>
+      <c r="I17" s="109"/>
+      <c r="J17" s="110"/>
+      <c r="K17" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="97"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="86"/>
+      <c r="N17" s="86"/>
+      <c r="O17" s="86"/>
+      <c r="P17" s="86"/>
+      <c r="Q17" s="86"/>
+      <c r="R17" s="87"/>
     </row>
     <row r="18" spans="2:18" ht="15.6">
       <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="103" t="s">
+      <c r="C18" s="108" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="104"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="104"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="109"/>
       <c r="G18" s="76" t="s">
         <v>62</v>
       </c>
       <c r="H18" s="76"/>
       <c r="I18" s="76"/>
       <c r="J18" s="81"/>
-      <c r="K18" s="96" t="s">
+      <c r="K18" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="L18" s="96"/>
-      <c r="M18" s="96"/>
-      <c r="N18" s="96"/>
-      <c r="O18" s="96"/>
-      <c r="P18" s="96"/>
-      <c r="Q18" s="96"/>
-      <c r="R18" s="97"/>
+      <c r="L18" s="86"/>
+      <c r="M18" s="86"/>
+      <c r="N18" s="86"/>
+      <c r="O18" s="86"/>
+      <c r="P18" s="86"/>
+      <c r="Q18" s="86"/>
+      <c r="R18" s="87"/>
     </row>
     <row r="19" spans="2:18" ht="15.6">
       <c r="B19" s="6" t="s">
@@ -2385,16 +2398,16 @@
       <c r="H19" s="20"/>
       <c r="I19" s="20"/>
       <c r="J19" s="20"/>
-      <c r="K19" s="92" t="s">
+      <c r="K19" s="117" t="s">
         <v>36</v>
       </c>
-      <c r="L19" s="92"/>
-      <c r="M19" s="92"/>
-      <c r="N19" s="92"/>
-      <c r="O19" s="92"/>
-      <c r="P19" s="92"/>
-      <c r="Q19" s="92"/>
-      <c r="R19" s="93"/>
+      <c r="L19" s="117"/>
+      <c r="M19" s="117"/>
+      <c r="N19" s="117"/>
+      <c r="O19" s="117"/>
+      <c r="P19" s="117"/>
+      <c r="Q19" s="117"/>
+      <c r="R19" s="118"/>
     </row>
     <row r="20" spans="2:18" ht="15.6">
       <c r="B20" s="6" t="s">
@@ -2408,16 +2421,16 @@
       <c r="H20" s="20"/>
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
-      <c r="K20" s="94" t="s">
+      <c r="K20" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="L20" s="94"/>
-      <c r="M20" s="94"/>
-      <c r="N20" s="94"/>
-      <c r="O20" s="94"/>
-      <c r="P20" s="94"/>
-      <c r="Q20" s="94"/>
-      <c r="R20" s="95"/>
+      <c r="L20" s="103"/>
+      <c r="M20" s="103"/>
+      <c r="N20" s="103"/>
+      <c r="O20" s="103"/>
+      <c r="P20" s="103"/>
+      <c r="Q20" s="103"/>
+      <c r="R20" s="119"/>
     </row>
     <row r="21" spans="2:18" ht="15.6">
       <c r="B21" s="6" t="s">
@@ -2431,16 +2444,16 @@
       <c r="H21" s="38"/>
       <c r="I21" s="38"/>
       <c r="J21" s="38"/>
-      <c r="K21" s="96" t="s">
+      <c r="K21" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="L21" s="96"/>
-      <c r="M21" s="96"/>
-      <c r="N21" s="96"/>
-      <c r="O21" s="96"/>
-      <c r="P21" s="96"/>
-      <c r="Q21" s="96"/>
-      <c r="R21" s="97"/>
+      <c r="L21" s="86"/>
+      <c r="M21" s="86"/>
+      <c r="N21" s="86"/>
+      <c r="O21" s="86"/>
+      <c r="P21" s="86"/>
+      <c r="Q21" s="86"/>
+      <c r="R21" s="87"/>
     </row>
     <row r="22" spans="2:18" ht="15.6">
       <c r="B22" s="6" t="s">
@@ -2454,16 +2467,16 @@
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
       <c r="J22" s="20"/>
-      <c r="K22" s="94" t="s">
+      <c r="K22" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="L22" s="94"/>
-      <c r="M22" s="94"/>
-      <c r="N22" s="94"/>
-      <c r="O22" s="94"/>
-      <c r="P22" s="94"/>
-      <c r="Q22" s="94"/>
-      <c r="R22" s="95"/>
+      <c r="L22" s="103"/>
+      <c r="M22" s="103"/>
+      <c r="N22" s="103"/>
+      <c r="O22" s="103"/>
+      <c r="P22" s="103"/>
+      <c r="Q22" s="103"/>
+      <c r="R22" s="119"/>
     </row>
     <row r="23" spans="2:18" ht="15.6" customHeight="1">
       <c r="B23" s="6" t="s">
@@ -2477,69 +2490,69 @@
       <c r="H23" s="20"/>
       <c r="I23" s="20"/>
       <c r="J23" s="20"/>
-      <c r="K23" s="86" t="s">
+      <c r="K23" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="L23" s="87"/>
-      <c r="M23" s="87"/>
-      <c r="N23" s="87"/>
-      <c r="O23" s="87"/>
-      <c r="P23" s="87"/>
-      <c r="Q23" s="87"/>
-      <c r="R23" s="88"/>
+      <c r="L23" s="89"/>
+      <c r="M23" s="89"/>
+      <c r="N23" s="89"/>
+      <c r="O23" s="89"/>
+      <c r="P23" s="89"/>
+      <c r="Q23" s="89"/>
+      <c r="R23" s="113"/>
     </row>
     <row r="24" spans="2:18" ht="16.2" customHeight="1" thickBot="1">
       <c r="B24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="98" t="s">
+      <c r="C24" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="99"/>
-      <c r="E24" s="99"/>
-      <c r="F24" s="99"/>
-      <c r="G24" s="99"/>
-      <c r="H24" s="99"/>
-      <c r="I24" s="99"/>
-      <c r="J24" s="100"/>
-      <c r="K24" s="86" t="s">
+      <c r="D24" s="121"/>
+      <c r="E24" s="121"/>
+      <c r="F24" s="121"/>
+      <c r="G24" s="121"/>
+      <c r="H24" s="121"/>
+      <c r="I24" s="121"/>
+      <c r="J24" s="122"/>
+      <c r="K24" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="L24" s="88"/>
+      <c r="L24" s="113"/>
       <c r="M24" s="83" t="s">
         <v>42</v>
       </c>
       <c r="N24" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="O24" s="89" t="s">
+      <c r="O24" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="P24" s="90"/>
-      <c r="Q24" s="90"/>
-      <c r="R24" s="91"/>
+      <c r="P24" s="115"/>
+      <c r="Q24" s="115"/>
+      <c r="R24" s="116"/>
     </row>
     <row r="26" spans="2:18">
-      <c r="C26" s="85" t="s">
+      <c r="C26" s="112" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="85"/>
-      <c r="E26" s="85"/>
-      <c r="F26" s="85"/>
-      <c r="G26" s="85"/>
-      <c r="H26" s="85"/>
-      <c r="I26" s="85"/>
-      <c r="J26" s="85"/>
-      <c r="K26" s="84" t="s">
+      <c r="D26" s="112"/>
+      <c r="E26" s="112"/>
+      <c r="F26" s="112"/>
+      <c r="G26" s="112"/>
+      <c r="H26" s="112"/>
+      <c r="I26" s="112"/>
+      <c r="J26" s="112"/>
+      <c r="K26" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="L26" s="84"/>
-      <c r="M26" s="84"/>
-      <c r="N26" s="84"/>
-      <c r="O26" s="84"/>
-      <c r="P26" s="84"/>
-      <c r="Q26" s="84"/>
-      <c r="R26" s="84"/>
+      <c r="L26" s="111"/>
+      <c r="M26" s="111"/>
+      <c r="N26" s="111"/>
+      <c r="O26" s="111"/>
+      <c r="P26" s="111"/>
+      <c r="Q26" s="111"/>
+      <c r="R26" s="111"/>
     </row>
     <row r="28" spans="2:18">
       <c r="C28" t="s">
@@ -2548,28 +2561,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="O11:R11"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="O14:R14"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="O9:R9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="O10:R10"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="O12:R12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="O13:R13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="K17:R17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="K18:R18"/>
     <mergeCell ref="K26:R26"/>
     <mergeCell ref="C26:J26"/>
     <mergeCell ref="K23:R23"/>
@@ -2580,6 +2571,28 @@
     <mergeCell ref="K22:R22"/>
     <mergeCell ref="C24:J24"/>
     <mergeCell ref="K24:L24"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="K17:R17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="K18:R18"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="O9:R9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="O10:R10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="O11:R11"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="O14:R14"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="O12:R12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="O13:R13"/>
+    <mergeCell ref="C14:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2650,12 +2663,12 @@
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="113"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="96"/>
       <c r="F2" s="24" t="s">
         <v>6</v>
       </c>
@@ -2668,18 +2681,18 @@
       <c r="I2" s="82" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="114" t="s">
+      <c r="J2" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="114"/>
-      <c r="L2" s="114"/>
-      <c r="M2" s="114"/>
-      <c r="N2" s="114" t="s">
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97" t="s">
         <v>80</v>
       </c>
-      <c r="O2" s="114"/>
-      <c r="P2" s="114"/>
-      <c r="Q2" s="115"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
+      <c r="Q2" s="98"/>
     </row>
     <row r="3" spans="1:17" ht="15.6">
       <c r="A3" s="14" t="s">
@@ -2709,29 +2722,29 @@
       <c r="I3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="96" t="s">
+      <c r="J3" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="116" t="s">
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="99" t="s">
         <v>82</v>
       </c>
-      <c r="O3" s="116"/>
-      <c r="P3" s="116"/>
-      <c r="Q3" s="117"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
+      <c r="Q3" s="100"/>
     </row>
     <row r="4" spans="1:17" ht="15.6">
       <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="84" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
       <c r="F4" s="24" t="s">
         <v>6</v>
       </c>
@@ -2744,18 +2757,18 @@
       <c r="I4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="96" t="s">
+      <c r="J4" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="96" t="s">
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="O4" s="96"/>
-      <c r="P4" s="96"/>
-      <c r="Q4" s="97"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="86"/>
+      <c r="Q4" s="87"/>
     </row>
     <row r="5" spans="1:17" ht="15.6">
       <c r="A5" s="11" t="s">
@@ -2785,58 +2798,58 @@
       <c r="I5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="94" t="s">
+      <c r="J5" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="K5" s="94"/>
-      <c r="L5" s="94"/>
-      <c r="M5" s="94"/>
-      <c r="N5" s="106" t="s">
+      <c r="K5" s="103"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="103"/>
+      <c r="N5" s="104" t="s">
         <v>86</v>
       </c>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="107"/>
+      <c r="O5" s="104"/>
+      <c r="P5" s="104"/>
+      <c r="Q5" s="105"/>
     </row>
     <row r="6" spans="1:17" ht="15.6">
       <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109" t="s">
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="110" t="s">
+      <c r="G6" s="102"/>
+      <c r="H6" s="102"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="123" t="s">
         <v>87</v>
       </c>
-      <c r="K6" s="110"/>
-      <c r="L6" s="110"/>
-      <c r="M6" s="110"/>
-      <c r="N6" s="96" t="s">
+      <c r="K6" s="123"/>
+      <c r="L6" s="123"/>
+      <c r="M6" s="123"/>
+      <c r="N6" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="O6" s="96"/>
-      <c r="P6" s="96"/>
-      <c r="Q6" s="97"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="86"/>
+      <c r="Q6" s="87"/>
     </row>
     <row r="7" spans="1:17" ht="15.6">
       <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="106" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="102"/>
-      <c r="D7" s="102"/>
-      <c r="E7" s="102"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
       <c r="F7" s="24" t="s">
         <v>6</v>
       </c>
@@ -2984,39 +2997,39 @@
       <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="108" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="104"/>
-      <c r="D10" s="104"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="104" t="s">
+      <c r="C10" s="109"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="G10" s="104"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="105"/>
-      <c r="J10" s="96" t="s">
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="110"/>
+      <c r="J10" s="86" t="s">
         <v>94</v>
       </c>
-      <c r="K10" s="96"/>
-      <c r="L10" s="96"/>
-      <c r="M10" s="96"/>
-      <c r="N10" s="96"/>
-      <c r="O10" s="96"/>
-      <c r="P10" s="96"/>
-      <c r="Q10" s="97"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="86"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="86"/>
+      <c r="P10" s="86"/>
+      <c r="Q10" s="87"/>
     </row>
     <row r="11" spans="1:17" ht="15.6">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="108" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="104"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="104"/>
+      <c r="C11" s="109"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
       <c r="F11" s="76" t="s">
         <v>6</v>
       </c>
@@ -3029,16 +3042,16 @@
       <c r="I11" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="96" t="s">
+      <c r="J11" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="K11" s="96"/>
-      <c r="L11" s="96"/>
-      <c r="M11" s="96"/>
-      <c r="N11" s="96"/>
-      <c r="O11" s="96"/>
-      <c r="P11" s="96"/>
-      <c r="Q11" s="97"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="87"/>
     </row>
     <row r="12" spans="1:17" ht="15.6">
       <c r="A12" s="6" t="s">
@@ -3068,16 +3081,16 @@
       <c r="I12" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="92" t="s">
+      <c r="J12" s="117" t="s">
         <v>96</v>
       </c>
-      <c r="K12" s="92"/>
-      <c r="L12" s="92"/>
-      <c r="M12" s="92"/>
-      <c r="N12" s="92"/>
-      <c r="O12" s="92"/>
-      <c r="P12" s="92"/>
-      <c r="Q12" s="93"/>
+      <c r="K12" s="117"/>
+      <c r="L12" s="117"/>
+      <c r="M12" s="117"/>
+      <c r="N12" s="117"/>
+      <c r="O12" s="117"/>
+      <c r="P12" s="117"/>
+      <c r="Q12" s="118"/>
     </row>
     <row r="13" spans="1:17" ht="15.6">
       <c r="A13" s="6" t="s">
@@ -3107,16 +3120,16 @@
       <c r="I13" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="94" t="s">
+      <c r="J13" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
-      <c r="M13" s="94"/>
-      <c r="N13" s="94"/>
-      <c r="O13" s="94"/>
-      <c r="P13" s="94"/>
-      <c r="Q13" s="95"/>
+      <c r="K13" s="103"/>
+      <c r="L13" s="103"/>
+      <c r="M13" s="103"/>
+      <c r="N13" s="103"/>
+      <c r="O13" s="103"/>
+      <c r="P13" s="103"/>
+      <c r="Q13" s="119"/>
     </row>
     <row r="14" spans="1:17" ht="15.6">
       <c r="A14" s="6" t="s">
@@ -3146,16 +3159,16 @@
       <c r="I14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J14" s="96" t="s">
+      <c r="J14" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="K14" s="96"/>
-      <c r="L14" s="96"/>
-      <c r="M14" s="96"/>
-      <c r="N14" s="96"/>
-      <c r="O14" s="96"/>
-      <c r="P14" s="96"/>
-      <c r="Q14" s="97"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="86"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="86"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="87"/>
     </row>
     <row r="15" spans="1:17" ht="15.6">
       <c r="A15" s="6" t="s">
@@ -3185,16 +3198,16 @@
       <c r="I15" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J15" s="94" t="s">
+      <c r="J15" s="103" t="s">
         <v>99</v>
       </c>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="94"/>
-      <c r="O15" s="94"/>
-      <c r="P15" s="94"/>
-      <c r="Q15" s="95"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="103"/>
+      <c r="M15" s="103"/>
+      <c r="N15" s="103"/>
+      <c r="O15" s="103"/>
+      <c r="P15" s="103"/>
+      <c r="Q15" s="119"/>
     </row>
     <row r="16" spans="1:17" ht="15.6">
       <c r="A16" s="6" t="s">
@@ -3224,47 +3237,47 @@
       <c r="I16" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="86" t="s">
+      <c r="J16" s="88" t="s">
         <v>103</v>
       </c>
-      <c r="K16" s="87"/>
-      <c r="L16" s="87"/>
-      <c r="M16" s="87"/>
-      <c r="N16" s="87"/>
-      <c r="O16" s="87"/>
-      <c r="P16" s="87"/>
-      <c r="Q16" s="88"/>
+      <c r="K16" s="89"/>
+      <c r="L16" s="89"/>
+      <c r="M16" s="89"/>
+      <c r="N16" s="89"/>
+      <c r="O16" s="89"/>
+      <c r="P16" s="89"/>
+      <c r="Q16" s="113"/>
     </row>
     <row r="17" spans="1:17" ht="16.2" thickBot="1">
       <c r="A17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="98" t="s">
+      <c r="B17" s="120" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="99"/>
-      <c r="D17" s="99"/>
-      <c r="E17" s="99"/>
-      <c r="F17" s="99"/>
-      <c r="G17" s="99"/>
-      <c r="H17" s="99"/>
-      <c r="I17" s="100"/>
-      <c r="J17" s="86" t="s">
+      <c r="C17" s="121"/>
+      <c r="D17" s="121"/>
+      <c r="E17" s="121"/>
+      <c r="F17" s="121"/>
+      <c r="G17" s="121"/>
+      <c r="H17" s="121"/>
+      <c r="I17" s="122"/>
+      <c r="J17" s="88" t="s">
         <v>90</v>
       </c>
-      <c r="K17" s="88"/>
-      <c r="L17" s="120" t="s">
+      <c r="K17" s="113"/>
+      <c r="L17" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="M17" s="120"/>
-      <c r="N17" s="120" t="s">
+      <c r="M17" s="124"/>
+      <c r="N17" s="124" t="s">
         <v>91</v>
       </c>
-      <c r="O17" s="120"/>
-      <c r="P17" s="120" t="s">
+      <c r="O17" s="124"/>
+      <c r="P17" s="124" t="s">
         <v>93</v>
       </c>
-      <c r="Q17" s="121"/>
+      <c r="Q17" s="125"/>
     </row>
     <row r="18" spans="1:17" ht="15" thickBot="1"/>
     <row r="19" spans="1:17" ht="16.2" thickBot="1">
@@ -3321,30 +3334,30 @@
       <c r="A20" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="111">
+      <c r="B20" s="94">
         <v>33.299999999999997</v>
       </c>
-      <c r="C20" s="112"/>
-      <c r="D20" s="112"/>
-      <c r="E20" s="113"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="96"/>
       <c r="F20" s="24"/>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
       <c r="I20" s="82">
         <v>119</v>
       </c>
-      <c r="J20" s="114">
+      <c r="J20" s="97">
         <v>33.299999999999997</v>
       </c>
-      <c r="K20" s="114"/>
-      <c r="L20" s="114"/>
-      <c r="M20" s="114"/>
-      <c r="N20" s="114">
+      <c r="K20" s="97"/>
+      <c r="L20" s="97"/>
+      <c r="M20" s="97"/>
+      <c r="N20" s="97">
         <v>128.79</v>
       </c>
-      <c r="O20" s="114"/>
-      <c r="P20" s="114"/>
-      <c r="Q20" s="115"/>
+      <c r="O20" s="97"/>
+      <c r="P20" s="97"/>
+      <c r="Q20" s="98"/>
     </row>
     <row r="21" spans="1:17" ht="15.6">
       <c r="A21" s="14" t="s">
@@ -3358,45 +3371,45 @@
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
       <c r="I21" s="24"/>
-      <c r="J21" s="96">
+      <c r="J21" s="86">
         <v>28.79</v>
       </c>
-      <c r="K21" s="96"/>
-      <c r="L21" s="96"/>
-      <c r="M21" s="96"/>
-      <c r="N21" s="116">
+      <c r="K21" s="86"/>
+      <c r="L21" s="86"/>
+      <c r="M21" s="86"/>
+      <c r="N21" s="99">
         <v>100</v>
       </c>
-      <c r="O21" s="116"/>
-      <c r="P21" s="116"/>
-      <c r="Q21" s="117"/>
+      <c r="O21" s="99"/>
+      <c r="P21" s="99"/>
+      <c r="Q21" s="100"/>
     </row>
     <row r="22" spans="1:17" ht="15.6">
       <c r="A22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="118">
+      <c r="B22" s="84">
         <v>8.8888800000000003</v>
       </c>
-      <c r="C22" s="119"/>
-      <c r="D22" s="119"/>
-      <c r="E22" s="119"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
       <c r="F22" s="24"/>
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
       <c r="I22" s="24"/>
-      <c r="J22" s="96">
+      <c r="J22" s="86">
         <v>5.5</v>
       </c>
-      <c r="K22" s="96"/>
-      <c r="L22" s="96"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="96">
+      <c r="K22" s="86"/>
+      <c r="L22" s="86"/>
+      <c r="M22" s="86"/>
+      <c r="N22" s="86">
         <v>2.5</v>
       </c>
-      <c r="O22" s="96"/>
-      <c r="P22" s="96"/>
-      <c r="Q22" s="97"/>
+      <c r="O22" s="86"/>
+      <c r="P22" s="86"/>
+      <c r="Q22" s="87"/>
     </row>
     <row r="23" spans="1:17" ht="15.6">
       <c r="A23" s="11" t="s">
@@ -3410,58 +3423,58 @@
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
       <c r="I23" s="27"/>
-      <c r="J23" s="94">
+      <c r="J23" s="103">
         <v>1.4</v>
       </c>
-      <c r="K23" s="94"/>
-      <c r="L23" s="94"/>
-      <c r="M23" s="94"/>
-      <c r="N23" s="106">
+      <c r="K23" s="103"/>
+      <c r="L23" s="103"/>
+      <c r="M23" s="103"/>
+      <c r="N23" s="104">
         <v>13.2</v>
       </c>
-      <c r="O23" s="106"/>
-      <c r="P23" s="106"/>
-      <c r="Q23" s="107"/>
+      <c r="O23" s="104"/>
+      <c r="P23" s="104"/>
+      <c r="Q23" s="105"/>
     </row>
     <row r="24" spans="1:17" ht="15.6">
       <c r="A24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="108">
+      <c r="B24" s="101">
         <v>0.15</v>
       </c>
-      <c r="C24" s="109"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="109">
+      <c r="C24" s="102"/>
+      <c r="D24" s="102"/>
+      <c r="E24" s="102"/>
+      <c r="F24" s="102">
         <v>11.7</v>
       </c>
-      <c r="G24" s="109"/>
-      <c r="H24" s="109"/>
-      <c r="I24" s="109"/>
-      <c r="J24" s="110">
+      <c r="G24" s="102"/>
+      <c r="H24" s="102"/>
+      <c r="I24" s="102"/>
+      <c r="J24" s="123">
         <v>0</v>
       </c>
-      <c r="K24" s="110"/>
-      <c r="L24" s="110"/>
-      <c r="M24" s="110"/>
-      <c r="N24" s="96">
+      <c r="K24" s="123"/>
+      <c r="L24" s="123"/>
+      <c r="M24" s="123"/>
+      <c r="N24" s="86">
         <v>8</v>
       </c>
-      <c r="O24" s="96"/>
-      <c r="P24" s="96"/>
-      <c r="Q24" s="97"/>
+      <c r="O24" s="86"/>
+      <c r="P24" s="86"/>
+      <c r="Q24" s="87"/>
     </row>
     <row r="25" spans="1:17" ht="15.6">
       <c r="A25" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="101">
+      <c r="B25" s="106">
         <v>125732</v>
       </c>
-      <c r="C25" s="102"/>
-      <c r="D25" s="102"/>
-      <c r="E25" s="102"/>
+      <c r="C25" s="107"/>
+      <c r="D25" s="107"/>
+      <c r="E25" s="107"/>
       <c r="F25" s="70"/>
       <c r="G25" s="70"/>
       <c r="H25" s="70"/>
@@ -3531,55 +3544,55 @@
       <c r="A28" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="103">
+      <c r="B28" s="108">
         <v>0.1234</v>
       </c>
-      <c r="C28" s="104"/>
-      <c r="D28" s="104"/>
-      <c r="E28" s="104"/>
-      <c r="F28" s="104">
+      <c r="C28" s="109"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="109"/>
+      <c r="F28" s="109">
         <v>2.3216999999999999</v>
       </c>
-      <c r="G28" s="104"/>
-      <c r="H28" s="104"/>
-      <c r="I28" s="105"/>
-      <c r="J28" s="96">
+      <c r="G28" s="109"/>
+      <c r="H28" s="109"/>
+      <c r="I28" s="110"/>
+      <c r="J28" s="86">
         <v>0.12</v>
       </c>
-      <c r="K28" s="96"/>
-      <c r="L28" s="96"/>
-      <c r="M28" s="96"/>
-      <c r="N28" s="96"/>
-      <c r="O28" s="96"/>
-      <c r="P28" s="96"/>
-      <c r="Q28" s="97"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="86"/>
+      <c r="N28" s="86"/>
+      <c r="O28" s="86"/>
+      <c r="P28" s="86"/>
+      <c r="Q28" s="87"/>
     </row>
     <row r="29" spans="1:17" ht="15.6">
       <c r="A29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="103">
+      <c r="B29" s="108">
         <v>128.78800000000001</v>
       </c>
-      <c r="C29" s="104"/>
-      <c r="D29" s="104"/>
-      <c r="E29" s="104"/>
+      <c r="C29" s="109"/>
+      <c r="D29" s="109"/>
+      <c r="E29" s="109"/>
       <c r="F29" s="76">
         <v>0</v>
       </c>
       <c r="G29" s="76"/>
       <c r="H29" s="76"/>
       <c r="I29" s="81"/>
-      <c r="J29" s="96">
+      <c r="J29" s="86">
         <v>1</v>
       </c>
-      <c r="K29" s="96"/>
-      <c r="L29" s="96"/>
-      <c r="M29" s="96"/>
-      <c r="N29" s="96"/>
-      <c r="O29" s="96"/>
-      <c r="P29" s="96"/>
-      <c r="Q29" s="97"/>
+      <c r="K29" s="86"/>
+      <c r="L29" s="86"/>
+      <c r="M29" s="86"/>
+      <c r="N29" s="86"/>
+      <c r="O29" s="86"/>
+      <c r="P29" s="86"/>
+      <c r="Q29" s="87"/>
     </row>
     <row r="30" spans="1:17" ht="15.6">
       <c r="A30" s="6" t="s">
@@ -3593,16 +3606,16 @@
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
-      <c r="J30" s="92">
+      <c r="J30" s="117">
         <v>13.289020320000001</v>
       </c>
-      <c r="K30" s="92"/>
-      <c r="L30" s="92"/>
-      <c r="M30" s="92"/>
-      <c r="N30" s="92"/>
-      <c r="O30" s="92"/>
-      <c r="P30" s="92"/>
-      <c r="Q30" s="93"/>
+      <c r="K30" s="117"/>
+      <c r="L30" s="117"/>
+      <c r="M30" s="117"/>
+      <c r="N30" s="117"/>
+      <c r="O30" s="117"/>
+      <c r="P30" s="117"/>
+      <c r="Q30" s="118"/>
     </row>
     <row r="31" spans="1:17" ht="15.6">
       <c r="A31" s="6" t="s">
@@ -3616,16 +3629,16 @@
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
-      <c r="J31" s="94">
+      <c r="J31" s="103">
         <v>0.11111111110000001</v>
       </c>
-      <c r="K31" s="94"/>
-      <c r="L31" s="94"/>
-      <c r="M31" s="94"/>
-      <c r="N31" s="94"/>
-      <c r="O31" s="94"/>
-      <c r="P31" s="94"/>
-      <c r="Q31" s="95"/>
+      <c r="K31" s="103"/>
+      <c r="L31" s="103"/>
+      <c r="M31" s="103"/>
+      <c r="N31" s="103"/>
+      <c r="O31" s="103"/>
+      <c r="P31" s="103"/>
+      <c r="Q31" s="119"/>
     </row>
     <row r="32" spans="1:17" ht="15.6">
       <c r="A32" s="6" t="s">
@@ -3639,16 +3652,16 @@
       <c r="G32" s="38"/>
       <c r="H32" s="38"/>
       <c r="I32" s="38"/>
-      <c r="J32" s="96">
+      <c r="J32" s="86">
         <v>0</v>
       </c>
-      <c r="K32" s="96"/>
-      <c r="L32" s="96"/>
-      <c r="M32" s="96"/>
-      <c r="N32" s="96"/>
-      <c r="O32" s="96"/>
-      <c r="P32" s="96"/>
-      <c r="Q32" s="97"/>
+      <c r="K32" s="86"/>
+      <c r="L32" s="86"/>
+      <c r="M32" s="86"/>
+      <c r="N32" s="86"/>
+      <c r="O32" s="86"/>
+      <c r="P32" s="86"/>
+      <c r="Q32" s="87"/>
     </row>
     <row r="33" spans="1:17" ht="15.6">
       <c r="A33" s="6" t="s">
@@ -3662,16 +3675,16 @@
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
-      <c r="J33" s="94">
+      <c r="J33" s="103">
         <v>1010101</v>
       </c>
-      <c r="K33" s="94"/>
-      <c r="L33" s="94"/>
-      <c r="M33" s="94"/>
-      <c r="N33" s="94"/>
-      <c r="O33" s="94"/>
-      <c r="P33" s="94"/>
-      <c r="Q33" s="95"/>
+      <c r="K33" s="103"/>
+      <c r="L33" s="103"/>
+      <c r="M33" s="103"/>
+      <c r="N33" s="103"/>
+      <c r="O33" s="103"/>
+      <c r="P33" s="103"/>
+      <c r="Q33" s="119"/>
     </row>
     <row r="34" spans="1:17" ht="15.6">
       <c r="A34" s="6" t="s">
@@ -3685,70 +3698,74 @@
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
-      <c r="J34" s="86" t="s">
+      <c r="J34" s="88" t="s">
         <v>101</v>
       </c>
-      <c r="K34" s="87"/>
-      <c r="L34" s="87"/>
-      <c r="M34" s="87"/>
-      <c r="N34" s="87"/>
-      <c r="O34" s="87"/>
-      <c r="P34" s="87"/>
-      <c r="Q34" s="88"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="89"/>
+      <c r="M34" s="89"/>
+      <c r="N34" s="89"/>
+      <c r="O34" s="89"/>
+      <c r="P34" s="89"/>
+      <c r="Q34" s="113"/>
     </row>
     <row r="35" spans="1:17" ht="16.2" thickBot="1">
       <c r="A35" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="98" t="s">
+      <c r="B35" s="120" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="99"/>
-      <c r="D35" s="99"/>
-      <c r="E35" s="99"/>
-      <c r="F35" s="99"/>
-      <c r="G35" s="99"/>
-      <c r="H35" s="99"/>
-      <c r="I35" s="100"/>
-      <c r="J35" s="86">
+      <c r="C35" s="121"/>
+      <c r="D35" s="121"/>
+      <c r="E35" s="121"/>
+      <c r="F35" s="121"/>
+      <c r="G35" s="121"/>
+      <c r="H35" s="121"/>
+      <c r="I35" s="122"/>
+      <c r="J35" s="88">
         <v>2021</v>
       </c>
-      <c r="K35" s="88"/>
-      <c r="L35" s="120">
+      <c r="K35" s="113"/>
+      <c r="L35" s="124">
         <v>1</v>
       </c>
-      <c r="M35" s="120"/>
-      <c r="N35" s="120">
+      <c r="M35" s="124"/>
+      <c r="N35" s="124">
         <v>8</v>
       </c>
-      <c r="O35" s="120"/>
-      <c r="P35" s="120">
+      <c r="O35" s="124"/>
+      <c r="P35" s="124">
         <v>23</v>
       </c>
-      <c r="Q35" s="121"/>
+      <c r="Q35" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="J10:Q10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="J11:Q11"/>
+    <mergeCell ref="J30:Q30"/>
+    <mergeCell ref="J31:Q31"/>
+    <mergeCell ref="J32:Q32"/>
+    <mergeCell ref="J33:Q33"/>
+    <mergeCell ref="J34:Q34"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="J28:Q28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="J29:Q29"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="N21:Q21"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="N23:Q23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="N24:Q24"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="J22:M22"/>
     <mergeCell ref="N22:Q22"/>
@@ -3765,30 +3782,26 @@
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="J20:M20"/>
     <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="N21:Q21"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="N23:Q23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="N24:Q24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="J28:Q28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="J29:Q29"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="P35:Q35"/>
-    <mergeCell ref="J30:Q30"/>
-    <mergeCell ref="J31:Q31"/>
-    <mergeCell ref="J32:Q32"/>
-    <mergeCell ref="J33:Q33"/>
-    <mergeCell ref="J34:Q34"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="J10:Q10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="J11:Q11"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3870,18 +3883,18 @@
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="136" t="s">
+      <c r="C8" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="137"/>
-      <c r="E8" s="137"/>
-      <c r="F8" s="137"/>
-      <c r="G8" s="137" t="s">
+      <c r="D8" s="139"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="139" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="137"/>
-      <c r="I8" s="137"/>
-      <c r="J8" s="137"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="139"/>
+      <c r="J8" s="139"/>
       <c r="K8" s="16"/>
       <c r="L8" s="17"/>
       <c r="M8" s="46"/>
@@ -3890,36 +3903,36 @@
       <c r="P8" s="46"/>
       <c r="Q8" s="18"/>
       <c r="R8" s="19"/>
-      <c r="S8" s="124" t="s">
+      <c r="S8" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="T8" s="125"/>
-      <c r="U8" s="125"/>
-      <c r="V8" s="125"/>
-      <c r="W8" s="125"/>
+      <c r="T8" s="127"/>
+      <c r="U8" s="127"/>
+      <c r="V8" s="127"/>
+      <c r="W8" s="127"/>
     </row>
     <row r="9" spans="1:23" ht="26.4" customHeight="1">
       <c r="B9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="129" t="s">
+      <c r="C9" s="131" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="130"/>
-      <c r="E9" s="130"/>
-      <c r="F9" s="130"/>
-      <c r="G9" s="134" t="s">
+      <c r="D9" s="132"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="134"/>
-      <c r="I9" s="134"/>
-      <c r="J9" s="134"/>
-      <c r="K9" s="128" t="s">
+      <c r="H9" s="136"/>
+      <c r="I9" s="136"/>
+      <c r="J9" s="136"/>
+      <c r="K9" s="130" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="128"/>
-      <c r="M9" s="128"/>
-      <c r="N9" s="128"/>
+      <c r="L9" s="130"/>
+      <c r="M9" s="130"/>
+      <c r="N9" s="130"/>
       <c r="O9" s="47" t="s">
         <v>30</v>
       </c>
@@ -3932,70 +3945,70 @@
       <c r="R9" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="S9" s="124"/>
-      <c r="T9" s="125"/>
-      <c r="U9" s="125"/>
-      <c r="V9" s="125"/>
-      <c r="W9" s="125"/>
+      <c r="S9" s="126"/>
+      <c r="T9" s="127"/>
+      <c r="U9" s="127"/>
+      <c r="V9" s="127"/>
+      <c r="W9" s="127"/>
     </row>
     <row r="10" spans="1:23" ht="22.8" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="129" t="s">
+      <c r="C10" s="131" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="130"/>
-      <c r="E10" s="130"/>
-      <c r="F10" s="130"/>
-      <c r="G10" s="130"/>
-      <c r="H10" s="130"/>
-      <c r="I10" s="130"/>
-      <c r="J10" s="130"/>
-      <c r="K10" s="130" t="s">
+      <c r="D10" s="132"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="132"/>
+      <c r="G10" s="132"/>
+      <c r="H10" s="132"/>
+      <c r="I10" s="132"/>
+      <c r="J10" s="132"/>
+      <c r="K10" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="130"/>
-      <c r="M10" s="130"/>
-      <c r="N10" s="130"/>
-      <c r="O10" s="130"/>
-      <c r="P10" s="130"/>
-      <c r="Q10" s="130"/>
-      <c r="R10" s="131"/>
-      <c r="S10" s="126" t="s">
+      <c r="L10" s="132"/>
+      <c r="M10" s="132"/>
+      <c r="N10" s="132"/>
+      <c r="O10" s="132"/>
+      <c r="P10" s="132"/>
+      <c r="Q10" s="132"/>
+      <c r="R10" s="133"/>
+      <c r="S10" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="T10" s="126"/>
-      <c r="U10" s="126"/>
-      <c r="V10" s="126"/>
-      <c r="W10" s="126"/>
+      <c r="T10" s="128"/>
+      <c r="U10" s="128"/>
+      <c r="V10" s="128"/>
+      <c r="W10" s="128"/>
     </row>
     <row r="11" spans="1:23" ht="22.8" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="132" t="s">
+      <c r="C11" s="134" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="133"/>
-      <c r="E11" s="133"/>
-      <c r="F11" s="133"/>
-      <c r="G11" s="133"/>
-      <c r="H11" s="133"/>
-      <c r="I11" s="133"/>
-      <c r="J11" s="133"/>
-      <c r="K11" s="134" t="s">
+      <c r="D11" s="135"/>
+      <c r="E11" s="135"/>
+      <c r="F11" s="135"/>
+      <c r="G11" s="135"/>
+      <c r="H11" s="135"/>
+      <c r="I11" s="135"/>
+      <c r="J11" s="135"/>
+      <c r="K11" s="136" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="134"/>
-      <c r="M11" s="134"/>
-      <c r="N11" s="134"/>
-      <c r="O11" s="134"/>
-      <c r="P11" s="134"/>
-      <c r="Q11" s="134"/>
-      <c r="R11" s="135"/>
+      <c r="L11" s="136"/>
+      <c r="M11" s="136"/>
+      <c r="N11" s="136"/>
+      <c r="O11" s="136"/>
+      <c r="P11" s="136"/>
+      <c r="Q11" s="136"/>
+      <c r="R11" s="137"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
@@ -4007,26 +4020,26 @@
       <c r="B12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="129" t="s">
+      <c r="C12" s="131" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="130"/>
-      <c r="E12" s="130"/>
-      <c r="F12" s="130"/>
-      <c r="G12" s="130"/>
-      <c r="H12" s="130"/>
-      <c r="I12" s="130"/>
-      <c r="J12" s="130"/>
-      <c r="K12" s="134" t="s">
+      <c r="D12" s="132"/>
+      <c r="E12" s="132"/>
+      <c r="F12" s="132"/>
+      <c r="G12" s="132"/>
+      <c r="H12" s="132"/>
+      <c r="I12" s="132"/>
+      <c r="J12" s="132"/>
+      <c r="K12" s="136" t="s">
         <v>39</v>
       </c>
-      <c r="L12" s="134"/>
-      <c r="M12" s="134"/>
-      <c r="N12" s="134"/>
-      <c r="O12" s="134"/>
-      <c r="P12" s="134"/>
-      <c r="Q12" s="134"/>
-      <c r="R12" s="135"/>
+      <c r="L12" s="136"/>
+      <c r="M12" s="136"/>
+      <c r="N12" s="136"/>
+      <c r="O12" s="136"/>
+      <c r="P12" s="136"/>
+      <c r="Q12" s="136"/>
+      <c r="R12" s="137"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
@@ -4054,13 +4067,13 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="21"/>
       <c r="R13" s="34"/>
-      <c r="S13" s="126" t="s">
+      <c r="S13" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="T13" s="127"/>
-      <c r="U13" s="127"/>
-      <c r="V13" s="127"/>
-      <c r="W13" s="127"/>
+      <c r="T13" s="129"/>
+      <c r="U13" s="129"/>
+      <c r="V13" s="129"/>
+      <c r="W13" s="129"/>
     </row>
     <row r="14" spans="1:23" ht="15.6">
       <c r="A14" s="1"/>
@@ -4121,26 +4134,26 @@
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="122" t="s">
+      <c r="C16" s="140" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="123"/>
-      <c r="E16" s="123" t="s">
+      <c r="D16" s="141"/>
+      <c r="E16" s="141" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="123"/>
-      <c r="G16" s="123" t="s">
+      <c r="F16" s="141"/>
+      <c r="G16" s="141" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="123"/>
-      <c r="I16" s="123" t="s">
+      <c r="H16" s="141"/>
+      <c r="I16" s="141" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="123"/>
-      <c r="K16" s="123" t="s">
+      <c r="J16" s="141"/>
+      <c r="K16" s="141" t="s">
         <v>44</v>
       </c>
-      <c r="L16" s="123"/>
+      <c r="L16" s="141"/>
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
       <c r="O16" s="20"/>
@@ -4344,6 +4357,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
     <mergeCell ref="S8:W9"/>
     <mergeCell ref="S13:W13"/>
     <mergeCell ref="S10:W10"/>
@@ -4358,11 +4376,6 @@
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="G9:J9"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4380,14 +4393,14 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:38" ht="15" thickBot="1">
-      <c r="A1" s="136"/>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
+      <c r="A1" s="138"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
       <c r="I1" s="16"/>
       <c r="J1" s="17"/>
       <c r="K1" s="46"/>
@@ -4398,18 +4411,18 @@
       <c r="P1" s="19"/>
     </row>
     <row r="2" spans="1:38" ht="16.2" thickBot="1">
-      <c r="A2" s="129"/>
-      <c r="B2" s="130"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="128"/>
+      <c r="A2" s="131"/>
+      <c r="B2" s="132"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="130"/>
+      <c r="J2" s="130"/>
+      <c r="K2" s="130"/>
+      <c r="L2" s="130"/>
       <c r="M2" s="47"/>
       <c r="N2" s="48"/>
       <c r="O2" s="47"/>
@@ -4465,22 +4478,22 @@
       </c>
     </row>
     <row r="3" spans="1:38">
-      <c r="A3" s="129"/>
-      <c r="B3" s="130"/>
-      <c r="C3" s="130"/>
-      <c r="D3" s="130"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="130"/>
-      <c r="G3" s="130"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="130"/>
-      <c r="K3" s="130"/>
-      <c r="L3" s="130"/>
-      <c r="M3" s="130"/>
-      <c r="N3" s="130"/>
-      <c r="O3" s="130"/>
-      <c r="P3" s="131"/>
+      <c r="A3" s="131"/>
+      <c r="B3" s="132"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="132"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="132"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="132"/>
+      <c r="M3" s="132"/>
+      <c r="N3" s="132"/>
+      <c r="O3" s="132"/>
+      <c r="P3" s="133"/>
       <c r="W3" s="53"/>
       <c r="X3" s="54"/>
       <c r="Y3" s="54"/>
@@ -4499,22 +4512,22 @@
       <c r="AL3" s="55"/>
     </row>
     <row r="4" spans="1:38">
-      <c r="A4" s="132"/>
-      <c r="B4" s="133"/>
-      <c r="C4" s="133"/>
-      <c r="D4" s="133"/>
-      <c r="E4" s="133"/>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
-      <c r="H4" s="133"/>
-      <c r="I4" s="134"/>
-      <c r="J4" s="134"/>
-      <c r="K4" s="134"/>
-      <c r="L4" s="134"/>
-      <c r="M4" s="134"/>
-      <c r="N4" s="134"/>
-      <c r="O4" s="134"/>
-      <c r="P4" s="135"/>
+      <c r="A4" s="134"/>
+      <c r="B4" s="135"/>
+      <c r="C4" s="135"/>
+      <c r="D4" s="135"/>
+      <c r="E4" s="135"/>
+      <c r="F4" s="135"/>
+      <c r="G4" s="135"/>
+      <c r="H4" s="135"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="136"/>
+      <c r="K4" s="136"/>
+      <c r="L4" s="136"/>
+      <c r="M4" s="136"/>
+      <c r="N4" s="136"/>
+      <c r="O4" s="136"/>
+      <c r="P4" s="137"/>
       <c r="W4" s="56"/>
       <c r="X4" s="24"/>
       <c r="Y4" s="24"/>
@@ -4533,22 +4546,22 @@
       <c r="AL4" s="57"/>
     </row>
     <row r="5" spans="1:38">
-      <c r="A5" s="129"/>
-      <c r="B5" s="130"/>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="134"/>
-      <c r="J5" s="134"/>
-      <c r="K5" s="134"/>
-      <c r="L5" s="134"/>
-      <c r="M5" s="134"/>
-      <c r="N5" s="134"/>
-      <c r="O5" s="134"/>
-      <c r="P5" s="135"/>
+      <c r="A5" s="131"/>
+      <c r="B5" s="132"/>
+      <c r="C5" s="132"/>
+      <c r="D5" s="132"/>
+      <c r="E5" s="132"/>
+      <c r="F5" s="132"/>
+      <c r="G5" s="132"/>
+      <c r="H5" s="132"/>
+      <c r="I5" s="136"/>
+      <c r="J5" s="136"/>
+      <c r="K5" s="136"/>
+      <c r="L5" s="136"/>
+      <c r="M5" s="136"/>
+      <c r="N5" s="136"/>
+      <c r="O5" s="136"/>
+      <c r="P5" s="137"/>
       <c r="W5" s="56"/>
       <c r="X5" s="24"/>
       <c r="Y5" s="24"/>
@@ -4669,16 +4682,16 @@
       <c r="AL8" s="62"/>
     </row>
     <row r="9" spans="1:38">
-      <c r="A9" s="122"/>
-      <c r="B9" s="123"/>
-      <c r="C9" s="123"/>
-      <c r="D9" s="123"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="123"/>
-      <c r="H9" s="123"/>
-      <c r="I9" s="123"/>
-      <c r="J9" s="123"/>
+      <c r="A9" s="140"/>
+      <c r="B9" s="141"/>
+      <c r="C9" s="141"/>
+      <c r="D9" s="141"/>
+      <c r="E9" s="141"/>
+      <c r="F9" s="141"/>
+      <c r="G9" s="141"/>
+      <c r="H9" s="141"/>
+      <c r="I9" s="141"/>
+      <c r="J9" s="141"/>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
@@ -4941,22 +4954,22 @@
       <c r="AL16" s="66"/>
     </row>
     <row r="17" spans="1:38">
-      <c r="A17" s="136"/>
-      <c r="B17" s="137"/>
-      <c r="C17" s="137"/>
-      <c r="D17" s="137"/>
-      <c r="E17" s="137"/>
-      <c r="F17" s="137"/>
-      <c r="G17" s="137"/>
-      <c r="H17" s="137"/>
-      <c r="I17" s="137"/>
-      <c r="J17" s="137"/>
-      <c r="K17" s="137"/>
-      <c r="L17" s="137"/>
-      <c r="M17" s="143"/>
-      <c r="N17" s="143"/>
-      <c r="O17" s="143"/>
-      <c r="P17" s="144"/>
+      <c r="A17" s="138"/>
+      <c r="B17" s="139"/>
+      <c r="C17" s="139"/>
+      <c r="D17" s="139"/>
+      <c r="E17" s="139"/>
+      <c r="F17" s="139"/>
+      <c r="G17" s="139"/>
+      <c r="H17" s="139"/>
+      <c r="I17" s="139"/>
+      <c r="J17" s="139"/>
+      <c r="K17" s="139"/>
+      <c r="L17" s="139"/>
+      <c r="M17" s="142"/>
+      <c r="N17" s="142"/>
+      <c r="O17" s="142"/>
+      <c r="P17" s="143"/>
       <c r="W17" s="61"/>
       <c r="X17" s="20"/>
       <c r="Y17" s="20"/>
@@ -4975,18 +4988,18 @@
       <c r="AL17" s="66"/>
     </row>
     <row r="18" spans="1:38">
-      <c r="A18" s="129"/>
-      <c r="B18" s="130"/>
-      <c r="C18" s="130"/>
-      <c r="D18" s="130"/>
-      <c r="E18" s="134"/>
-      <c r="F18" s="134"/>
-      <c r="G18" s="134"/>
-      <c r="H18" s="134"/>
-      <c r="I18" s="128"/>
-      <c r="J18" s="128"/>
-      <c r="K18" s="128"/>
-      <c r="L18" s="128"/>
+      <c r="A18" s="131"/>
+      <c r="B18" s="132"/>
+      <c r="C18" s="132"/>
+      <c r="D18" s="132"/>
+      <c r="E18" s="136"/>
+      <c r="F18" s="136"/>
+      <c r="G18" s="136"/>
+      <c r="H18" s="136"/>
+      <c r="I18" s="130"/>
+      <c r="J18" s="130"/>
+      <c r="K18" s="130"/>
+      <c r="L18" s="130"/>
       <c r="M18" s="20"/>
       <c r="N18" s="21"/>
       <c r="O18" s="20"/>
@@ -5009,32 +5022,32 @@
       <c r="AL18" s="69"/>
     </row>
     <row r="19" spans="1:38" ht="15" thickBot="1">
-      <c r="A19" s="129"/>
-      <c r="B19" s="130"/>
-      <c r="C19" s="130"/>
-      <c r="D19" s="130"/>
-      <c r="E19" s="130"/>
-      <c r="F19" s="130"/>
-      <c r="G19" s="130"/>
-      <c r="H19" s="130"/>
-      <c r="I19" s="130"/>
-      <c r="J19" s="130"/>
-      <c r="K19" s="130"/>
-      <c r="L19" s="130"/>
+      <c r="A19" s="131"/>
+      <c r="B19" s="132"/>
+      <c r="C19" s="132"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="132"/>
+      <c r="F19" s="132"/>
+      <c r="G19" s="132"/>
+      <c r="H19" s="132"/>
+      <c r="I19" s="132"/>
+      <c r="J19" s="132"/>
+      <c r="K19" s="132"/>
+      <c r="L19" s="132"/>
       <c r="M19" s="24"/>
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
       <c r="P19" s="25"/>
     </row>
     <row r="20" spans="1:38" ht="16.2" thickBot="1">
-      <c r="A20" s="132"/>
-      <c r="B20" s="133"/>
-      <c r="C20" s="133"/>
-      <c r="D20" s="133"/>
-      <c r="E20" s="133"/>
-      <c r="F20" s="133"/>
-      <c r="G20" s="133"/>
-      <c r="H20" s="133"/>
+      <c r="A20" s="134"/>
+      <c r="B20" s="135"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="135"/>
+      <c r="E20" s="135"/>
+      <c r="F20" s="135"/>
+      <c r="G20" s="135"/>
+      <c r="H20" s="135"/>
       <c r="I20" s="44"/>
       <c r="J20" s="44"/>
       <c r="K20" s="44"/>
@@ -5113,28 +5126,28 @@
       <c r="V21" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="W21" s="111" t="s">
+      <c r="W21" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="X21" s="112"/>
-      <c r="Y21" s="112"/>
-      <c r="Z21" s="113"/>
+      <c r="X21" s="95"/>
+      <c r="Y21" s="95"/>
+      <c r="Z21" s="96"/>
       <c r="AA21" s="24"/>
       <c r="AB21" s="24"/>
       <c r="AC21" s="24"/>
       <c r="AD21" s="24"/>
-      <c r="AE21" s="114" t="s">
+      <c r="AE21" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="AF21" s="114"/>
-      <c r="AG21" s="114"/>
-      <c r="AH21" s="114"/>
-      <c r="AI21" s="114" t="s">
+      <c r="AF21" s="97"/>
+      <c r="AG21" s="97"/>
+      <c r="AH21" s="97"/>
+      <c r="AI21" s="97" t="s">
         <v>48</v>
       </c>
-      <c r="AJ21" s="114"/>
-      <c r="AK21" s="114"/>
-      <c r="AL21" s="115"/>
+      <c r="AJ21" s="97"/>
+      <c r="AK21" s="97"/>
+      <c r="AL21" s="98"/>
     </row>
     <row r="22" spans="1:38" ht="15.6">
       <c r="A22" s="33"/>
@@ -5164,18 +5177,18 @@
       <c r="AB22" s="24"/>
       <c r="AC22" s="24"/>
       <c r="AD22" s="24"/>
-      <c r="AE22" s="96" t="s">
+      <c r="AE22" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="AF22" s="96"/>
-      <c r="AG22" s="96"/>
-      <c r="AH22" s="96"/>
-      <c r="AI22" s="116" t="s">
+      <c r="AF22" s="86"/>
+      <c r="AG22" s="86"/>
+      <c r="AH22" s="86"/>
+      <c r="AI22" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="AJ22" s="116"/>
-      <c r="AK22" s="116"/>
-      <c r="AL22" s="117"/>
+      <c r="AJ22" s="99"/>
+      <c r="AK22" s="99"/>
+      <c r="AL22" s="100"/>
     </row>
     <row r="23" spans="1:38" ht="15.6">
       <c r="A23" s="31"/>
@@ -5197,28 +5210,28 @@
       <c r="V23" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="W23" s="118" t="s">
+      <c r="W23" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="X23" s="119"/>
-      <c r="Y23" s="119"/>
-      <c r="Z23" s="119"/>
+      <c r="X23" s="85"/>
+      <c r="Y23" s="85"/>
+      <c r="Z23" s="85"/>
       <c r="AA23" s="24"/>
       <c r="AB23" s="24"/>
       <c r="AC23" s="24"/>
       <c r="AD23" s="24"/>
-      <c r="AE23" s="96" t="s">
+      <c r="AE23" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="AF23" s="96"/>
-      <c r="AG23" s="96"/>
-      <c r="AH23" s="96"/>
-      <c r="AI23" s="96" t="s">
+      <c r="AF23" s="86"/>
+      <c r="AG23" s="86"/>
+      <c r="AH23" s="86"/>
+      <c r="AI23" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="AJ23" s="96"/>
-      <c r="AK23" s="96"/>
-      <c r="AL23" s="97"/>
+      <c r="AJ23" s="86"/>
+      <c r="AK23" s="86"/>
+      <c r="AL23" s="87"/>
     </row>
     <row r="24" spans="1:38" ht="15.6">
       <c r="A24" s="35"/>
@@ -5248,24 +5261,24 @@
       <c r="AB24" s="27"/>
       <c r="AC24" s="27"/>
       <c r="AD24" s="27"/>
-      <c r="AE24" s="94" t="s">
+      <c r="AE24" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="AF24" s="94"/>
-      <c r="AG24" s="94"/>
-      <c r="AH24" s="94"/>
-      <c r="AI24" s="106" t="s">
+      <c r="AF24" s="103"/>
+      <c r="AG24" s="103"/>
+      <c r="AH24" s="103"/>
+      <c r="AI24" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="AJ24" s="106"/>
-      <c r="AK24" s="106"/>
-      <c r="AL24" s="107"/>
+      <c r="AJ24" s="104"/>
+      <c r="AK24" s="104"/>
+      <c r="AL24" s="105"/>
     </row>
     <row r="25" spans="1:38" ht="15.6">
-      <c r="A25" s="122"/>
-      <c r="B25" s="123"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="123"/>
+      <c r="A25" s="140"/>
+      <c r="B25" s="141"/>
+      <c r="C25" s="141"/>
+      <c r="D25" s="141"/>
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
       <c r="G25" s="47"/>
@@ -5281,30 +5294,30 @@
       <c r="V25" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="W25" s="108" t="s">
+      <c r="W25" s="101" t="s">
         <v>54</v>
       </c>
-      <c r="X25" s="109"/>
-      <c r="Y25" s="109"/>
-      <c r="Z25" s="109"/>
-      <c r="AA25" s="109" t="s">
+      <c r="X25" s="102"/>
+      <c r="Y25" s="102"/>
+      <c r="Z25" s="102"/>
+      <c r="AA25" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="AB25" s="109"/>
-      <c r="AC25" s="109"/>
-      <c r="AD25" s="109"/>
-      <c r="AE25" s="110" t="s">
+      <c r="AB25" s="102"/>
+      <c r="AC25" s="102"/>
+      <c r="AD25" s="102"/>
+      <c r="AE25" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="AF25" s="110"/>
-      <c r="AG25" s="110"/>
-      <c r="AH25" s="110"/>
-      <c r="AI25" s="96" t="s">
+      <c r="AF25" s="123"/>
+      <c r="AG25" s="123"/>
+      <c r="AH25" s="123"/>
+      <c r="AI25" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="AJ25" s="96"/>
-      <c r="AK25" s="96"/>
-      <c r="AL25" s="97"/>
+      <c r="AJ25" s="86"/>
+      <c r="AK25" s="86"/>
+      <c r="AL25" s="87"/>
     </row>
     <row r="26" spans="1:38" ht="15.6">
       <c r="A26" s="37"/>
@@ -5326,12 +5339,12 @@
       <c r="V26" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="W26" s="101" t="s">
+      <c r="W26" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="X26" s="102"/>
-      <c r="Y26" s="102"/>
-      <c r="Z26" s="102"/>
+      <c r="X26" s="107"/>
+      <c r="Y26" s="107"/>
+      <c r="Z26" s="107"/>
       <c r="AA26" s="70"/>
       <c r="AB26" s="70"/>
       <c r="AC26" s="70"/>
@@ -5428,55 +5441,55 @@
       <c r="AL28" s="22"/>
     </row>
     <row r="29" spans="1:38" ht="15.6">
-      <c r="A29" s="140" t="s">
+      <c r="A29" s="144" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="141"/>
-      <c r="C29" s="141"/>
-      <c r="D29" s="141"/>
-      <c r="E29" s="141" t="s">
+      <c r="B29" s="145"/>
+      <c r="C29" s="145"/>
+      <c r="D29" s="145"/>
+      <c r="E29" s="145" t="s">
         <v>60</v>
       </c>
-      <c r="F29" s="141"/>
-      <c r="G29" s="141"/>
-      <c r="H29" s="141"/>
-      <c r="I29" s="141" t="s">
+      <c r="F29" s="145"/>
+      <c r="G29" s="145"/>
+      <c r="H29" s="145"/>
+      <c r="I29" s="145" t="s">
         <v>61</v>
       </c>
-      <c r="J29" s="141"/>
-      <c r="K29" s="141"/>
-      <c r="L29" s="141"/>
-      <c r="M29" s="123" t="s">
+      <c r="J29" s="145"/>
+      <c r="K29" s="145"/>
+      <c r="L29" s="145"/>
+      <c r="M29" s="141" t="s">
         <v>62</v>
       </c>
-      <c r="N29" s="123"/>
-      <c r="O29" s="123"/>
-      <c r="P29" s="142"/>
+      <c r="N29" s="141"/>
+      <c r="O29" s="141"/>
+      <c r="P29" s="146"/>
       <c r="V29" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="W29" s="103" t="s">
+      <c r="W29" s="108" t="s">
         <v>59</v>
       </c>
-      <c r="X29" s="104"/>
-      <c r="Y29" s="104"/>
-      <c r="Z29" s="104"/>
-      <c r="AA29" s="104" t="s">
+      <c r="X29" s="109"/>
+      <c r="Y29" s="109"/>
+      <c r="Z29" s="109"/>
+      <c r="AA29" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="AB29" s="104"/>
-      <c r="AC29" s="104"/>
-      <c r="AD29" s="105"/>
-      <c r="AE29" s="96" t="s">
+      <c r="AB29" s="109"/>
+      <c r="AC29" s="109"/>
+      <c r="AD29" s="110"/>
+      <c r="AE29" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="AF29" s="96"/>
-      <c r="AG29" s="96"/>
-      <c r="AH29" s="96"/>
-      <c r="AI29" s="96"/>
-      <c r="AJ29" s="96"/>
-      <c r="AK29" s="96"/>
-      <c r="AL29" s="97"/>
+      <c r="AF29" s="86"/>
+      <c r="AG29" s="86"/>
+      <c r="AH29" s="86"/>
+      <c r="AI29" s="86"/>
+      <c r="AJ29" s="86"/>
+      <c r="AK29" s="86"/>
+      <c r="AL29" s="87"/>
     </row>
     <row r="30" spans="1:38" ht="15.6">
       <c r="A30" s="35"/>
@@ -5498,28 +5511,28 @@
       <c r="V30" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="W30" s="103" t="s">
+      <c r="W30" s="108" t="s">
         <v>61</v>
       </c>
-      <c r="X30" s="104"/>
-      <c r="Y30" s="104"/>
-      <c r="Z30" s="104"/>
-      <c r="AA30" s="138" t="s">
+      <c r="X30" s="109"/>
+      <c r="Y30" s="109"/>
+      <c r="Z30" s="109"/>
+      <c r="AA30" s="147" t="s">
         <v>62</v>
       </c>
-      <c r="AB30" s="138"/>
-      <c r="AC30" s="138"/>
-      <c r="AD30" s="139"/>
-      <c r="AE30" s="96" t="s">
+      <c r="AB30" s="147"/>
+      <c r="AC30" s="147"/>
+      <c r="AD30" s="148"/>
+      <c r="AE30" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="AF30" s="96"/>
-      <c r="AG30" s="96"/>
-      <c r="AH30" s="96"/>
-      <c r="AI30" s="96"/>
-      <c r="AJ30" s="96"/>
-      <c r="AK30" s="96"/>
-      <c r="AL30" s="97"/>
+      <c r="AF30" s="86"/>
+      <c r="AG30" s="86"/>
+      <c r="AH30" s="86"/>
+      <c r="AI30" s="86"/>
+      <c r="AJ30" s="86"/>
+      <c r="AK30" s="86"/>
+      <c r="AL30" s="87"/>
     </row>
     <row r="31" spans="1:38" ht="15.6">
       <c r="A31" s="33"/>
@@ -5549,16 +5562,16 @@
       <c r="AB31" s="20"/>
       <c r="AC31" s="20"/>
       <c r="AD31" s="20"/>
-      <c r="AE31" s="92" t="s">
+      <c r="AE31" s="117" t="s">
         <v>36</v>
       </c>
-      <c r="AF31" s="92"/>
-      <c r="AG31" s="92"/>
-      <c r="AH31" s="92"/>
-      <c r="AI31" s="92"/>
-      <c r="AJ31" s="92"/>
-      <c r="AK31" s="92"/>
-      <c r="AL31" s="93"/>
+      <c r="AF31" s="117"/>
+      <c r="AG31" s="117"/>
+      <c r="AH31" s="117"/>
+      <c r="AI31" s="117"/>
+      <c r="AJ31" s="117"/>
+      <c r="AK31" s="117"/>
+      <c r="AL31" s="118"/>
     </row>
     <row r="32" spans="1:38" ht="15.6">
       <c r="A32" s="35"/>
@@ -5588,16 +5601,16 @@
       <c r="AB32" s="20"/>
       <c r="AC32" s="20"/>
       <c r="AD32" s="20"/>
-      <c r="AE32" s="94" t="s">
+      <c r="AE32" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="AF32" s="94"/>
-      <c r="AG32" s="94"/>
-      <c r="AH32" s="94"/>
-      <c r="AI32" s="94"/>
-      <c r="AJ32" s="94"/>
-      <c r="AK32" s="94"/>
-      <c r="AL32" s="95"/>
+      <c r="AF32" s="103"/>
+      <c r="AG32" s="103"/>
+      <c r="AH32" s="103"/>
+      <c r="AI32" s="103"/>
+      <c r="AJ32" s="103"/>
+      <c r="AK32" s="103"/>
+      <c r="AL32" s="119"/>
     </row>
     <row r="33" spans="1:38" ht="15.6">
       <c r="A33" s="53"/>
@@ -5627,16 +5640,16 @@
       <c r="AB33" s="38"/>
       <c r="AC33" s="38"/>
       <c r="AD33" s="38"/>
-      <c r="AE33" s="96" t="s">
+      <c r="AE33" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="AF33" s="96"/>
-      <c r="AG33" s="96"/>
-      <c r="AH33" s="96"/>
-      <c r="AI33" s="96"/>
-      <c r="AJ33" s="96"/>
-      <c r="AK33" s="96"/>
-      <c r="AL33" s="97"/>
+      <c r="AF33" s="86"/>
+      <c r="AG33" s="86"/>
+      <c r="AH33" s="86"/>
+      <c r="AI33" s="86"/>
+      <c r="AJ33" s="86"/>
+      <c r="AK33" s="86"/>
+      <c r="AL33" s="87"/>
     </row>
     <row r="34" spans="1:38" ht="15.6">
       <c r="A34" s="56"/>
@@ -5666,16 +5679,16 @@
       <c r="AB34" s="20"/>
       <c r="AC34" s="20"/>
       <c r="AD34" s="20"/>
-      <c r="AE34" s="94" t="s">
+      <c r="AE34" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="AF34" s="94"/>
-      <c r="AG34" s="94"/>
-      <c r="AH34" s="94"/>
-      <c r="AI34" s="94"/>
-      <c r="AJ34" s="94"/>
-      <c r="AK34" s="94"/>
-      <c r="AL34" s="95"/>
+      <c r="AF34" s="103"/>
+      <c r="AG34" s="103"/>
+      <c r="AH34" s="103"/>
+      <c r="AI34" s="103"/>
+      <c r="AJ34" s="103"/>
+      <c r="AK34" s="103"/>
+      <c r="AL34" s="119"/>
     </row>
     <row r="35" spans="1:38" ht="15.6">
       <c r="A35" s="56"/>
@@ -5711,10 +5724,10 @@
       <c r="AH35" s="20"/>
       <c r="AI35" s="20"/>
       <c r="AJ35" s="20"/>
-      <c r="AK35" s="86" t="s">
+      <c r="AK35" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="AL35" s="88"/>
+      <c r="AL35" s="113"/>
     </row>
     <row r="36" spans="1:38" ht="16.2" thickBot="1">
       <c r="A36" s="59"/>
@@ -5736,32 +5749,32 @@
       <c r="V36" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="W36" s="98" t="s">
+      <c r="W36" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="X36" s="99"/>
-      <c r="Y36" s="99"/>
-      <c r="Z36" s="99"/>
-      <c r="AA36" s="99"/>
-      <c r="AB36" s="99"/>
-      <c r="AC36" s="99"/>
-      <c r="AD36" s="100"/>
-      <c r="AE36" s="120" t="s">
+      <c r="X36" s="121"/>
+      <c r="Y36" s="121"/>
+      <c r="Z36" s="121"/>
+      <c r="AA36" s="121"/>
+      <c r="AB36" s="121"/>
+      <c r="AC36" s="121"/>
+      <c r="AD36" s="122"/>
+      <c r="AE36" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="AF36" s="120"/>
-      <c r="AG36" s="120" t="s">
+      <c r="AF36" s="124"/>
+      <c r="AG36" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="AH36" s="120"/>
-      <c r="AI36" s="120" t="s">
+      <c r="AH36" s="124"/>
+      <c r="AI36" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="AJ36" s="120"/>
-      <c r="AK36" s="120" t="s">
+      <c r="AJ36" s="124"/>
+      <c r="AK36" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="AL36" s="121"/>
+      <c r="AL36" s="125"/>
     </row>
     <row r="37" spans="1:38">
       <c r="A37" s="56"/>
@@ -5981,55 +5994,6 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:P3"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="I4:P4"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="I5:P5"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="W26:Z26"/>
-    <mergeCell ref="W29:Z29"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="I29:L29"/>
-    <mergeCell ref="M29:P29"/>
-    <mergeCell ref="AI24:AL24"/>
-    <mergeCell ref="AI21:AL21"/>
-    <mergeCell ref="W25:Z25"/>
-    <mergeCell ref="AA25:AD25"/>
-    <mergeCell ref="AE25:AH25"/>
-    <mergeCell ref="AI25:AL25"/>
-    <mergeCell ref="AE21:AH21"/>
-    <mergeCell ref="AE22:AH22"/>
-    <mergeCell ref="AI22:AL22"/>
-    <mergeCell ref="AE23:AH23"/>
-    <mergeCell ref="AI23:AL23"/>
-    <mergeCell ref="AE24:AH24"/>
-    <mergeCell ref="W21:Z21"/>
-    <mergeCell ref="W23:Z23"/>
     <mergeCell ref="AA29:AD29"/>
     <mergeCell ref="W30:Z30"/>
     <mergeCell ref="AA30:AD30"/>
@@ -6045,6 +6009,55 @@
     <mergeCell ref="AG36:AH36"/>
     <mergeCell ref="AI36:AJ36"/>
     <mergeCell ref="AK36:AL36"/>
+    <mergeCell ref="AI24:AL24"/>
+    <mergeCell ref="AI21:AL21"/>
+    <mergeCell ref="W25:Z25"/>
+    <mergeCell ref="AA25:AD25"/>
+    <mergeCell ref="AE25:AH25"/>
+    <mergeCell ref="AI25:AL25"/>
+    <mergeCell ref="AE21:AH21"/>
+    <mergeCell ref="AE22:AH22"/>
+    <mergeCell ref="AI22:AL22"/>
+    <mergeCell ref="AE23:AH23"/>
+    <mergeCell ref="AI23:AL23"/>
+    <mergeCell ref="AE24:AH24"/>
+    <mergeCell ref="W21:Z21"/>
+    <mergeCell ref="W23:Z23"/>
+    <mergeCell ref="W26:Z26"/>
+    <mergeCell ref="W29:Z29"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="M29:P29"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="I4:P4"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="I5:P5"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:P3"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6127,122 +6140,122 @@
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="136" t="s">
+      <c r="C8" s="138" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="137"/>
-      <c r="E8" s="137"/>
-      <c r="F8" s="137"/>
-      <c r="G8" s="137" t="s">
+      <c r="D8" s="139"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="139" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="137"/>
-      <c r="I8" s="137"/>
-      <c r="J8" s="137"/>
-      <c r="K8" s="137" t="s">
+      <c r="H8" s="139"/>
+      <c r="I8" s="139"/>
+      <c r="J8" s="139"/>
+      <c r="K8" s="139" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="137"/>
-      <c r="M8" s="137"/>
-      <c r="N8" s="137"/>
-      <c r="O8" s="143" t="s">
+      <c r="L8" s="139"/>
+      <c r="M8" s="139"/>
+      <c r="N8" s="139"/>
+      <c r="O8" s="142" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="143"/>
-      <c r="Q8" s="143"/>
-      <c r="R8" s="144"/>
-      <c r="S8" s="124" t="s">
+      <c r="P8" s="142"/>
+      <c r="Q8" s="142"/>
+      <c r="R8" s="143"/>
+      <c r="S8" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="T8" s="125"/>
-      <c r="U8" s="125"/>
-      <c r="V8" s="125"/>
-      <c r="W8" s="125"/>
+      <c r="T8" s="127"/>
+      <c r="U8" s="127"/>
+      <c r="V8" s="127"/>
+      <c r="W8" s="127"/>
     </row>
     <row r="9" spans="1:23" ht="26.4" customHeight="1">
       <c r="B9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="129" t="s">
+      <c r="C9" s="131" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="130"/>
-      <c r="E9" s="130"/>
-      <c r="F9" s="130"/>
-      <c r="G9" s="134" t="s">
+      <c r="D9" s="132"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="134"/>
-      <c r="I9" s="134"/>
-      <c r="J9" s="134"/>
-      <c r="K9" s="128" t="s">
+      <c r="H9" s="136"/>
+      <c r="I9" s="136"/>
+      <c r="J9" s="136"/>
+      <c r="K9" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="128"/>
-      <c r="M9" s="128"/>
-      <c r="N9" s="128"/>
+      <c r="L9" s="130"/>
+      <c r="M9" s="130"/>
+      <c r="N9" s="130"/>
       <c r="O9" s="20"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="20"/>
       <c r="R9" s="22"/>
-      <c r="S9" s="124"/>
-      <c r="T9" s="125"/>
-      <c r="U9" s="125"/>
-      <c r="V9" s="125"/>
-      <c r="W9" s="125"/>
+      <c r="S9" s="126"/>
+      <c r="T9" s="127"/>
+      <c r="U9" s="127"/>
+      <c r="V9" s="127"/>
+      <c r="W9" s="127"/>
     </row>
     <row r="10" spans="1:23" ht="22.8" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="129" t="s">
+      <c r="C10" s="131" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="130"/>
-      <c r="E10" s="130"/>
-      <c r="F10" s="130"/>
-      <c r="G10" s="130" t="s">
+      <c r="D10" s="132"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="132"/>
+      <c r="G10" s="132" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="130"/>
-      <c r="I10" s="130"/>
-      <c r="J10" s="130"/>
-      <c r="K10" s="130" t="s">
+      <c r="H10" s="132"/>
+      <c r="I10" s="132"/>
+      <c r="J10" s="132"/>
+      <c r="K10" s="132" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="130"/>
-      <c r="M10" s="130"/>
-      <c r="N10" s="130"/>
+      <c r="L10" s="132"/>
+      <c r="M10" s="132"/>
+      <c r="N10" s="132"/>
       <c r="O10" s="24"/>
       <c r="P10" s="24"/>
       <c r="Q10" s="24"/>
       <c r="R10" s="25"/>
-      <c r="S10" s="126" t="s">
+      <c r="S10" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="T10" s="126"/>
-      <c r="U10" s="126"/>
-      <c r="V10" s="126"/>
-      <c r="W10" s="126"/>
+      <c r="T10" s="128"/>
+      <c r="U10" s="128"/>
+      <c r="V10" s="128"/>
+      <c r="W10" s="128"/>
     </row>
     <row r="11" spans="1:23" ht="22.8" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="132" t="s">
+      <c r="C11" s="134" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="133"/>
-      <c r="E11" s="133"/>
-      <c r="F11" s="133"/>
-      <c r="G11" s="133" t="s">
+      <c r="D11" s="135"/>
+      <c r="E11" s="135"/>
+      <c r="F11" s="135"/>
+      <c r="G11" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="133"/>
-      <c r="I11" s="133"/>
-      <c r="J11" s="133"/>
+      <c r="H11" s="135"/>
+      <c r="I11" s="135"/>
+      <c r="J11" s="135"/>
       <c r="K11" s="44"/>
       <c r="L11" s="44"/>
       <c r="M11" s="44"/>
@@ -6305,13 +6318,13 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="21"/>
       <c r="R13" s="34"/>
-      <c r="S13" s="126" t="s">
+      <c r="S13" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="T13" s="127"/>
-      <c r="U13" s="127"/>
-      <c r="V13" s="127"/>
-      <c r="W13" s="127"/>
+      <c r="T13" s="129"/>
+      <c r="U13" s="129"/>
+      <c r="V13" s="129"/>
+      <c r="W13" s="129"/>
     </row>
     <row r="14" spans="1:23" ht="15.6">
       <c r="A14" s="1"/>
@@ -6372,12 +6385,12 @@
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="122" t="s">
+      <c r="C16" s="140" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="123"/>
-      <c r="E16" s="123"/>
-      <c r="F16" s="123"/>
+      <c r="D16" s="141"/>
+      <c r="E16" s="141"/>
+      <c r="F16" s="141"/>
       <c r="G16" s="47" t="s">
         <v>56</v>
       </c>
@@ -6490,30 +6503,30 @@
       <c r="B20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="140" t="s">
+      <c r="C20" s="144" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="141"/>
-      <c r="E20" s="141"/>
-      <c r="F20" s="141"/>
-      <c r="G20" s="141" t="s">
+      <c r="D20" s="145"/>
+      <c r="E20" s="145"/>
+      <c r="F20" s="145"/>
+      <c r="G20" s="145" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="141"/>
-      <c r="I20" s="141"/>
-      <c r="J20" s="141"/>
-      <c r="K20" s="141" t="s">
+      <c r="H20" s="145"/>
+      <c r="I20" s="145"/>
+      <c r="J20" s="145"/>
+      <c r="K20" s="145" t="s">
         <v>61</v>
       </c>
-      <c r="L20" s="141"/>
-      <c r="M20" s="141"/>
-      <c r="N20" s="141"/>
-      <c r="O20" s="123" t="s">
+      <c r="L20" s="145"/>
+      <c r="M20" s="145"/>
+      <c r="N20" s="145"/>
+      <c r="O20" s="141" t="s">
         <v>62</v>
       </c>
-      <c r="P20" s="123"/>
-      <c r="Q20" s="123"/>
-      <c r="R20" s="142"/>
+      <c r="P20" s="141"/>
+      <c r="Q20" s="141"/>
+      <c r="R20" s="146"/>
       <c r="S20" s="5"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
@@ -6603,18 +6616,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="S13:W13"/>
-    <mergeCell ref="S10:W10"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:N10"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="S8:W9"/>
@@ -6623,6 +6624,18 @@
     <mergeCell ref="K9:N9"/>
     <mergeCell ref="K8:N8"/>
     <mergeCell ref="O8:R8"/>
+    <mergeCell ref="S13:W13"/>
+    <mergeCell ref="S10:W10"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6703,96 +6716,96 @@
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="136" t="s">
+      <c r="C8" s="138" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="137"/>
-      <c r="E8" s="137"/>
-      <c r="F8" s="137"/>
-      <c r="G8" s="137"/>
-      <c r="H8" s="137"/>
-      <c r="I8" s="137"/>
-      <c r="J8" s="137"/>
-      <c r="K8" s="137" t="s">
+      <c r="D8" s="139"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="139"/>
+      <c r="J8" s="139"/>
+      <c r="K8" s="139" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="137"/>
-      <c r="M8" s="137"/>
-      <c r="N8" s="137"/>
-      <c r="O8" s="137"/>
-      <c r="P8" s="137"/>
-      <c r="Q8" s="137"/>
-      <c r="R8" s="145"/>
-      <c r="S8" s="124" t="s">
+      <c r="L8" s="139"/>
+      <c r="M8" s="139"/>
+      <c r="N8" s="139"/>
+      <c r="O8" s="139"/>
+      <c r="P8" s="139"/>
+      <c r="Q8" s="139"/>
+      <c r="R8" s="149"/>
+      <c r="S8" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="T8" s="125"/>
-      <c r="U8" s="125"/>
-      <c r="V8" s="125"/>
-      <c r="W8" s="125"/>
+      <c r="T8" s="127"/>
+      <c r="U8" s="127"/>
+      <c r="V8" s="127"/>
+      <c r="W8" s="127"/>
     </row>
     <row r="9" spans="1:23" ht="26.4" customHeight="1">
       <c r="B9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="129" t="s">
+      <c r="C9" s="131" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="130"/>
-      <c r="E9" s="130"/>
-      <c r="F9" s="130"/>
-      <c r="G9" s="130"/>
-      <c r="H9" s="130"/>
-      <c r="I9" s="130"/>
-      <c r="J9" s="130"/>
-      <c r="K9" s="128" t="s">
+      <c r="D9" s="132"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="132"/>
+      <c r="H9" s="132"/>
+      <c r="I9" s="132"/>
+      <c r="J9" s="132"/>
+      <c r="K9" s="130" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="128"/>
-      <c r="M9" s="128"/>
-      <c r="N9" s="128"/>
-      <c r="O9" s="128"/>
-      <c r="P9" s="128"/>
-      <c r="Q9" s="128"/>
-      <c r="R9" s="146"/>
-      <c r="S9" s="124"/>
-      <c r="T9" s="125"/>
-      <c r="U9" s="125"/>
-      <c r="V9" s="125"/>
-      <c r="W9" s="125"/>
+      <c r="L9" s="130"/>
+      <c r="M9" s="130"/>
+      <c r="N9" s="130"/>
+      <c r="O9" s="130"/>
+      <c r="P9" s="130"/>
+      <c r="Q9" s="130"/>
+      <c r="R9" s="150"/>
+      <c r="S9" s="126"/>
+      <c r="T9" s="127"/>
+      <c r="U9" s="127"/>
+      <c r="V9" s="127"/>
+      <c r="W9" s="127"/>
     </row>
     <row r="10" spans="1:23" ht="22.8" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="129" t="s">
+      <c r="C10" s="131" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="130"/>
-      <c r="E10" s="130"/>
-      <c r="F10" s="130"/>
-      <c r="G10" s="130"/>
-      <c r="H10" s="130"/>
-      <c r="I10" s="130"/>
-      <c r="J10" s="130"/>
-      <c r="K10" s="130" t="s">
+      <c r="D10" s="132"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="132"/>
+      <c r="G10" s="132"/>
+      <c r="H10" s="132"/>
+      <c r="I10" s="132"/>
+      <c r="J10" s="132"/>
+      <c r="K10" s="132" t="s">
         <v>39</v>
       </c>
-      <c r="L10" s="130"/>
-      <c r="M10" s="130"/>
-      <c r="N10" s="130"/>
-      <c r="O10" s="130"/>
-      <c r="P10" s="130"/>
-      <c r="Q10" s="130"/>
-      <c r="R10" s="131"/>
-      <c r="S10" s="126" t="s">
+      <c r="L10" s="132"/>
+      <c r="M10" s="132"/>
+      <c r="N10" s="132"/>
+      <c r="O10" s="132"/>
+      <c r="P10" s="132"/>
+      <c r="Q10" s="132"/>
+      <c r="R10" s="133"/>
+      <c r="S10" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="T10" s="126"/>
-      <c r="U10" s="126"/>
-      <c r="V10" s="126"/>
-      <c r="W10" s="126"/>
+      <c r="T10" s="128"/>
+      <c r="U10" s="128"/>
+      <c r="V10" s="128"/>
+      <c r="W10" s="128"/>
     </row>
     <row r="11" spans="1:23" ht="22.8" customHeight="1">
       <c r="A11" s="4"/>
@@ -6869,13 +6882,13 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="21"/>
       <c r="R13" s="34"/>
-      <c r="S13" s="126" t="s">
+      <c r="S13" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="T13" s="127"/>
-      <c r="U13" s="127"/>
-      <c r="V13" s="127"/>
-      <c r="W13" s="127"/>
+      <c r="T13" s="129"/>
+      <c r="U13" s="129"/>
+      <c r="V13" s="129"/>
+      <c r="W13" s="129"/>
     </row>
     <row r="14" spans="1:23" ht="15.6">
       <c r="A14" s="1"/>

</xml_diff>